<commit_message>
Updated Interview Question with Named Ranges
</commit_message>
<xml_diff>
--- a/assets/AzureADAssessment-Interview.xlsx
+++ b/assets/AzureADAssessment-Interview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10707"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/meferna_microsoft_com/Documents/AzureAD Assessment/ExcelReader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1BA432-7A21-5744-ABD0-2799773343CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="13_ncr:1_{4D1BA432-7A21-5744-ABD0-2799773343CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61DDCB2F-C334-0640-B355-A70B5A9BF65B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15780" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
   </bookViews>
@@ -18,9 +18,90 @@
     <sheet name="Lookups" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="EM_App_OutboundProvisioning">'Interview Questions'!$E$36</definedName>
-    <definedName name="IM_AADC_SyncSameForestUsersLogIntoWindows">'Interview Questions'!$E$25</definedName>
-    <definedName name="IM_KP_OwnersOfKeyTasksIdentified">'Interview Questions'!$E$9</definedName>
+    <definedName name="AccMgmt_Are_all_your_office_clients_in_versions_that_support_modern_authentication">'Interview Questions'!$E$184</definedName>
+    <definedName name="AccMgmt_Are_strong_credentials_used_for_SSPR">'Interview Questions'!$E$92</definedName>
+    <definedName name="AccMgmt_Are_strong_credentials_used_in_conditional_access_policies">'Interview Questions'!$E$90</definedName>
+    <definedName name="AccMgmt_Are_there_applications_that_can_be_candidates_to_use_attribute_based_access_control">'Interview Questions'!$E$160</definedName>
+    <definedName name="AccMgmt_Are_you_Archiving_AD_FS_audits">'Interview Questions'!$E$228</definedName>
+    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_security_incident_response">'Interview Questions'!$E$236</definedName>
+    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_support_and_troubleshooting_access_issues">'Interview Questions'!$E$238</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$220</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$224</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Sign_in_Activity_Logs">'Interview Questions'!$E$216</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Office_365_activity_logs">'Interview Questions'!$E$232</definedName>
+    <definedName name="AccMgmt_Do_you_enable_SSO_for_capable_apps_or_are_the_apps_that_use_local_accounts">'Interview Questions'!$E$142</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_self_service_password_reset_solution">'Interview Questions'!$E$63</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_SIEM_system">'Interview Questions'!$E$212</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today">'Interview Questions'!$E$156</definedName>
+    <definedName name="AccMgmt_Do_you_have_applications_that_support_SAML_OpenID_connect_or_OAuth">'Interview Questions'!$E$138</definedName>
+    <definedName name="AccMgmt_Do_you_have_desktop_management_policies">'Interview Questions'!$E$122</definedName>
+    <definedName name="AccMgmt_Do_you_have_initiative_to_migrate_SSO_configuration_from_AD_FS_to_Azure_AD">'Interview Questions'!$E$150</definedName>
+    <definedName name="AccMgmt_Do_you_have_Intune_Application_Management_MAM_policies_defined">'Interview Questions'!$E$166</definedName>
+    <definedName name="AccMgmt_Do_you_have_mobile_management_policies_defined">'Interview Questions'!$E$120</definedName>
+    <definedName name="AccMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$44</definedName>
+    <definedName name="AccMgmt_Do_you_have_scripts_that_run_on_a_regular_basis">'Interview Questions'!$E$104</definedName>
+    <definedName name="AccMgmt_Do_you_have_service_accounts_or_applications_that_rely_on_legacy_authentication">'Interview Questions'!$E$190</definedName>
+    <definedName name="AccMgmt_Do_you_provision_strong_credentials_alongside_identity_provisioning_or_device_provisioning">'Interview Questions'!$E$88</definedName>
+    <definedName name="AccMgmt_Do_you_provision_strong_credentials_to_all_users_with_privileged_roles">'Interview Questions'!$E$86</definedName>
+    <definedName name="AccMgmt_Do_you_use_device_compliance_as_a_control_in_Conditional_Access">'Interview Questions'!$E$126</definedName>
+    <definedName name="AccMgmt_Do_you_use_them_in_CA_policies">'Interview Questions'!$E$168</definedName>
+    <definedName name="AccMgmt_Do_your_users_use_Windows_Hello_in_their_Windows_10_Desktops">'Interview Questions'!$E$130</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Azure_Log_Analytics">'Interview Questions'!$E$204</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Hybrid_Azure_AD_joined_in_your_environment">'Interview Questions'!$E$124</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Windows_Hello_as_an_enterprise_wide_policy">'Interview Questions'!$E$132</definedName>
+    <definedName name="AccMgmt_Have_you_enabled_All_Office_365_Auditing">'Interview Questions'!$E$230</definedName>
+    <definedName name="AccMgmt_Have_you_enabled_Password_Hash_Sync">'Interview Questions'!$E$96</definedName>
+    <definedName name="AccMgmt_Have_you_explicitly_identified_regions_where_authentication_should_NOT_be_coming_from">'Interview Questions'!$E$196</definedName>
+    <definedName name="AccMgmt_Have_you_identified_the_regions_of_the_world_where_authentication_traffic_should_be_coming_from">'Interview Questions'!$E$194</definedName>
+    <definedName name="AccMgmt_If_so_do_you_have_a_dedicated_service_principal_to_run_it_against">'Interview Questions'!$E$106</definedName>
+    <definedName name="AccMgmt_If_so_do_you_have_configured_the_applications_to_support_SSO_using_those_protocols">'Interview Questions'!$E$140</definedName>
+    <definedName name="AccMgmt_If_so_does_your_operations_team_use_it_regularly_to_understand_Azure_AD_usage">'Interview Questions'!$E$206</definedName>
+    <definedName name="AccMgmt_If_you_are_using_passwords_how_do_you_manage_the_them">'Interview Questions'!$E$108</definedName>
+    <definedName name="AccMgmt_If_you_use_cloud_authentication_PHS_or_PTA_do_you_have_Seamless_SSO_enabled">'Interview Questions'!$E$114</definedName>
+    <definedName name="AccMgmt_If_you_use_federated_authentication_do_you_use_windows_integrated_authentication_WIA_when_inside_the_corporate_network">'Interview Questions'!$E$116</definedName>
+    <definedName name="AccMgmt_Is_legacy_authentication_blocked_by_conditional_access">'Interview Questions'!$E$188</definedName>
+    <definedName name="AccMgmt_Is_legacy_authentication_disabled_at_the_mailbox_level">'Interview Questions'!$E$186</definedName>
+    <definedName name="AccMgmt_Is_the_password_reset_part_of_the_operational_procedures_to_remediate_a_user_incident">'Interview Questions'!$E$65</definedName>
+    <definedName name="AccMgmt_Is_the_procedure_to_switch_to_PHS_practiced_enabled_to_the_IAM_Ops_team">'Interview Questions'!$E$98</definedName>
+    <definedName name="AccMgmt_What_platforms_do_you_use_to_provide_SSO_to_the_applications">'Interview Questions'!$E$144</definedName>
+    <definedName name="AccMgmt_What_process_do_you_have_to_discover_applications_that_are_not_configured_using_the_SSO_enterprise_solution">'Interview Questions'!$E$146</definedName>
+    <definedName name="EntMgmt_Do_you_use_Azure_AD_Outbound_provisioning_for_applications_in_your_environment_that_supports_Azure_AD_provisioning">'Interview Questions'!$E$36</definedName>
+    <definedName name="EntMgmt_What_is_the_approach_to_provision_to_applications_today">'Interview Questions'!$E$34</definedName>
+    <definedName name="Gov_Access_Review_Guest_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$295</definedName>
+    <definedName name="Gov_Access_Review_Guest_Is_it_automated">'Interview Questions'!$E$283</definedName>
+    <definedName name="Gov_AccessReview_Privileged_If_so_are_they_automated">'Interview Questions'!$E$311</definedName>
+    <definedName name="Gov_All_Users_Is_it_automated">'Interview Questions'!$E$293</definedName>
+    <definedName name="Gov_Are_there_system_accounts_that_are_also_privileged">'Interview Questions'!$E$315</definedName>
+    <definedName name="Gov_Do_administrators_have_dedicated_accounts_used_to_perform_privileged_operations">'Interview Questions'!$E$303</definedName>
+    <definedName name="Gov_Do_administrators_have_standing_access_to_privileges_in_your_environment">'Interview Questions'!$E$301</definedName>
+    <definedName name="Gov_Do_you_assign_users_to_the_All_Users_group">'Interview Questions'!$E$291</definedName>
+    <definedName name="Gov_Do_you_have_a_guest_access_review_strategy_in_place">'Interview Questions'!$E$289</definedName>
+    <definedName name="Gov_Do_you_have_a_privileged_role_strategy_for_Azure_Resources">'Interview Questions'!$E$323</definedName>
+    <definedName name="Gov_Do_you_have_a_process_to_identify_the_least_privileged_role_to_different_users_in_your_organization">'Interview Questions'!$E$307</definedName>
+    <definedName name="Gov_Do_you_have_a_test_environment">'Interview Questions'!$E$258</definedName>
+    <definedName name="Gov_Do_you_have_access_reviews_in_place_for_privileged_accounts">'Interview Questions'!$E$309</definedName>
+    <definedName name="Gov_Do_you_have_an_access_review_strategy_in_place">'Interview Questions'!$E$281</definedName>
+    <definedName name="Gov_Do_you_have_emergency_accounts_also_known_as_break_glass_provisioned_in_your_Azure_AD_tenant">'Interview Questions'!$E$328</definedName>
+    <definedName name="Gov_Do_you_have_owners_in_your_organization_for_all_the_tasks_listed_below">'Interview Questions'!$E$246</definedName>
+    <definedName name="Gov_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$285</definedName>
+    <definedName name="Gov_If_not_what_is_the_strategy_to_clean_up_remove_access">'Interview Questions'!$E$313</definedName>
+    <definedName name="Gov_If_so_how_do_establish_ownership_of_those_accounts">'Interview Questions'!$E$317</definedName>
+    <definedName name="Gov_Is_there_any_global_admin_outside_the_IAM_team">'Interview Questions'!$E$319</definedName>
+    <definedName name="IdMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$9</definedName>
+    <definedName name="IdMgmt_Do_you_synchronize_the_same_forest_where_users_log_in_to_their_Windows_devices">'Interview Questions'!$E$25</definedName>
+    <definedName name="Ops_Are_there_compensating_controls_for_cases_where_the_answer_above_is_No">'Interview Questions'!$E$379</definedName>
+    <definedName name="Ops_Azure_AD_App_Proxy_debug_connector_group_deployed">'Interview Questions'!$F$357</definedName>
+    <definedName name="Ops_Debugging_tools_deployed_in_debug_app_proxy_connector">'Interview Questions'!$F$358</definedName>
+    <definedName name="Ops_Is_any_of_the_servers_above_virtualized_If_so__is_there_proper_isolation_between_VM_Host_administrators_and_the_IAM_team">'Interview Questions'!$E$375</definedName>
+    <definedName name="Ops_Is_there_proper_isolation_between_SQL_Admins_and_the_IAM_team">'Interview Questions'!$E$377</definedName>
+    <definedName name="Ops_Multiple_Azure_AD_Application_Proxy_connectors_per_group_deployed">'Interview Questions'!$F$355</definedName>
+    <definedName name="Ops_Multiple_Azure_AD_Pass_through_authentication_agents_deployed">'Interview Questions'!$F$356</definedName>
+    <definedName name="Ops_Secured_Azure_AD_App_Proxy_Connector">'Interview Questions'!$F$370</definedName>
+    <definedName name="Ops_Secured_Azure_AD_Connect_Servers">'Interview Questions'!$F$366</definedName>
+    <definedName name="Ops_Secured_NPS_Extension">'Interview Questions'!$F$372</definedName>
+    <definedName name="Ops_Secured_Pass_through_Authentication_Agent">'Interview Questions'!$F$371</definedName>
+    <definedName name="Ops_Secured_SQL_Server_for_ADFS">'Interview Questions'!$F$369</definedName>
+    <definedName name="Ops_Secured_SQL_Server_for_Azure_AD_Connect">'Interview Questions'!$F$367</definedName>
     <definedName name="YesNo">Lookups!$B$8:$B$9</definedName>
     <definedName name="YesNoPartial">Lookups!$B$3:$B$5</definedName>
   </definedNames>
@@ -43,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="385">
   <si>
     <t>Identity Management</t>
   </si>
@@ -294,9 +375,6 @@
     <t>Do your users use Windows Hello in their Windows 10 Desktops?</t>
   </si>
   <si>
-    <t>Have you deployed Windows Hello as an enterprise-wide policy, or is this usage is based on end-users initiative?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Application Authentication and Assignment </t>
   </si>
   <si>
@@ -604,12 +682,6 @@
   </si>
   <si>
     <t xml:space="preserve">If not, what is the strategy to clean up / remove access? </t>
-  </si>
-  <si>
-    <t>Are there “system accounts” that are also privileged? If so, how do establish ownership of those accounts?</t>
-  </si>
-  <si>
-    <t>Is there any global admin outside the IAM team? Why?</t>
   </si>
   <si>
     <t>Do you have a privileged role strategy for Azure Resources?</t>
@@ -1217,6 +1289,21 @@
       </rPr>
       <t xml:space="preserve"> tab to answer the remaining questions.</t>
     </r>
+  </si>
+  <si>
+    <t>Have you deployed Windows Hello as an enterprise-wide policy?</t>
+  </si>
+  <si>
+    <t>Are there “system accounts” that are also privileged?</t>
+  </si>
+  <si>
+    <t>If so, how do establish ownership of those accounts?</t>
+  </si>
+  <si>
+    <t>Why?</t>
+  </si>
+  <si>
+    <t>Is there any global admin outside the IAM team?</t>
   </si>
 </sst>
 </file>
@@ -1492,6 +1579,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
@@ -1500,9 +1590,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
@@ -1593,8 +1680,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}" name="Table7" displayName="Table7" ref="E333:F345" totalsRowShown="0">
-  <autoFilter ref="E333:F345" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}" name="Table7" displayName="Table7" ref="E337:F349" totalsRowShown="0">
+  <autoFilter ref="E337:F349" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E9AA62EB-CA64-A84A-90FE-4FB406CFBB9B}" name="Task"/>
     <tableColumn id="2" xr3:uid="{A95B16A3-9350-3B42-AEC0-844DDF1A8645}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1604,8 +1691,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}" name="Table8" displayName="Table8" ref="E350:F354" totalsRowShown="0">
-  <autoFilter ref="E350:F354" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}" name="Table8" displayName="Table8" ref="E354:F358" totalsRowShown="0">
+  <autoFilter ref="E354:F358" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8E26C403-A376-C242-AC8E-6B61F7C1302E}" name="Best Practice"/>
     <tableColumn id="2" xr3:uid="{020742E9-39A6-0A45-9032-2C3C5E3B59B3}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1914,7 +2001,7 @@
   <dimension ref="A2:N297"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1929,7 +2016,7 @@
   <sheetData>
     <row r="2" spans="2:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1946,52 +2033,52 @@
     </row>
     <row r="3" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C4" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="13"/>
+      <c r="C4" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="16"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="8" spans="2:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2008,7 +2095,7 @@
     <row r="9" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -2024,7 +2111,7 @@
     <row r="11" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E12" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -2038,12 +2125,12 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F13" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E15" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -2057,32 +2144,32 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F16" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F19" s="11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F21" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F22" s="11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G24" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.2">
@@ -2090,7 +2177,7 @@
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.2">
@@ -2098,17 +2185,17 @@
     </row>
     <row r="30" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F31" s="11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E33" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -2122,52 +2209,52 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F34" s="11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F38" s="11" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F40" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F41" s="11" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G42" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G43" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G45" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -2175,7 +2262,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -2183,7 +2270,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G51" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -2191,7 +2278,7 @@
     </row>
     <row r="54" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E54" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -2205,32 +2292,32 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E55" s="11" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F58" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F59" s="11" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G61" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -2238,7 +2325,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G64" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -2246,7 +2333,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G67" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -2254,7 +2341,7 @@
     </row>
     <row r="70" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E70" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -2268,15 +2355,15 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E71" s="11" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -2290,87 +2377,87 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E74" s="11" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E75" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F76" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F77" s="11" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F78" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F79" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F80" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F81" s="11" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="83" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F83" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F84" s="11" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="85" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F85" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F86" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F87" s="11" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="88" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F88" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F89" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F90" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="92" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E92" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -2384,17 +2471,17 @@
     </row>
     <row r="93" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E93" s="11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="94" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E94" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E95" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -2408,23 +2495,23 @@
     </row>
     <row r="96" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F96" s="11" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="97" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E97" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F97" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="99" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G99" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="100" spans="5:7" x14ac:dyDescent="0.2">
@@ -2432,7 +2519,7 @@
     </row>
     <row r="102" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G102" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="5:7" x14ac:dyDescent="0.2">
@@ -2440,7 +2527,7 @@
     </row>
     <row r="105" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G105" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="5:7" x14ac:dyDescent="0.2">
@@ -2448,7 +2535,7 @@
     </row>
     <row r="108" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G108" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="109" spans="5:7" x14ac:dyDescent="0.2">
@@ -2456,7 +2543,7 @@
     </row>
     <row r="111" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G111" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="112" spans="5:7" x14ac:dyDescent="0.2">
@@ -2464,7 +2551,7 @@
     </row>
     <row r="114" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G114" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="115" spans="5:14" x14ac:dyDescent="0.2">
@@ -2472,7 +2559,7 @@
     </row>
     <row r="117" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G117" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="118" spans="5:14" x14ac:dyDescent="0.2">
@@ -2480,7 +2567,7 @@
     </row>
     <row r="120" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E120" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
@@ -2494,17 +2581,17 @@
     </row>
     <row r="121" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E121" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="122" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E122" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E123" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
@@ -2518,17 +2605,17 @@
     </row>
     <row r="124" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E124" s="11" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="125" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E125" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="126" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E126" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
@@ -2542,77 +2629,77 @@
     </row>
     <row r="127" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E127" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="128" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="129" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F129" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="130" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F130" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="131" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F131" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="132" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F132" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="133" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F133" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="134" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F134" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="135" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F135" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="136" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F136" s="11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="138" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F138" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="139" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F139" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="141" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F141" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="142" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F142" s="11" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="145" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D145" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
@@ -2628,7 +2715,7 @@
     <row r="146" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="147" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E147" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F147" s="3"/>
       <c r="G147" s="3"/>
@@ -2642,23 +2729,23 @@
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E148" s="11" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G150" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G151" s="7"/>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G153" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
@@ -2666,7 +2753,7 @@
     </row>
     <row r="156" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E156" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F156" s="3"/>
       <c r="G156" s="3"/>
@@ -2680,17 +2767,17 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E157" s="11" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E158" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G159" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
@@ -2698,7 +2785,7 @@
     </row>
     <row r="162" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G162" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="163" spans="5:14" x14ac:dyDescent="0.2">
@@ -2706,7 +2793,7 @@
     </row>
     <row r="165" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E165" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F165" s="3"/>
       <c r="G165" s="3"/>
@@ -2720,102 +2807,102 @@
     </row>
     <row r="166" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E166" s="11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="167" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E167" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="168" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F168" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="169" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F169" s="11" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="170" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F170" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="171" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F171" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="172" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F172" s="11" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="173" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G173" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="174" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G174" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="175" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F175" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="176" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F176" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="177" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F177" s="11" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="178" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F178" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="179" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F179" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="180" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F180" s="11" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="181" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F181" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="182" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F182" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="183" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F183" s="11" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="184" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E184" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="186" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E186" s="3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
@@ -2829,17 +2916,17 @@
     </row>
     <row r="187" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E187" s="11" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="188" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E188" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="189" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E189" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F189" s="3"/>
       <c r="G189" s="3"/>
@@ -2853,12 +2940,12 @@
     </row>
     <row r="190" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E190" s="11" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="192" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G192" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="193" spans="5:14" x14ac:dyDescent="0.2">
@@ -2866,7 +2953,7 @@
     </row>
     <row r="195" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G195" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="196" spans="5:14" x14ac:dyDescent="0.2">
@@ -2874,7 +2961,7 @@
     </row>
     <row r="198" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G198" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="199" spans="5:14" x14ac:dyDescent="0.2">
@@ -2882,7 +2969,7 @@
     </row>
     <row r="201" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E201" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F201" s="3"/>
       <c r="G201" s="3"/>
@@ -2896,42 +2983,42 @@
     </row>
     <row r="202" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E202" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="204" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E204" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="205" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E205" s="11" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="206" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E206" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="207" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E207" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="208" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E208" s="11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="209" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E209" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="210" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E210" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F210" s="3"/>
       <c r="G210" s="3"/>
@@ -2945,82 +3032,82 @@
     </row>
     <row r="211" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F211" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="212" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F212" s="11" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="214" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F214" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="215" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F215" s="11" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="216" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F216" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="217" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F217" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="218" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F218" s="11" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="220" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F220" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="221" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F221" s="11" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="223" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F223" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="224" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F224" s="11" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="225" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E225" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="226" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F226" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="227" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F227" s="11" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="228" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E228" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="229" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E229" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F229" s="3"/>
       <c r="G229" s="3"/>
@@ -3034,165 +3121,165 @@
     </row>
     <row r="230" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F230" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="231" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F231" s="11" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="232" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F232" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="233" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F233" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="234" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F234" s="11" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="235" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F235" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="236" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F236" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="237" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F237" s="11" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="238" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F238" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="239" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F239" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="240" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F240" s="11" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="241" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F241" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="242" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F242" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="243" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F243" s="11" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="244" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F244" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="245" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F245" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="246" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F246" s="11" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="247" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F247" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="248" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F248" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="249" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F249" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="250" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F250" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="251" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F251" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="252" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F252" s="11" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="253" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F253" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="255" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F255" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="256" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F256" s="11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="258" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F258" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="259" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F259" s="11" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="261" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F261" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="262" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E262" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F262" s="11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="264" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E264" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="265" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E265" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F265" s="3"/>
       <c r="G265" s="3"/>
@@ -3206,82 +3293,82 @@
     </row>
     <row r="267" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F267" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="268" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F268" s="11" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="269" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F269" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="270" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F270" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="271" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F271" s="11" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="272" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F272" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="273" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F273" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="274" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F274" s="11" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="275" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F275" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="276" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F276" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="277" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F277" s="11" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="278" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F278" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="279" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F279" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="280" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F280" s="11" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="281" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E281" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="282" spans="3:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C282" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D282" s="1"/>
       <c r="E282" s="1"/>
@@ -3298,7 +3385,7 @@
     <row r="283" spans="3:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="284" spans="3:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D284" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E284" s="2"/>
       <c r="F284" s="2"/>
@@ -3313,27 +3400,27 @@
     </row>
     <row r="285" spans="3:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="E285" s="11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="286" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E286" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="287" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E287" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="289" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E289" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="290" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C290" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D290" s="1"/>
       <c r="E290" s="1"/>
@@ -3349,17 +3436,17 @@
     </row>
     <row r="291" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D291" s="11" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="293" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E293" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="297" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3439,7 +3526,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8F88F7-5CA7-5843-BD88-A88F2BE33EC7}">
-  <dimension ref="B2:G375"/>
+  <dimension ref="B2:G379"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -3562,7 +3649,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -3605,7 +3692,7 @@
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3867,9 +3954,7 @@
       </c>
     </row>
     <row r="86" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E86" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="E86" s="7"/>
     </row>
     <row r="87" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E87" t="s">
@@ -4051,7 +4136,7 @@
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E131" t="s">
-        <v>83</v>
+        <v>380</v>
       </c>
     </row>
     <row r="132" spans="3:7" x14ac:dyDescent="0.2">
@@ -4059,7 +4144,7 @@
     </row>
     <row r="134" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C134" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
@@ -4069,7 +4154,7 @@
     <row r="135" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="136" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D136" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E136" s="3"/>
       <c r="F136" s="3"/>
@@ -4077,7 +4162,7 @@
     </row>
     <row r="137" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E137" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="138" spans="3:7" x14ac:dyDescent="0.2">
@@ -4085,7 +4170,7 @@
     </row>
     <row r="139" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E139" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="140" spans="3:7" x14ac:dyDescent="0.2">
@@ -4093,7 +4178,7 @@
     </row>
     <row r="141" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E141" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="142" spans="3:7" x14ac:dyDescent="0.2">
@@ -4101,7 +4186,7 @@
     </row>
     <row r="143" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E143" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="144" spans="3:7" x14ac:dyDescent="0.2">
@@ -4109,7 +4194,7 @@
     </row>
     <row r="145" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E145" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="146" spans="4:7" x14ac:dyDescent="0.2">
@@ -4117,7 +4202,7 @@
     </row>
     <row r="148" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D148" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E148" s="3"/>
       <c r="F148" s="3"/>
@@ -4125,7 +4210,7 @@
     </row>
     <row r="149" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E149" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="150" spans="4:7" x14ac:dyDescent="0.2">
@@ -4133,7 +4218,7 @@
     </row>
     <row r="151" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E151" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="152" spans="4:7" x14ac:dyDescent="0.2">
@@ -4141,7 +4226,7 @@
     </row>
     <row r="154" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D154" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E154" s="3"/>
       <c r="F154" s="3"/>
@@ -4149,7 +4234,7 @@
     </row>
     <row r="155" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E155" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="156" spans="4:7" x14ac:dyDescent="0.2">
@@ -4157,7 +4242,7 @@
     </row>
     <row r="157" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E157" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="158" spans="4:7" x14ac:dyDescent="0.2">
@@ -4165,7 +4250,7 @@
     </row>
     <row r="159" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E159" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="160" spans="4:7" x14ac:dyDescent="0.2">
@@ -4173,7 +4258,7 @@
     </row>
     <row r="162" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C162" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
@@ -4183,7 +4268,7 @@
     <row r="163" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="164" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D164" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
@@ -4191,7 +4276,7 @@
     </row>
     <row r="165" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E165" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="166" spans="3:7" x14ac:dyDescent="0.2">
@@ -4199,7 +4284,7 @@
     </row>
     <row r="167" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E167" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="168" spans="3:7" x14ac:dyDescent="0.2">
@@ -4207,7 +4292,7 @@
     </row>
     <row r="170" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D170" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E170" s="3"/>
       <c r="F170" s="3"/>
@@ -4215,51 +4300,51 @@
     </row>
     <row r="172" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E172" t="s">
+        <v>100</v>
+      </c>
+      <c r="F172" t="s">
         <v>101</v>
-      </c>
-      <c r="F172" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="173" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E173" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F173" s="7"/>
     </row>
     <row r="174" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E174" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F174" s="7"/>
     </row>
     <row r="175" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E175" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F175" s="7"/>
     </row>
     <row r="176" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E176" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F176" s="7"/>
     </row>
     <row r="177" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E177" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F177" s="7"/>
     </row>
     <row r="178" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E178" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F178" s="7"/>
     </row>
     <row r="180" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C180" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
@@ -4269,7 +4354,7 @@
     <row r="181" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="182" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D182" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E182" s="3"/>
       <c r="F182" s="3"/>
@@ -4277,7 +4362,7 @@
     </row>
     <row r="183" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E183" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="184" spans="3:7" x14ac:dyDescent="0.2">
@@ -4285,7 +4370,7 @@
     </row>
     <row r="185" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E185" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="186" spans="3:7" x14ac:dyDescent="0.2">
@@ -4293,7 +4378,7 @@
     </row>
     <row r="187" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E187" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="188" spans="3:7" x14ac:dyDescent="0.2">
@@ -4301,7 +4386,7 @@
     </row>
     <row r="189" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E189" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="190" spans="3:7" x14ac:dyDescent="0.2">
@@ -4309,7 +4394,7 @@
     </row>
     <row r="192" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D192" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E192" s="3"/>
       <c r="F192" s="3"/>
@@ -4317,7 +4402,7 @@
     </row>
     <row r="193" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E193" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="194" spans="3:7" x14ac:dyDescent="0.2">
@@ -4325,7 +4410,7 @@
     </row>
     <row r="195" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E195" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="196" spans="3:7" x14ac:dyDescent="0.2">
@@ -4333,7 +4418,7 @@
     </row>
     <row r="197" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E197" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="198" spans="3:7" x14ac:dyDescent="0.2">
@@ -4341,7 +4426,7 @@
     </row>
     <row r="200" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C200" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -4351,7 +4436,7 @@
     <row r="201" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="202" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D202" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E202" s="3"/>
       <c r="F202" s="3"/>
@@ -4359,7 +4444,7 @@
     </row>
     <row r="203" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E203" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="204" spans="3:7" x14ac:dyDescent="0.2">
@@ -4367,7 +4452,7 @@
     </row>
     <row r="205" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E205" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="206" spans="3:7" x14ac:dyDescent="0.2">
@@ -4375,7 +4460,7 @@
     </row>
     <row r="207" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E207" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="208" spans="3:7" x14ac:dyDescent="0.2">
@@ -4383,7 +4468,7 @@
     </row>
     <row r="210" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D210" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E210" s="3"/>
       <c r="F210" s="3"/>
@@ -4391,7 +4476,7 @@
     </row>
     <row r="211" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E211" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="212" spans="4:7" x14ac:dyDescent="0.2">
@@ -4399,7 +4484,7 @@
     </row>
     <row r="213" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E213" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="214" spans="4:7" x14ac:dyDescent="0.2">
@@ -4407,7 +4492,7 @@
     </row>
     <row r="215" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E215" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="216" spans="4:7" x14ac:dyDescent="0.2">
@@ -4415,7 +4500,7 @@
     </row>
     <row r="217" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E217" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="218" spans="4:7" x14ac:dyDescent="0.2">
@@ -4423,7 +4508,7 @@
     </row>
     <row r="219" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E219" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="220" spans="4:7" x14ac:dyDescent="0.2">
@@ -4431,7 +4516,7 @@
     </row>
     <row r="221" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E221" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="222" spans="4:7" x14ac:dyDescent="0.2">
@@ -4439,7 +4524,7 @@
     </row>
     <row r="223" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E223" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="224" spans="4:7" x14ac:dyDescent="0.2">
@@ -4447,7 +4532,7 @@
     </row>
     <row r="225" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E225" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="226" spans="2:7" x14ac:dyDescent="0.2">
@@ -4455,7 +4540,7 @@
     </row>
     <row r="227" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E227" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="228" spans="2:7" x14ac:dyDescent="0.2">
@@ -4463,7 +4548,7 @@
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E229" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="230" spans="2:7" x14ac:dyDescent="0.2">
@@ -4471,7 +4556,7 @@
     </row>
     <row r="231" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E231" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="232" spans="2:7" x14ac:dyDescent="0.2">
@@ -4479,7 +4564,7 @@
     </row>
     <row r="233" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E233" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="234" spans="2:7" x14ac:dyDescent="0.2">
@@ -4487,7 +4572,7 @@
     </row>
     <row r="235" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E235" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="236" spans="2:7" x14ac:dyDescent="0.2">
@@ -4495,7 +4580,7 @@
     </row>
     <row r="237" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E237" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="238" spans="2:7" x14ac:dyDescent="0.2">
@@ -4503,7 +4588,7 @@
     </row>
     <row r="240" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B240" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
@@ -4540,7 +4625,7 @@
     <row r="245" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D245" s="10"/>
       <c r="E245" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F245" s="10"/>
       <c r="G245" s="10"/>
@@ -4553,48 +4638,48 @@
         <v>8</v>
       </c>
       <c r="F247" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="248" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E248" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F248" s="7"/>
     </row>
     <row r="249" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E249" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F249" s="7"/>
     </row>
     <row r="250" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E250" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F250" s="7"/>
     </row>
     <row r="251" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E251" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F251" s="7"/>
     </row>
     <row r="252" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E252" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F252" s="7"/>
     </row>
     <row r="253" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E253" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F253" s="7"/>
     </row>
     <row r="256" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D256" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E256" s="3"/>
       <c r="F256" s="3"/>
@@ -4602,7 +4687,7 @@
     </row>
     <row r="257" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E257" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="258" spans="5:6" x14ac:dyDescent="0.2">
@@ -4610,7 +4695,7 @@
     </row>
     <row r="259" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E259" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="260" spans="5:6" x14ac:dyDescent="0.2">
@@ -4618,12 +4703,12 @@
     </row>
     <row r="261" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E261" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="263" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E263" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F263" t="s">
         <v>9</v>
@@ -4631,73 +4716,73 @@
     </row>
     <row r="264" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E264" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F264" s="7"/>
     </row>
     <row r="265" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E265" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F265" s="7"/>
     </row>
     <row r="266" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E266" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F266" s="7"/>
     </row>
     <row r="267" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E267" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F267" s="7"/>
     </row>
     <row r="268" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E268" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F268" s="7"/>
     </row>
     <row r="269" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E269" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F269" s="7"/>
     </row>
     <row r="270" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E270" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F270" s="7"/>
     </row>
     <row r="271" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E271" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F271" s="7"/>
     </row>
     <row r="272" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E272" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F272" s="7"/>
     </row>
     <row r="273" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E273" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F273" s="7"/>
     </row>
     <row r="274" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E274" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F274" s="7"/>
     </row>
     <row r="277" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C277" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D277" s="2"/>
       <c r="E277" s="2"/>
@@ -4707,7 +4792,7 @@
     <row r="278" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="279" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D279" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E279" s="3"/>
       <c r="F279" s="3"/>
@@ -4715,7 +4800,7 @@
     </row>
     <row r="280" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E280" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="281" spans="3:7" x14ac:dyDescent="0.2">
@@ -4723,7 +4808,7 @@
     </row>
     <row r="282" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E282" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="283" spans="3:7" x14ac:dyDescent="0.2">
@@ -4731,7 +4816,7 @@
     </row>
     <row r="284" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E284" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="285" spans="3:7" x14ac:dyDescent="0.2">
@@ -4739,7 +4824,7 @@
     </row>
     <row r="287" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D287" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E287" s="3"/>
       <c r="F287" s="3"/>
@@ -4747,7 +4832,7 @@
     </row>
     <row r="288" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E288" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="289" spans="3:7" x14ac:dyDescent="0.2">
@@ -4755,7 +4840,7 @@
     </row>
     <row r="290" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E290" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="291" spans="3:7" x14ac:dyDescent="0.2">
@@ -4763,7 +4848,7 @@
     </row>
     <row r="292" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E292" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="293" spans="3:7" x14ac:dyDescent="0.2">
@@ -4771,7 +4856,7 @@
     </row>
     <row r="294" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E294" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="295" spans="3:7" x14ac:dyDescent="0.2">
@@ -4779,7 +4864,7 @@
     </row>
     <row r="297" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C297" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D297" s="2"/>
       <c r="E297" s="2"/>
@@ -4789,7 +4874,7 @@
     <row r="298" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="299" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D299" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E299" s="3"/>
       <c r="F299" s="3"/>
@@ -4797,7 +4882,7 @@
     </row>
     <row r="300" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E300" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="301" spans="3:7" x14ac:dyDescent="0.2">
@@ -4805,7 +4890,7 @@
     </row>
     <row r="302" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E302" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="303" spans="3:7" x14ac:dyDescent="0.2">
@@ -4813,12 +4898,15 @@
     </row>
     <row r="304" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E304" t="s">
-        <v>182</v>
-      </c>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="305" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E305" s="7"/>
     </row>
     <row r="306" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E306" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="307" spans="5:5" x14ac:dyDescent="0.2">
@@ -4826,7 +4914,7 @@
     </row>
     <row r="308" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E308" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="309" spans="5:5" x14ac:dyDescent="0.2">
@@ -4834,7 +4922,7 @@
     </row>
     <row r="310" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E310" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="311" spans="5:5" x14ac:dyDescent="0.2">
@@ -4842,12 +4930,15 @@
     </row>
     <row r="312" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E312" t="s">
-        <v>186</v>
-      </c>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="313" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E313" s="7"/>
     </row>
     <row r="314" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E314" t="s">
-        <v>187</v>
+        <v>381</v>
       </c>
     </row>
     <row r="315" spans="5:5" x14ac:dyDescent="0.2">
@@ -4855,7 +4946,7 @@
     </row>
     <row r="316" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E316" t="s">
-        <v>188</v>
+        <v>382</v>
       </c>
     </row>
     <row r="317" spans="5:5" x14ac:dyDescent="0.2">
@@ -4863,303 +4954,322 @@
     </row>
     <row r="318" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E318" t="s">
-        <v>189</v>
+        <v>384</v>
       </c>
     </row>
     <row r="319" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E319" s="7"/>
     </row>
-    <row r="321" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D321" s="3" t="s">
+    <row r="320" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E320" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="321" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E321" s="7"/>
+    </row>
+    <row r="322" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E322" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E323" s="7"/>
+    </row>
+    <row r="325" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D325" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E325" s="3"/>
+      <c r="F325" s="3"/>
+      <c r="G325" s="3"/>
+    </row>
+    <row r="327" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E327" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="328" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E328" s="7"/>
+    </row>
+    <row r="329" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E329" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="330" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E330" s="7"/>
+    </row>
+    <row r="331" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B331" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E321" s="3"/>
-      <c r="F321" s="3"/>
-      <c r="G321" s="3"/>
-    </row>
-    <row r="323" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E323" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="324" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E324" s="7"/>
-    </row>
-    <row r="325" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E325" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="327" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B327" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C327" s="1"/>
-      <c r="D327" s="1"/>
-      <c r="E327" s="1"/>
-      <c r="F327" s="1"/>
-      <c r="G327" s="1"/>
-    </row>
-    <row r="328" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B328" s="9"/>
-      <c r="C328" s="9"/>
-      <c r="D328" s="9"/>
-      <c r="E328" s="9"/>
-      <c r="F328" s="9"/>
-      <c r="G328" s="9"/>
-    </row>
-    <row r="329" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C329" s="2" t="s">
+      <c r="C331" s="1"/>
+      <c r="D331" s="1"/>
+      <c r="E331" s="1"/>
+      <c r="F331" s="1"/>
+      <c r="G331" s="1"/>
+    </row>
+    <row r="332" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B332" s="9"/>
+      <c r="C332" s="9"/>
+      <c r="D332" s="9"/>
+      <c r="E332" s="9"/>
+      <c r="F332" s="9"/>
+      <c r="G332" s="9"/>
+    </row>
+    <row r="333" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C333" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D329" s="2"/>
-      <c r="E329" s="2"/>
-      <c r="F329" s="2"/>
-      <c r="G329" s="2"/>
-    </row>
-    <row r="330" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="331" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D331" s="3" t="s">
+      <c r="D333" s="2"/>
+      <c r="E333" s="2"/>
+      <c r="F333" s="2"/>
+      <c r="G333" s="2"/>
+    </row>
+    <row r="334" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="335" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D335" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E331" s="3"/>
-      <c r="F331" s="3"/>
-      <c r="G331" s="3"/>
-    </row>
-    <row r="332" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E332" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="333" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E333" t="s">
-        <v>8</v>
-      </c>
-      <c r="F333" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="334" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E334" t="s">
-        <v>148</v>
-      </c>
-      <c r="F334" s="7"/>
-    </row>
-    <row r="335" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E335" t="s">
-        <v>149</v>
-      </c>
-      <c r="F335" s="7"/>
+      <c r="E335" s="3"/>
+      <c r="F335" s="3"/>
+      <c r="G335" s="3"/>
     </row>
     <row r="336" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E336" t="s">
-        <v>150</v>
-      </c>
-      <c r="F336" s="7"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="337" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E337" t="s">
-        <v>151</v>
-      </c>
-      <c r="F337" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F337" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="338" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E338" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F338" s="7"/>
     </row>
     <row r="339" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E339" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F339" s="7"/>
     </row>
     <row r="340" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E340" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F340" s="7"/>
     </row>
     <row r="341" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E341" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F341" s="7"/>
     </row>
     <row r="342" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E342" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F342" s="7"/>
     </row>
     <row r="343" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E343" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F343" s="7"/>
     </row>
     <row r="344" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E344" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F344" s="7"/>
     </row>
     <row r="345" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E345" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F345" s="7"/>
     </row>
+    <row r="346" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E346" t="s">
+        <v>155</v>
+      </c>
+      <c r="F346" s="7"/>
+    </row>
     <row r="347" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B347" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="348" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D348" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="E348" s="3"/>
-      <c r="F348" s="3"/>
-      <c r="G348" s="3"/>
+      <c r="E347" t="s">
+        <v>156</v>
+      </c>
+      <c r="F347" s="7"/>
+    </row>
+    <row r="348" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E348" t="s">
+        <v>157</v>
+      </c>
+      <c r="F348" s="7"/>
     </row>
     <row r="349" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E349" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="350" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E350" t="s">
-        <v>101</v>
-      </c>
-      <c r="F350" t="s">
-        <v>9</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="F349" s="7"/>
     </row>
     <row r="351" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E351" t="s">
-        <v>161</v>
-      </c>
-      <c r="F351" s="7"/>
-    </row>
-    <row r="352" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E352" t="s">
-        <v>162</v>
-      </c>
-      <c r="F352" s="7"/>
+      <c r="B351" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="352" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D352" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E352" s="3"/>
+      <c r="F352" s="3"/>
+      <c r="G352" s="3"/>
     </row>
     <row r="353" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E353" t="s">
-        <v>163</v>
-      </c>
-      <c r="F353" s="7"/>
+        <v>192</v>
+      </c>
     </row>
     <row r="354" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E354" t="s">
-        <v>164</v>
-      </c>
-      <c r="F354" s="7"/>
-    </row>
-    <row r="357" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C357" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D357" s="2"/>
-      <c r="E357" s="2"/>
-      <c r="F357" s="2"/>
-      <c r="G357" s="2"/>
-    </row>
-    <row r="358" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="359" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D359" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E359" s="3"/>
-      <c r="F359" s="3"/>
-      <c r="G359" s="3"/>
-    </row>
-    <row r="360" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E360" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="361" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E361" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="362" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E362" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F362" s="7"/>
-    </row>
-    <row r="363" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E363" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="F363" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="F354" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="355" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E355" t="s">
+        <v>160</v>
+      </c>
+      <c r="F355" s="7"/>
+    </row>
+    <row r="356" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E356" t="s">
+        <v>161</v>
+      </c>
+      <c r="F356" s="7"/>
+    </row>
+    <row r="357" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E357" t="s">
+        <v>162</v>
+      </c>
+      <c r="F357" s="7"/>
+    </row>
+    <row r="358" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E358" t="s">
+        <v>163</v>
+      </c>
+      <c r="F358" s="7"/>
+    </row>
+    <row r="361" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C361" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D361" s="2"/>
+      <c r="E361" s="2"/>
+      <c r="F361" s="2"/>
+      <c r="G361" s="2"/>
+    </row>
+    <row r="362" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="363" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D363" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E363" s="3"/>
+      <c r="F363" s="3"/>
+      <c r="G363" s="3"/>
     </row>
     <row r="364" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E364" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
     </row>
     <row r="365" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E365" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="F365" s="7"/>
+      <c r="E365" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="366" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E366" s="8" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F366" s="7"/>
     </row>
     <row r="367" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E367" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F367" s="7"/>
+    </row>
+    <row r="368" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E368" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="369" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E369" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F369" s="7"/>
+    </row>
+    <row r="370" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E370" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F370" s="7"/>
+    </row>
+    <row r="371" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E371" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F371" s="7"/>
+    </row>
+    <row r="372" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E372" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F372" s="7"/>
+    </row>
+    <row r="374" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E374" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="375" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E375" s="7"/>
+    </row>
+    <row r="376" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E376" t="s">
         <v>203</v>
       </c>
-      <c r="F367" s="7"/>
-    </row>
-    <row r="368" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E368" s="8" t="s">
+    </row>
+    <row r="377" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E377" s="7"/>
+    </row>
+    <row r="378" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E378" t="s">
         <v>204</v>
       </c>
-      <c r="F368" s="7"/>
-    </row>
-    <row r="370" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E370" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="371" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E371" s="7"/>
-    </row>
-    <row r="372" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E372" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="373" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E373" s="7"/>
-    </row>
-    <row r="374" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E374" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="375" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E375" s="7"/>
+    </row>
+    <row r="379" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E379" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9 E44 E36" xr:uid="{3C594C12-590A-7343-A03C-F6F925CF2C6D}">
       <formula1>YesNoPartial</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25 E63 E65 E86 E88 E90 E92 E96 E98 E104 E106 E114 E116:E117 E120 E122 E124 E126 E130 E132 E138 E140 E142 E144 E150 E156 E160 E166 E168 F173:F178 E184 E186 E188 E190 E194 E196 E204 E206 E230 E228 E236 E238 E232 E224 E220 E216 E212 E246 E258 E281 E283 E285 E289 E291 E293 E295 E301 E303 E307 E309 E311 E315 E317 E319 E324 F351:F354 F362:F363 F365:F368 E371 E373 E375" xr:uid="{4BED4D73-49DB-8D4A-8D1E-63B573D30EBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25 E63 E65 E86 E88 E90 E92 E96 E98 E104 E106 E114 E116:E117 E120 E122 E124 E126 E130 E132 E138 E140 E142 E144 E150 E156 E160 E166 E168 F173:F178 E184 E186 E188 E190 E194 E196 E204 E206 E230 E228 E236 E238 E232 E224 E220 E216 E212 E246 E258 E281 E283 E285 E289 E291 E293 E295 E301 E303 E307 E309 E311 E315 E319 E323 E328 F355:F358 F366:F367 F369:F372 E375 E377 E379" xr:uid="{4BED4D73-49DB-8D4A-8D1E-63B573D30EBF}">
       <formula1>YesNo</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added Sync Perf checks
</commit_message>
<xml_diff>
--- a/assets/AzureADAssessment-Interview.xlsx
+++ b/assets/AzureADAssessment-Interview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Documents/GitHub/AzureADAssessment/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0205EB20-79CE-B343-A9A7-4FF86C0F649F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138B55B3-0AF4-1B48-BC79-0A4160C7D715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15780" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15780" activeTab="2" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Guided Walkthrough" sheetId="3" r:id="rId1"/>
@@ -20,86 +20,90 @@
   </sheets>
   <definedNames>
     <definedName name="AADC_Are_there_custom_rules_with_precedence_value_over_100">'Post-Interview Assessment'!$E$36</definedName>
+    <definedName name="AADC_Are_there_full_sync_cycles_that_are_not_needed">'Post-Interview Assessment'!$E$58</definedName>
     <definedName name="AADC_Are_there_overly_complex_rules">'Post-Interview Assessment'!$E$40</definedName>
+    <definedName name="AADC_Are_there_significant_discrepancies_between_the_delta_sync_performance_of_staging_and_production">'Post-Interview Assessment'!$E$54</definedName>
     <definedName name="AADC_Are_there_sync_errors_lingering_for_more_than_100_days">'Post-Interview Assessment'!$E$14</definedName>
     <definedName name="AADC_Are_there_too_many_objects_being_imported_that_are_not_exported_to_the_cloud">'Post-Interview Assessment'!$E$20</definedName>
+    <definedName name="AADC_Is_delta_sync_taking_over_30_minutes_for_95th_percentile">'Post-Interview Assessment'!$E$50</definedName>
     <definedName name="AADC_Is_Group_Filtering_used_in_Production">'Post-Interview Assessment'!$E$44</definedName>
     <definedName name="AADC_Is_ms_ds_ConsistencyGuid_used_as_the_source_anchor__instead_of_ObjectGuid">'Post-Interview Assessment'!$E$32</definedName>
     <definedName name="AADC_Is_the_Azure_AD_Connect_version_more_than_6_months_behind_the_latest_release">'Post-Interview Assessment'!$E$28</definedName>
+    <definedName name="AADC_Is_there_a_consistent_volume_trend_of_add_deletes_over_1__and_or_updates_is_over_10">'Post-Interview Assessment'!$E$62</definedName>
     <definedName name="AADC_Is_there_a_mismatch_between_the_production_and_staging_configuration">'Post-Interview Assessment'!$E$24</definedName>
-    <definedName name="AccMgmt_Are_all_your_office_clients_in_versions_that_support_modern_authentication">'Interview Questions'!$E$205</definedName>
-    <definedName name="AccMgmt_Are_strong_credentials_used_for_SSPR">'Interview Questions'!$E$113</definedName>
-    <definedName name="AccMgmt_Are_strong_credentials_used_in_conditional_access_policies">'Interview Questions'!$E$111</definedName>
-    <definedName name="AccMgmt_Are_there_applications_that_can_be_candidates_to_use_attribute_based_access_control">'Interview Questions'!$E$181</definedName>
-    <definedName name="AccMgmt_Are_you_Archiving_AD_FS_audits">'Interview Questions'!$E$249</definedName>
-    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_security_incident_response">'Interview Questions'!$E$257</definedName>
-    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_support_and_troubleshooting_access_issues">'Interview Questions'!$E$259</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$241</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$245</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Sign_in_Activity_Logs">'Interview Questions'!$E$237</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Office_365_activity_logs">'Interview Questions'!$E$253</definedName>
-    <definedName name="AccMgmt_Do_you_enable_SSO_for_capable_apps_or_are_the_apps_that_use_local_accounts">'Interview Questions'!$E$163</definedName>
-    <definedName name="AccMgmt_Do_you_have_a_self_service_password_reset_solution">'Interview Questions'!$E$84</definedName>
-    <definedName name="AccMgmt_Do_you_have_a_SIEM_system">'Interview Questions'!$E$233</definedName>
-    <definedName name="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today">'Interview Questions'!$E$177</definedName>
-    <definedName name="AccMgmt_Do_you_have_applications_that_support_SAML_OpenID_connect_or_OAuth">'Interview Questions'!$E$159</definedName>
-    <definedName name="AccMgmt_Do_you_have_desktop_management_policies">'Interview Questions'!$E$143</definedName>
-    <definedName name="AccMgmt_Do_you_have_initiative_to_migrate_SSO_configuration_from_AD_FS_to_Azure_AD">'Interview Questions'!$E$171</definedName>
-    <definedName name="AccMgmt_Do_you_have_Intune_Application_Management_MAM_policies_defined">'Interview Questions'!$E$187</definedName>
-    <definedName name="AccMgmt_Do_you_have_mobile_management_policies_defined">'Interview Questions'!$E$141</definedName>
-    <definedName name="AccMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$65</definedName>
-    <definedName name="AccMgmt_Do_you_have_scripts_that_run_on_a_regular_basis">'Interview Questions'!$E$125</definedName>
-    <definedName name="AccMgmt_Do_you_have_service_accounts_or_applications_that_rely_on_legacy_authentication">'Interview Questions'!$E$211</definedName>
-    <definedName name="AccMgmt_Do_you_provision_strong_credentials_alongside_identity_provisioning_or_device_provisioning">'Interview Questions'!$E$109</definedName>
-    <definedName name="AccMgmt_Do_you_provision_strong_credentials_to_all_users_with_privileged_roles">'Interview Questions'!$E$107</definedName>
-    <definedName name="AccMgmt_Do_you_use_device_compliance_as_a_control_in_Conditional_Access">'Interview Questions'!$E$147</definedName>
-    <definedName name="AccMgmt_Do_you_use_them_in_CA_policies">'Interview Questions'!$E$189</definedName>
-    <definedName name="AccMgmt_Do_your_users_use_Windows_Hello_in_their_Windows_10_Desktops">'Interview Questions'!$E$151</definedName>
-    <definedName name="AccMgmt_Have_you_deployed_Azure_Log_Analytics">'Interview Questions'!$E$225</definedName>
-    <definedName name="AccMgmt_Have_you_deployed_Hybrid_Azure_AD_joined_in_your_environment">'Interview Questions'!$E$145</definedName>
-    <definedName name="AccMgmt_Have_you_deployed_Windows_Hello_as_an_enterprise_wide_policy">'Interview Questions'!$E$153</definedName>
-    <definedName name="AccMgmt_Have_you_enabled_All_Office_365_Auditing">'Interview Questions'!$E$251</definedName>
-    <definedName name="AccMgmt_Have_you_enabled_Password_Hash_Sync">'Interview Questions'!$E$117</definedName>
-    <definedName name="AccMgmt_Have_you_explicitly_identified_regions_where_authentication_should_NOT_be_coming_from">'Interview Questions'!$E$217</definedName>
-    <definedName name="AccMgmt_Have_you_identified_the_regions_of_the_world_where_authentication_traffic_should_be_coming_from">'Interview Questions'!$E$215</definedName>
-    <definedName name="AccMgmt_If_so_do_you_have_a_dedicated_service_principal_to_run_it_against">'Interview Questions'!$E$127</definedName>
-    <definedName name="AccMgmt_If_so_do_you_have_configured_the_applications_to_support_SSO_using_those_protocols">'Interview Questions'!$E$161</definedName>
-    <definedName name="AccMgmt_If_so_does_your_operations_team_use_it_regularly_to_understand_Azure_AD_usage">'Interview Questions'!$E$227</definedName>
-    <definedName name="AccMgmt_If_you_are_using_passwords_how_do_you_manage_the_them">'Interview Questions'!$E$129</definedName>
-    <definedName name="AccMgmt_If_you_use_cloud_authentication_PHS_or_PTA_do_you_have_Seamless_SSO_enabled">'Interview Questions'!$E$135</definedName>
-    <definedName name="AccMgmt_If_you_use_federated_authentication_do_you_use_windows_integrated_authentication_WIA_when_inside_the_corporate_network">'Interview Questions'!$E$137</definedName>
-    <definedName name="AccMgmt_Is_legacy_authentication_blocked_by_conditional_access">'Interview Questions'!$E$209</definedName>
-    <definedName name="AccMgmt_Is_legacy_authentication_disabled_at_the_mailbox_level">'Interview Questions'!$E$207</definedName>
-    <definedName name="AccMgmt_Is_the_password_reset_part_of_the_operational_procedures_to_remediate_a_user_incident">'Interview Questions'!$E$86</definedName>
-    <definedName name="AccMgmt_Is_the_procedure_to_switch_to_PHS_practiced_enabled_to_the_IAM_Ops_team">'Interview Questions'!$E$119</definedName>
-    <definedName name="AccMgmt_What_platforms_do_you_use_to_provide_SSO_to_the_applications">'Interview Questions'!$E$165</definedName>
-    <definedName name="AccMgmt_What_process_do_you_have_to_discover_applications_that_are_not_configured_using_the_SSO_enterprise_solution">'Interview Questions'!$E$167</definedName>
+    <definedName name="AccMgmt_Are_all_your_office_clients_in_versions_that_support_modern_authentication">'Interview Questions'!$E$206</definedName>
+    <definedName name="AccMgmt_Are_strong_credentials_used_for_SSPR">'Interview Questions'!$E$114</definedName>
+    <definedName name="AccMgmt_Are_strong_credentials_used_in_conditional_access_policies">'Interview Questions'!$E$112</definedName>
+    <definedName name="AccMgmt_Are_there_applications_that_can_be_candidates_to_use_attribute_based_access_control">'Interview Questions'!$E$182</definedName>
+    <definedName name="AccMgmt_Are_you_Archiving_AD_FS_audits">'Interview Questions'!$E$250</definedName>
+    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_security_incident_response">'Interview Questions'!$E$258</definedName>
+    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_support_and_troubleshooting_access_issues">'Interview Questions'!$E$260</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$242</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$246</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Sign_in_Activity_Logs">'Interview Questions'!$E$238</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Office_365_activity_logs">'Interview Questions'!$E$254</definedName>
+    <definedName name="AccMgmt_Do_you_enable_SSO_for_capable_apps_or_are_the_apps_that_use_local_accounts">'Interview Questions'!$E$164</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_self_service_password_reset_solution">'Interview Questions'!$E$85</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_SIEM_system">'Interview Questions'!$E$234</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today">'Interview Questions'!$E$178</definedName>
+    <definedName name="AccMgmt_Do_you_have_applications_that_support_SAML_OpenID_connect_or_OAuth">'Interview Questions'!$E$160</definedName>
+    <definedName name="AccMgmt_Do_you_have_desktop_management_policies">'Interview Questions'!$E$144</definedName>
+    <definedName name="AccMgmt_Do_you_have_initiative_to_migrate_SSO_configuration_from_AD_FS_to_Azure_AD">'Interview Questions'!$E$172</definedName>
+    <definedName name="AccMgmt_Do_you_have_Intune_Application_Management_MAM_policies_defined">'Interview Questions'!$E$188</definedName>
+    <definedName name="AccMgmt_Do_you_have_mobile_management_policies_defined">'Interview Questions'!$E$142</definedName>
+    <definedName name="AccMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$66</definedName>
+    <definedName name="AccMgmt_Do_you_have_scripts_that_run_on_a_regular_basis">'Interview Questions'!$E$126</definedName>
+    <definedName name="AccMgmt_Do_you_have_service_accounts_or_applications_that_rely_on_legacy_authentication">'Interview Questions'!$E$212</definedName>
+    <definedName name="AccMgmt_Do_you_provision_strong_credentials_alongside_identity_provisioning_or_device_provisioning">'Interview Questions'!$E$110</definedName>
+    <definedName name="AccMgmt_Do_you_provision_strong_credentials_to_all_users_with_privileged_roles">'Interview Questions'!$E$108</definedName>
+    <definedName name="AccMgmt_Do_you_use_device_compliance_as_a_control_in_Conditional_Access">'Interview Questions'!$E$148</definedName>
+    <definedName name="AccMgmt_Do_you_use_them_in_CA_policies">'Interview Questions'!$E$190</definedName>
+    <definedName name="AccMgmt_Do_your_users_use_Windows_Hello_in_their_Windows_10_Desktops">'Interview Questions'!$E$152</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Azure_Log_Analytics">'Interview Questions'!$E$226</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Hybrid_Azure_AD_joined_in_your_environment">'Interview Questions'!$E$146</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Windows_Hello_as_an_enterprise_wide_policy">'Interview Questions'!$E$154</definedName>
+    <definedName name="AccMgmt_Have_you_enabled_All_Office_365_Auditing">'Interview Questions'!$E$252</definedName>
+    <definedName name="AccMgmt_Have_you_enabled_Password_Hash_Sync">'Interview Questions'!$E$118</definedName>
+    <definedName name="AccMgmt_Have_you_explicitly_identified_regions_where_authentication_should_NOT_be_coming_from">'Interview Questions'!$E$218</definedName>
+    <definedName name="AccMgmt_Have_you_identified_the_regions_of_the_world_where_authentication_traffic_should_be_coming_from">'Interview Questions'!$E$216</definedName>
+    <definedName name="AccMgmt_If_so_do_you_have_a_dedicated_service_principal_to_run_it_against">'Interview Questions'!$E$128</definedName>
+    <definedName name="AccMgmt_If_so_do_you_have_configured_the_applications_to_support_SSO_using_those_protocols">'Interview Questions'!$E$162</definedName>
+    <definedName name="AccMgmt_If_so_does_your_operations_team_use_it_regularly_to_understand_Azure_AD_usage">'Interview Questions'!$E$228</definedName>
+    <definedName name="AccMgmt_If_you_are_using_passwords_how_do_you_manage_the_them">'Interview Questions'!$E$130</definedName>
+    <definedName name="AccMgmt_If_you_use_cloud_authentication_PHS_or_PTA_do_you_have_Seamless_SSO_enabled">'Interview Questions'!$E$136</definedName>
+    <definedName name="AccMgmt_If_you_use_federated_authentication_do_you_use_windows_integrated_authentication_WIA_when_inside_the_corporate_network">'Interview Questions'!$E$138</definedName>
+    <definedName name="AccMgmt_Is_legacy_authentication_blocked_by_conditional_access">'Interview Questions'!$E$210</definedName>
+    <definedName name="AccMgmt_Is_legacy_authentication_disabled_at_the_mailbox_level">'Interview Questions'!$E$208</definedName>
+    <definedName name="AccMgmt_Is_the_password_reset_part_of_the_operational_procedures_to_remediate_a_user_incident">'Interview Questions'!$E$87</definedName>
+    <definedName name="AccMgmt_Is_the_procedure_to_switch_to_PHS_practiced_enabled_to_the_IAM_Ops_team">'Interview Questions'!$E$120</definedName>
+    <definedName name="AccMgmt_What_platforms_do_you_use_to_provide_SSO_to_the_applications">'Interview Questions'!$E$166</definedName>
+    <definedName name="AccMgmt_What_process_do_you_have_to_discover_applications_that_are_not_configured_using_the_SSO_enterprise_solution">'Interview Questions'!$E$168</definedName>
     <definedName name="AD_AssessmentDate">'Interview Questions'!$E$14</definedName>
     <definedName name="AD_AssessorName">'Interview Questions'!$E$11</definedName>
     <definedName name="AD_OrgName">'Interview Questions'!$E$5</definedName>
     <definedName name="AD_OrgPrimaryContact">'Interview Questions'!$E$8</definedName>
-    <definedName name="EntMgmt_Do_you_use_Azure_AD_Outbound_provisioning_for_applications_in_your_environment_that_supports_Azure_AD_provisioning">'Interview Questions'!$E$57</definedName>
+    <definedName name="EntMgmt_Do_you_use_Azure_AD_Outbound_provisioning_for_applications_in_your_environment_that_supports_Azure_AD_provisioning">'Interview Questions'!$E$58</definedName>
     <definedName name="EntMgmt_What_is_the_approach_to_provision_to_applications_today">'Interview Questions'!$E$55</definedName>
-    <definedName name="Gov_Access_Review_Guest_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$316</definedName>
-    <definedName name="Gov_Access_Review_Guest_Is_it_automated">'Interview Questions'!$E$304</definedName>
-    <definedName name="Gov_AccessReview_Privileged_If_so_are_they_automated">'Interview Questions'!$E$332</definedName>
-    <definedName name="Gov_All_Users_Is_it_automated">'Interview Questions'!$E$314</definedName>
-    <definedName name="Gov_Are_there_system_accounts_that_are_also_privileged">'Interview Questions'!$E$336</definedName>
-    <definedName name="Gov_Do_administrators_have_dedicated_accounts_used_to_perform_privileged_operations">'Interview Questions'!$E$324</definedName>
-    <definedName name="Gov_Do_administrators_have_standing_access_to_privileges_in_your_environment">'Interview Questions'!$E$322</definedName>
-    <definedName name="Gov_Do_you_assign_users_to_the_All_Users_group">'Interview Questions'!$E$312</definedName>
-    <definedName name="Gov_Do_you_have_a_guest_access_review_strategy_in_place">'Interview Questions'!$E$310</definedName>
-    <definedName name="Gov_Do_you_have_a_privileged_role_strategy_for_Azure_Resources">'Interview Questions'!$E$344</definedName>
-    <definedName name="Gov_Do_you_have_a_process_to_identify_the_least_privileged_role_to_different_users_in_your_organization">'Interview Questions'!$E$328</definedName>
-    <definedName name="Gov_Do_you_have_a_test_environment">'Interview Questions'!$E$279</definedName>
-    <definedName name="Gov_Do_you_have_access_reviews_in_place_for_privileged_accounts">'Interview Questions'!$E$330</definedName>
-    <definedName name="Gov_Do_you_have_an_access_review_strategy_in_place">'Interview Questions'!$E$302</definedName>
-    <definedName name="Gov_Do_you_have_emergency_accounts_also_known_as_break_glass_provisioned_in_your_Azure_AD_tenant">'Interview Questions'!$E$349</definedName>
-    <definedName name="Gov_Do_you_have_owners_in_your_organization_for_all_the_tasks_listed_below">'Interview Questions'!$E$267</definedName>
-    <definedName name="Gov_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$306</definedName>
-    <definedName name="Gov_If_not_what_is_the_strategy_to_clean_up_remove_access">'Interview Questions'!$E$334</definedName>
-    <definedName name="Gov_If_so_how_do_establish_ownership_of_those_accounts">'Interview Questions'!$E$338</definedName>
-    <definedName name="Gov_Is_there_any_global_admin_outside_the_IAM_team">'Interview Questions'!$E$340</definedName>
+    <definedName name="Gov_Access_Review_Guest_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$317</definedName>
+    <definedName name="Gov_Access_Review_Guest_Is_it_automated">'Interview Questions'!$E$305</definedName>
+    <definedName name="Gov_AccessReview_Privileged_If_so_are_they_automated">'Interview Questions'!$E$333</definedName>
+    <definedName name="Gov_All_Users_Is_it_automated">'Interview Questions'!$E$315</definedName>
+    <definedName name="Gov_Are_there_system_accounts_that_are_also_privileged">'Interview Questions'!$E$337</definedName>
+    <definedName name="Gov_Do_administrators_have_dedicated_accounts_used_to_perform_privileged_operations">'Interview Questions'!$E$325</definedName>
+    <definedName name="Gov_Do_administrators_have_standing_access_to_privileges_in_your_environment">'Interview Questions'!$E$323</definedName>
+    <definedName name="Gov_Do_you_assign_users_to_the_All_Users_group">'Interview Questions'!$E$313</definedName>
+    <definedName name="Gov_Do_you_have_a_guest_access_review_strategy_in_place">'Interview Questions'!$E$311</definedName>
+    <definedName name="Gov_Do_you_have_a_privileged_role_strategy_for_Azure_Resources">'Interview Questions'!$E$345</definedName>
+    <definedName name="Gov_Do_you_have_a_process_to_identify_the_least_privileged_role_to_different_users_in_your_organization">'Interview Questions'!$E$329</definedName>
+    <definedName name="Gov_Do_you_have_a_test_environment">'Interview Questions'!$E$280</definedName>
+    <definedName name="Gov_Do_you_have_access_reviews_in_place_for_privileged_accounts">'Interview Questions'!$E$331</definedName>
+    <definedName name="Gov_Do_you_have_an_access_review_strategy_in_place">'Interview Questions'!$E$303</definedName>
+    <definedName name="Gov_Do_you_have_emergency_accounts_also_known_as_break_glass_provisioned_in_your_Azure_AD_tenant">'Interview Questions'!$E$350</definedName>
+    <definedName name="Gov_Do_you_have_owners_in_your_organization_for_all_the_tasks_listed_below">'Interview Questions'!$E$268</definedName>
+    <definedName name="Gov_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$307</definedName>
+    <definedName name="Gov_If_not_what_is_the_strategy_to_clean_up_remove_access">'Interview Questions'!$E$335</definedName>
+    <definedName name="Gov_If_so_how_do_establish_ownership_of_those_accounts">'Interview Questions'!$E$339</definedName>
+    <definedName name="Gov_Is_there_any_global_admin_outside_the_IAM_team">'Interview Questions'!$E$341</definedName>
     <definedName name="IdMgmt_Do_you_have_a_disaster_recovery_production_instance_of_AAD_Connect_deployed_in_Staging_Mode">'Interview Questions'!$E$45</definedName>
     <definedName name="IdMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$23</definedName>
     <definedName name="IdMgmt_Do_you_synchronize_the_same_forest_where_users_log_in_to_their_Windows_devices">'Interview Questions'!$E$39</definedName>
@@ -111,19 +115,19 @@
     <definedName name="Lic_If_GBL_is_not_used__how_would_you_rate_your_current_approach_to_licensing">'Guided Walkthrough'!$G$116</definedName>
     <definedName name="Lic_If_yes__is_GBL_deployed_against_on_premises_groups_that_lack_lifecycle_management">'Guided Walkthrough'!$G$113</definedName>
     <definedName name="LookupLicenceMaturity">Lookups!$B$14:$B$17</definedName>
-    <definedName name="Ops_Are_there_compensating_controls_for_cases_where_the_answer_above_is_No">'Interview Questions'!$E$400</definedName>
-    <definedName name="Ops_Azure_AD_App_Proxy_debug_connector_group_deployed">'Interview Questions'!$F$378</definedName>
-    <definedName name="Ops_Debugging_tools_deployed_in_debug_app_proxy_connector">'Interview Questions'!$F$379</definedName>
-    <definedName name="Ops_Is_any_of_the_servers_above_virtualized_If_so__is_there_proper_isolation_between_VM_Host_administrators_and_the_IAM_team">'Interview Questions'!$E$396</definedName>
-    <definedName name="Ops_Is_there_proper_isolation_between_SQL_Admins_and_the_IAM_team">'Interview Questions'!$E$398</definedName>
-    <definedName name="Ops_Multiple_Azure_AD_Application_Proxy_connectors_per_group_deployed">'Interview Questions'!$F$376</definedName>
-    <definedName name="Ops_Multiple_Azure_AD_Pass_through_authentication_agents_deployed">'Interview Questions'!$F$377</definedName>
-    <definedName name="Ops_Secured_Azure_AD_App_Proxy_Connector">'Interview Questions'!$F$391</definedName>
-    <definedName name="Ops_Secured_Azure_AD_Connect_Servers">'Interview Questions'!$F$387</definedName>
-    <definedName name="Ops_Secured_NPS_Extension">'Interview Questions'!$F$393</definedName>
-    <definedName name="Ops_Secured_Pass_through_Authentication_Agent">'Interview Questions'!$F$392</definedName>
-    <definedName name="Ops_Secured_SQL_Server_for_ADFS">'Interview Questions'!$F$390</definedName>
-    <definedName name="Ops_Secured_SQL_Server_for_Azure_AD_Connect">'Interview Questions'!$F$388</definedName>
+    <definedName name="Ops_Are_there_compensating_controls_for_cases_where_the_answer_above_is_No">'Interview Questions'!$E$401</definedName>
+    <definedName name="Ops_Azure_AD_App_Proxy_debug_connector_group_deployed">'Interview Questions'!$F$379</definedName>
+    <definedName name="Ops_Debugging_tools_deployed_in_debug_app_proxy_connector">'Interview Questions'!$F$380</definedName>
+    <definedName name="Ops_Is_any_of_the_servers_above_virtualized_If_so__is_there_proper_isolation_between_VM_Host_administrators_and_the_IAM_team">'Interview Questions'!$E$397</definedName>
+    <definedName name="Ops_Is_there_proper_isolation_between_SQL_Admins_and_the_IAM_team">'Interview Questions'!$E$399</definedName>
+    <definedName name="Ops_Multiple_Azure_AD_Application_Proxy_connectors_per_group_deployed">'Interview Questions'!$F$377</definedName>
+    <definedName name="Ops_Multiple_Azure_AD_Pass_through_authentication_agents_deployed">'Interview Questions'!$F$378</definedName>
+    <definedName name="Ops_Secured_Azure_AD_App_Proxy_Connector">'Interview Questions'!$F$392</definedName>
+    <definedName name="Ops_Secured_Azure_AD_Connect_Servers">'Interview Questions'!$F$388</definedName>
+    <definedName name="Ops_Secured_NPS_Extension">'Interview Questions'!$F$394</definedName>
+    <definedName name="Ops_Secured_Pass_through_Authentication_Agent">'Interview Questions'!$F$393</definedName>
+    <definedName name="Ops_Secured_SQL_Server_for_ADFS">'Interview Questions'!$F$391</definedName>
+    <definedName name="Ops_Secured_SQL_Server_for_Azure_AD_Connect">'Interview Questions'!$F$389</definedName>
     <definedName name="YesNo">Lookups!$B$9:$B$11</definedName>
     <definedName name="YesNoPartial">Lookups!$B$3:$B$6</definedName>
   </definedNames>
@@ -147,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="428">
   <si>
     <t>Identity Management</t>
   </si>
@@ -1347,9 +1351,117 @@
     <t>8 Jan 2020</t>
   </si>
   <si>
+    <t>Sync Configuration</t>
+  </si>
+  <si>
+    <t>Are there too many objects being imported that are not exported to the cloud?</t>
+  </si>
+  <si>
+    <t>Sync Issues</t>
+  </si>
+  <si>
+    <t>Source: Azure AD Config Documenter Output</t>
+  </si>
+  <si>
+    <t>Do you have a disaster recovery production instance of AAD Connect deployed in Staging Mode?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If yes, do you have a process in place to ensure the configuration of the instances are kept in sync? </t>
+  </si>
+  <si>
+    <t>Is there a mismatch between the production and staging configuration?</t>
+  </si>
+  <si>
+    <t>Source: AAD Connect Health Portal ScreenShot or **Power BI: Telemetry - Tab 'AADCH – Alerts'</t>
+  </si>
+  <si>
+    <t>Source: Azure AD Config Documenter Output or **Power BI: Telemetry - Tab 'AADCH – Alerts'</t>
+  </si>
+  <si>
+    <t>Is the Azure AD Connect version more than 6 months behind the latest release?</t>
+  </si>
+  <si>
+    <t>Is ms-ds-ConsistencyGuid used as the source anchor (instead of ObjectGuid)?</t>
+  </si>
+  <si>
+    <t>Source: **Power BI: Telemetry - Tab "Sync – Object Count"</t>
+  </si>
+  <si>
+    <t>Are there custom rules with precedence value over 100?</t>
+  </si>
+  <si>
+    <t>Are there overly complex rules?</t>
+  </si>
+  <si>
+    <t>Is Group Filtering used in Production?</t>
+  </si>
+  <si>
+    <t>Group Based Licensing</t>
+  </si>
+  <si>
+    <t>Are there outstanding licensing errors shown in the portal?</t>
+  </si>
+  <si>
+    <t>Source: Licences &gt; Overview blade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have a defined process (automated or manual) to monitor and resolve licensing errors? </t>
+  </si>
+  <si>
+    <t>Does your existing license assignment strategy fully cover Joiners/Movers/Leavers consistently?</t>
+  </si>
+  <si>
+    <t>License Assignment</t>
+  </si>
+  <si>
+    <t>Ad hoc</t>
+  </si>
+  <si>
+    <t>Standardized</t>
+  </si>
+  <si>
+    <t>Mature</t>
+  </si>
+  <si>
+    <t>Standardized: but manual process to assign licenses and assign components to users</t>
+  </si>
+  <si>
+    <t>Do you use Group Based Licensing to assign licenses?</t>
+  </si>
+  <si>
+    <t>If yes, is GBL deployed against on-premises groups that lack lifecycle management?</t>
+  </si>
+  <si>
+    <t>If GBL is not used, how would you rate your current approach to licensing?</t>
+  </si>
+  <si>
+    <t>Ad hoc: manual process to assign licenses and assign components to users</t>
+  </si>
+  <si>
+    <t>Mature: process and tools to assign licenses to users (e.g. MIM / Oracle Access Manager, etc.), but rely on on-premises infrastructure</t>
+  </si>
+  <si>
+    <t>Sync Performance</t>
+  </si>
+  <si>
+    <t>Is delta sync taking over 30 minutes for 95th percentile?</t>
+  </si>
+  <si>
+    <t>Source: **Power BI: Telemetry - Tab "Sync Performance"</t>
+  </si>
+  <si>
+    <t>Are there significant discrepancies between the delta sync performance of staging and production?</t>
+  </si>
+  <si>
+    <t>Are there full sync cycles that are not needed?</t>
+  </si>
+  <si>
+    <t>Is there a consistent volume trend of add/deletes over 1% and/or updates is over 10%?</t>
+  </si>
+  <si>
     <r>
       <t>This post-interview section needs to be filled in by the person performing the assessment. The questions in this section cover areas that are not currently accessible by the Graph API or rely on analysis of Power BI data and other outputs from on-premises components. 
-If you are not a Microsoft Identity team member the questions relying on a source marked with '</t>
+If you are not a Microsoft Identity team member please mark  the questions relying on a source marked with '</t>
     </r>
     <r>
       <rPr>
@@ -1370,7 +1482,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>' should be answered as '</t>
+      <t>' as '</t>
     </r>
     <r>
       <rPr>
@@ -1393,96 +1505,6 @@
       </rPr>
       <t>'</t>
     </r>
-  </si>
-  <si>
-    <t>Sync Configuration</t>
-  </si>
-  <si>
-    <t>Are there too many objects being imported that are not exported to the cloud?</t>
-  </si>
-  <si>
-    <t>Sync Issues</t>
-  </si>
-  <si>
-    <t>Source: Azure AD Config Documenter Output</t>
-  </si>
-  <si>
-    <t>Do you have a disaster recovery production instance of AAD Connect deployed in Staging Mode?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If yes, do you have a process in place to ensure the configuration of the instances are kept in sync? </t>
-  </si>
-  <si>
-    <t>Is there a mismatch between the production and staging configuration?</t>
-  </si>
-  <si>
-    <t>Source: AAD Connect Health Portal ScreenShot or **Power BI: Telemetry - Tab 'AADCH – Alerts'</t>
-  </si>
-  <si>
-    <t>Source: Azure AD Config Documenter Output or **Power BI: Telemetry - Tab 'AADCH – Alerts'</t>
-  </si>
-  <si>
-    <t>Is the Azure AD Connect version more than 6 months behind the latest release?</t>
-  </si>
-  <si>
-    <t>Is ms-ds-ConsistencyGuid used as the source anchor (instead of ObjectGuid)?</t>
-  </si>
-  <si>
-    <t>Source: **Power BI: Telemetry - Tab "Sync – Object Count"</t>
-  </si>
-  <si>
-    <t>Are there custom rules with precedence value over 100?</t>
-  </si>
-  <si>
-    <t>Are there overly complex rules?</t>
-  </si>
-  <si>
-    <t>Is Group Filtering used in Production?</t>
-  </si>
-  <si>
-    <t>Group Based Licensing</t>
-  </si>
-  <si>
-    <t>Are there outstanding licensing errors shown in the portal?</t>
-  </si>
-  <si>
-    <t>Source: Licences &gt; Overview blade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have a defined process (automated or manual) to monitor and resolve licensing errors? </t>
-  </si>
-  <si>
-    <t>Does your existing license assignment strategy fully cover Joiners/Movers/Leavers consistently?</t>
-  </si>
-  <si>
-    <t>License Assignment</t>
-  </si>
-  <si>
-    <t>Ad hoc</t>
-  </si>
-  <si>
-    <t>Standardized</t>
-  </si>
-  <si>
-    <t>Mature</t>
-  </si>
-  <si>
-    <t>Standardized: but manual process to assign licenses and assign components to users</t>
-  </si>
-  <si>
-    <t>Do you use Group Based Licensing to assign licenses?</t>
-  </si>
-  <si>
-    <t>If yes, is GBL deployed against on-premises groups that lack lifecycle management?</t>
-  </si>
-  <si>
-    <t>If GBL is not used, how would you rate your current approach to licensing?</t>
-  </si>
-  <si>
-    <t>Ad hoc: manual process to assign licenses and assign components to users</t>
-  </si>
-  <si>
-    <t>Mature: process and tools to assign licenses to users (e.g. MIM / Oracle Access Manager, etc.), but rely on on-premises infrastructure</t>
   </si>
 </sst>
 </file>
@@ -1824,8 +1846,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1C4D0D2B-6272-644B-B58A-F2D915C5B531}" name="Table2" displayName="Table2" ref="E67:F78" totalsRowShown="0">
-  <autoFilter ref="E67:F78" xr:uid="{1C4D0D2B-6272-644B-B58A-F2D915C5B531}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1C4D0D2B-6272-644B-B58A-F2D915C5B531}" name="Table2" displayName="Table2" ref="E68:F79" totalsRowShown="0">
+  <autoFilter ref="E68:F79" xr:uid="{1C4D0D2B-6272-644B-B58A-F2D915C5B531}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C04652F9-C32E-3C48-8CFD-8D2D01D07ADB}" name="Task"/>
     <tableColumn id="2" xr3:uid="{24027322-E3B5-184F-9BAA-F77393BB4FF9}" name="Name of Person/Team owning task" dataCellStyle="20% - Accent6"/>
@@ -1835,8 +1857,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6048BA92-D829-6543-BE60-C242238787A6}" name="Table3" displayName="Table3" ref="E91:F103" totalsRowShown="0">
-  <autoFilter ref="E91:F103" xr:uid="{6048BA92-D829-6543-BE60-C242238787A6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6048BA92-D829-6543-BE60-C242238787A6}" name="Table3" displayName="Table3" ref="E92:F104" totalsRowShown="0">
+  <autoFilter ref="E92:F104" xr:uid="{6048BA92-D829-6543-BE60-C242238787A6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{65AE8C0B-4B46-A24D-86F8-26F3FA1BFA41}" name="Policy Setting"/>
     <tableColumn id="2" xr3:uid="{F0A657E9-871F-E942-AB05-DE5CB9B6CBF1}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1846,8 +1868,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}" name="Table4" displayName="Table4" ref="E193:F199" totalsRowShown="0">
-  <autoFilter ref="E193:F199" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}" name="Table4" displayName="Table4" ref="E194:F200" totalsRowShown="0">
+  <autoFilter ref="E194:F200" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2F02BBB5-1E25-204E-B1A1-4DC986B80F65}" name="Best Practice"/>
     <tableColumn id="2" xr3:uid="{3C3E276B-0F40-5E47-996E-D83E08871D21}" name="Implemented by customer?" dataCellStyle="20% - Accent6"/>
@@ -1857,8 +1879,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}" name="Table5" displayName="Table5" ref="E268:F274" totalsRowShown="0">
-  <autoFilter ref="E268:F274" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}" name="Table5" displayName="Table5" ref="E269:F275" totalsRowShown="0">
+  <autoFilter ref="E269:F275" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2457BC44-3D28-2542-B982-8033983B8754}" name="Task"/>
     <tableColumn id="2" xr3:uid="{CED65D15-1D68-B246-875D-F0A2C4A946D3}" name="Person or Team name" dataCellStyle="20% - Accent6"/>
@@ -1868,8 +1890,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}" name="Table6" displayName="Table6" ref="E284:F295" totalsRowShown="0">
-  <autoFilter ref="E284:F295" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}" name="Table6" displayName="Table6" ref="E285:F296" totalsRowShown="0">
+  <autoFilter ref="E285:F296" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A3FEF98E-FE28-B84C-8912-4098BA527E76}" name="Kind of Change"/>
     <tableColumn id="2" xr3:uid="{CC851B68-8394-934D-96E0-625A92D7812E}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1879,8 +1901,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}" name="Table7" displayName="Table7" ref="E358:F370" totalsRowShown="0">
-  <autoFilter ref="E358:F370" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}" name="Table7" displayName="Table7" ref="E359:F371" totalsRowShown="0">
+  <autoFilter ref="E359:F371" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E9AA62EB-CA64-A84A-90FE-4FB406CFBB9B}" name="Task"/>
     <tableColumn id="2" xr3:uid="{A95B16A3-9350-3B42-AEC0-844DDF1A8645}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1890,8 +1912,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}" name="Table8" displayName="Table8" ref="E375:F379" totalsRowShown="0">
-  <autoFilter ref="E375:F379" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}" name="Table8" displayName="Table8" ref="E376:F380" totalsRowShown="0">
+  <autoFilter ref="E376:F380" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8E26C403-A376-C242-AC8E-6B61F7C1302E}" name="Best Practice"/>
     <tableColumn id="2" xr3:uid="{020742E9-39A6-0A45-9032-2C3C5E3B59B3}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -2202,8 +2224,8 @@
   </sheetPr>
   <dimension ref="A2:N299"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A111" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G118" sqref="G118"/>
+    <sheetView showGridLines="0" topLeftCell="A51" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2711,7 +2733,7 @@
     </row>
     <row r="99" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G99" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="100" spans="5:7" x14ac:dyDescent="0.2">
@@ -2721,7 +2743,7 @@
     </row>
     <row r="101" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G101" s="23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="102" spans="5:7" x14ac:dyDescent="0.2">
@@ -2729,7 +2751,7 @@
     </row>
     <row r="103" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G103" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.2">
@@ -2742,7 +2764,7 @@
     </row>
     <row r="106" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G106" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="107" spans="5:7" x14ac:dyDescent="0.2">
@@ -2755,7 +2777,7 @@
     </row>
     <row r="109" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G109" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="110" spans="5:7" x14ac:dyDescent="0.2">
@@ -2768,7 +2790,7 @@
     </row>
     <row r="112" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G112" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="113" spans="5:14" x14ac:dyDescent="0.2">
@@ -2781,27 +2803,27 @@
     </row>
     <row r="115" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G115" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="116" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G116" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="117" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G117" s="23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="118" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G118" s="23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="119" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G119" s="23" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="122" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3773,10 +3795,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B2:G400"/>
+  <dimension ref="B2:G401"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView showGridLines="0" topLeftCell="A77" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3967,7 +3989,7 @@
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E44" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.2">
@@ -3977,7 +3999,7 @@
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.2">
@@ -4013,1591 +4035,1591 @@
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E56" t="s">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E57" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="1" t="s">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E58" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="2" t="s">
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D63" s="3" t="s">
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E64" t="s">
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E65" s="5" t="s">
+    <row r="66" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E66" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E67" t="s">
+    <row r="68" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
         <v>8</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F68" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E68" t="s">
+    <row r="69" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
         <v>29</v>
       </c>
-      <c r="F68" s="7"/>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E69" t="s">
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E70" t="s">
         <v>30</v>
       </c>
-      <c r="F69" s="7"/>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E70" t="s">
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
         <v>31</v>
       </c>
-      <c r="F70" s="7"/>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E71" t="s">
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
         <v>32</v>
       </c>
-      <c r="F71" s="7"/>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E72" t="s">
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
         <v>33</v>
       </c>
-      <c r="F72" s="7"/>
-    </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E73" t="s">
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
         <v>34</v>
       </c>
-      <c r="F73" s="7"/>
-    </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E74" t="s">
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
         <v>35</v>
       </c>
-      <c r="F74" s="7"/>
-    </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E75" t="s">
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
         <v>36</v>
       </c>
-      <c r="F75" s="7"/>
-    </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E76" t="s">
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
         <v>37</v>
       </c>
-      <c r="F76" s="7"/>
-    </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E77" t="s">
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
         <v>38</v>
       </c>
-      <c r="F77" s="7"/>
-    </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E78" t="s">
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
         <v>39</v>
       </c>
-      <c r="F78" s="7"/>
-    </row>
-    <row r="80" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="2" t="s">
+      <c r="F79" s="7"/>
+    </row>
+    <row r="81" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-    </row>
-    <row r="81" spans="4:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="82" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D82" s="3" t="s">
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="83" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-    </row>
-    <row r="83" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E83" t="s">
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E84" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="84" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E84" s="7" t="s">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E85" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E85" t="s">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="86" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E86" s="7"/>
-    </row>
-    <row r="87" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E87" t="s">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E87" s="7"/>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E88" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E88" s="6"/>
-    </row>
-    <row r="89" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D89" s="3" t="s">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D90" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-    </row>
-    <row r="91" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E91" t="s">
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E92" t="s">
         <v>46</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F92" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E92" t="s">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E93" t="s">
         <v>47</v>
       </c>
-      <c r="F92" s="7"/>
-    </row>
-    <row r="93" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E93" t="s">
+      <c r="F93" s="7"/>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E94" t="s">
         <v>48</v>
       </c>
-      <c r="F93" s="7"/>
-    </row>
-    <row r="94" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E94" t="s">
+      <c r="F94" s="7"/>
+    </row>
+    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E95" t="s">
         <v>49</v>
       </c>
-      <c r="F94" s="7"/>
-    </row>
-    <row r="95" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E95" t="s">
+      <c r="F95" s="7"/>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E96" t="s">
         <v>50</v>
-      </c>
-      <c r="F95" s="7"/>
-    </row>
-    <row r="96" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E96" t="s">
-        <v>51</v>
       </c>
       <c r="F96" s="7"/>
     </row>
     <row r="97" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E97" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F97" s="7"/>
     </row>
     <row r="98" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E98" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F98" s="7"/>
     </row>
     <row r="99" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E99" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F99" s="7"/>
     </row>
     <row r="100" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F100" s="7"/>
     </row>
     <row r="101" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E101" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F101" s="7"/>
     </row>
     <row r="102" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E102" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F102" s="7"/>
     </row>
     <row r="103" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E103" t="s">
+        <v>57</v>
+      </c>
+      <c r="F103" s="7"/>
+    </row>
+    <row r="104" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E104" t="s">
         <v>58</v>
       </c>
-      <c r="F103" s="7"/>
-    </row>
-    <row r="105" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D105" s="3" t="s">
+      <c r="F104" s="7"/>
+    </row>
+    <row r="106" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D106" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
-    </row>
-    <row r="106" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E106" t="s">
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+    </row>
+    <row r="107" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E107" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E107" s="7"/>
-    </row>
     <row r="108" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E108" t="s">
+      <c r="E108" s="7"/>
+    </row>
+    <row r="109" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E109" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="109" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E109" s="7"/>
-    </row>
     <row r="110" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E110" t="s">
+      <c r="E110" s="7"/>
+    </row>
+    <row r="111" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E111" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="111" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E111" s="7"/>
-    </row>
     <row r="112" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E112" t="s">
+      <c r="E112" s="7"/>
+    </row>
+    <row r="113" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E113" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="113" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E113" s="7"/>
-    </row>
-    <row r="115" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D115" s="3" t="s">
+    <row r="114" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E114" s="7"/>
+    </row>
+    <row r="116" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D116" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-      <c r="G115" s="3"/>
-    </row>
-    <row r="116" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E116" t="s">
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+    </row>
+    <row r="117" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E117" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="117" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E117" s="7"/>
-    </row>
     <row r="118" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E118" t="s">
+      <c r="E118" s="7"/>
+    </row>
+    <row r="119" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E119" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="119" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E119" s="7"/>
-    </row>
     <row r="120" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E120" t="s">
+      <c r="E120" s="7"/>
+    </row>
+    <row r="121" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E121" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="121" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E121" s="6"/>
-    </row>
-    <row r="123" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D123" s="3" t="s">
+    <row r="122" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E122" s="6"/>
+    </row>
+    <row r="124" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D124" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E123" s="3"/>
-      <c r="F123" s="3"/>
-      <c r="G123" s="3"/>
-    </row>
-    <row r="124" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E124" t="s">
+      <c r="E124" s="3"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+    </row>
+    <row r="125" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E125" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E125" s="7"/>
-    </row>
     <row r="126" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E126" t="s">
+      <c r="E126" s="7"/>
+    </row>
+    <row r="127" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E127" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="127" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E127" s="7"/>
-    </row>
     <row r="128" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E128" t="s">
+      <c r="E128" s="7"/>
+    </row>
+    <row r="129" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E129" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E129" s="6"/>
-    </row>
-    <row r="131" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C131" s="2" t="s">
+    <row r="130" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E130" s="6"/>
+    </row>
+    <row r="132" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C132" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
-      <c r="G131" s="2"/>
-    </row>
-    <row r="132" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="133" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D133" s="3" t="s">
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+    </row>
+    <row r="133" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="134" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D134" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E133" s="3"/>
-      <c r="F133" s="3"/>
-      <c r="G133" s="3"/>
-    </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E134" t="s">
+      <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+    </row>
+    <row r="135" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E135" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="135" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E135" s="7"/>
-    </row>
     <row r="136" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E136" t="s">
+      <c r="E136" s="7"/>
+    </row>
+    <row r="137" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E137" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E137" s="7"/>
-    </row>
-    <row r="139" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D139" s="3" t="s">
+    <row r="138" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E138" s="7"/>
+    </row>
+    <row r="140" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D140" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E139" s="3"/>
-      <c r="F139" s="3"/>
-      <c r="G139" s="3"/>
-    </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E140" t="s">
+      <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
+    </row>
+    <row r="141" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E141" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="141" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E141" s="7"/>
-    </row>
     <row r="142" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E142" t="s">
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E143" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E143" s="7"/>
-    </row>
     <row r="144" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E144" t="s">
+      <c r="E144" s="7"/>
+    </row>
+    <row r="145" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E145" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E145" s="7"/>
-    </row>
     <row r="146" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E146" t="s">
+      <c r="E146" s="7"/>
+    </row>
+    <row r="147" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E147" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="147" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E147" s="7"/>
-    </row>
-    <row r="149" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D149" s="3" t="s">
+    <row r="148" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E148" s="7"/>
+    </row>
+    <row r="150" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D150" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E149" s="3"/>
-      <c r="F149" s="3"/>
-      <c r="G149" s="3"/>
-    </row>
-    <row r="150" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E150" t="s">
+      <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3"/>
+    </row>
+    <row r="151" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E151" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="151" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E151" s="7"/>
-    </row>
     <row r="152" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E152" t="s">
+      <c r="E152" s="7"/>
+    </row>
+    <row r="153" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E153" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="153" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E153" s="7"/>
-    </row>
-    <row r="155" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C155" s="2" t="s">
+    <row r="154" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E154" s="7"/>
+    </row>
+    <row r="156" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C156" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D155" s="2"/>
-      <c r="E155" s="2"/>
-      <c r="F155" s="2"/>
-      <c r="G155" s="2"/>
-    </row>
-    <row r="156" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="157" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D157" s="3" t="s">
+      <c r="D156" s="2"/>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+    </row>
+    <row r="157" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="158" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D158" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E157" s="3"/>
-      <c r="F157" s="3"/>
-      <c r="G157" s="3"/>
-    </row>
-    <row r="158" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E158" t="s">
+      <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
+    </row>
+    <row r="159" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E159" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="159" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E159" s="7"/>
-    </row>
     <row r="160" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E160" t="s">
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E161" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="161" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E161" s="7"/>
-    </row>
     <row r="162" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E162" t="s">
+      <c r="E162" s="7"/>
+    </row>
+    <row r="163" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E163" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="163" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E163" s="7"/>
-    </row>
     <row r="164" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E164" t="s">
+      <c r="E164" s="7"/>
+    </row>
+    <row r="165" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E165" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="165" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E165" s="7"/>
-    </row>
     <row r="166" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E166" t="s">
+      <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E167" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="167" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E167" s="6"/>
-    </row>
-    <row r="169" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D169" s="3" t="s">
+    <row r="168" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E168" s="6"/>
+    </row>
+    <row r="170" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D170" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E169" s="3"/>
-      <c r="F169" s="3"/>
-      <c r="G169" s="3"/>
-    </row>
-    <row r="170" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E170" t="s">
+      <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3"/>
+    </row>
+    <row r="171" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E171" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="171" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E171" s="7"/>
-    </row>
     <row r="172" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E172" t="s">
+      <c r="E172" s="7"/>
+    </row>
+    <row r="173" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E173" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="173" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E173" s="6"/>
-    </row>
-    <row r="175" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D175" s="3" t="s">
+    <row r="174" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E174" s="6"/>
+    </row>
+    <row r="176" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D176" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E175" s="3"/>
-      <c r="F175" s="3"/>
-      <c r="G175" s="3"/>
-    </row>
-    <row r="176" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E176" t="s">
+      <c r="E176" s="3"/>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3"/>
+    </row>
+    <row r="177" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E177" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="177" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E177" s="7"/>
-    </row>
     <row r="178" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E178" t="s">
+      <c r="E178" s="7"/>
+    </row>
+    <row r="179" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E179" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="179" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E179" s="6"/>
-    </row>
     <row r="180" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E180" t="s">
+      <c r="E180" s="6"/>
+    </row>
+    <row r="181" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E181" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="181" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E181" s="7"/>
-    </row>
-    <row r="183" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C183" s="2" t="s">
+    <row r="182" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E182" s="7"/>
+    </row>
+    <row r="184" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C184" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D183" s="2"/>
-      <c r="E183" s="2"/>
-      <c r="F183" s="2"/>
-      <c r="G183" s="2"/>
-    </row>
-    <row r="184" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="185" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D185" s="3" t="s">
+      <c r="D184" s="2"/>
+      <c r="E184" s="2"/>
+      <c r="F184" s="2"/>
+      <c r="G184" s="2"/>
+    </row>
+    <row r="185" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="186" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D186" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E185" s="3"/>
-      <c r="F185" s="3"/>
-      <c r="G185" s="3"/>
-    </row>
-    <row r="186" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E186" t="s">
+      <c r="E186" s="3"/>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
+    </row>
+    <row r="187" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E187" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="187" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E187" s="7"/>
-    </row>
     <row r="188" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E188" t="s">
+      <c r="E188" s="7"/>
+    </row>
+    <row r="189" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E189" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="189" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E189" s="7"/>
-    </row>
-    <row r="191" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D191" s="3" t="s">
+    <row r="190" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E190" s="7"/>
+    </row>
+    <row r="192" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D192" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E191" s="3"/>
-      <c r="F191" s="3"/>
-      <c r="G191" s="3"/>
-    </row>
-    <row r="193" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E193" t="s">
-        <v>100</v>
-      </c>
-      <c r="F193" t="s">
-        <v>101</v>
-      </c>
+      <c r="E192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
     </row>
     <row r="194" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E194" t="s">
-        <v>102</v>
-      </c>
-      <c r="F194" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="F194" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="195" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E195" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F195" s="7"/>
     </row>
     <row r="196" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E196" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F196" s="7"/>
     </row>
     <row r="197" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E197" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F197" s="7"/>
     </row>
     <row r="198" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E198" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F198" s="7"/>
     </row>
     <row r="199" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E199" t="s">
+        <v>106</v>
+      </c>
+      <c r="F199" s="7"/>
+    </row>
+    <row r="200" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E200" t="s">
         <v>107</v>
       </c>
-      <c r="F199" s="7"/>
-    </row>
-    <row r="201" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C201" s="2" t="s">
+      <c r="F200" s="7"/>
+    </row>
+    <row r="202" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C202" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D201" s="2"/>
-      <c r="E201" s="2"/>
-      <c r="F201" s="2"/>
-      <c r="G201" s="2"/>
-    </row>
-    <row r="202" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="203" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D203" s="3" t="s">
+      <c r="D202" s="2"/>
+      <c r="E202" s="2"/>
+      <c r="F202" s="2"/>
+      <c r="G202" s="2"/>
+    </row>
+    <row r="203" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="204" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D204" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E203" s="3"/>
-      <c r="F203" s="3"/>
-      <c r="G203" s="3"/>
-    </row>
-    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E204" t="s">
+      <c r="E204" s="3"/>
+      <c r="F204" s="3"/>
+      <c r="G204" s="3"/>
+    </row>
+    <row r="205" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E205" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="205" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E205" s="7"/>
-    </row>
     <row r="206" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E206" t="s">
+      <c r="E206" s="7"/>
+    </row>
+    <row r="207" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E207" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="207" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E207" s="7"/>
-    </row>
     <row r="208" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E208" t="s">
+      <c r="E208" s="7"/>
+    </row>
+    <row r="209" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E209" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="209" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E209" s="7"/>
-    </row>
     <row r="210" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E210" t="s">
+      <c r="E210" s="7"/>
+    </row>
+    <row r="211" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E211" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="211" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E211" s="7"/>
-    </row>
-    <row r="213" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D213" s="3" t="s">
+    <row r="212" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E212" s="7"/>
+    </row>
+    <row r="214" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D214" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E213" s="3"/>
-      <c r="F213" s="3"/>
-      <c r="G213" s="3"/>
-    </row>
-    <row r="214" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E214" t="s">
+      <c r="E214" s="3"/>
+      <c r="F214" s="3"/>
+      <c r="G214" s="3"/>
+    </row>
+    <row r="215" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E215" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="215" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E215" s="7"/>
-    </row>
     <row r="216" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E216" t="s">
+      <c r="E216" s="7"/>
+    </row>
+    <row r="217" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E217" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="217" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E217" s="7"/>
-    </row>
     <row r="218" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E218" t="s">
+      <c r="E218" s="7"/>
+    </row>
+    <row r="219" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E219" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="219" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E219" s="6"/>
-    </row>
-    <row r="221" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C221" s="2" t="s">
+    <row r="220" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E220" s="6"/>
+    </row>
+    <row r="222" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C222" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D221" s="2"/>
-      <c r="E221" s="2"/>
-      <c r="F221" s="2"/>
-      <c r="G221" s="2"/>
-    </row>
-    <row r="222" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="223" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D223" s="3" t="s">
+      <c r="D222" s="2"/>
+      <c r="E222" s="2"/>
+      <c r="F222" s="2"/>
+      <c r="G222" s="2"/>
+    </row>
+    <row r="223" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="224" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D224" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E223" s="3"/>
-      <c r="F223" s="3"/>
-      <c r="G223" s="3"/>
-    </row>
-    <row r="224" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E224" t="s">
+      <c r="E224" s="3"/>
+      <c r="F224" s="3"/>
+      <c r="G224" s="3"/>
+    </row>
+    <row r="225" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E225" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="225" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E225" s="7"/>
-    </row>
     <row r="226" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E226" t="s">
+      <c r="E226" s="7"/>
+    </row>
+    <row r="227" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E227" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="227" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E227" s="7"/>
-    </row>
     <row r="228" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E228" t="s">
+      <c r="E228" s="7"/>
+    </row>
+    <row r="229" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E229" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="229" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E229" s="6"/>
-    </row>
-    <row r="231" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D231" s="3" t="s">
+    <row r="230" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E230" s="6"/>
+    </row>
+    <row r="232" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D232" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E231" s="3"/>
-      <c r="F231" s="3"/>
-      <c r="G231" s="3"/>
-    </row>
-    <row r="232" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E232" t="s">
+      <c r="E232" s="3"/>
+      <c r="F232" s="3"/>
+      <c r="G232" s="3"/>
+    </row>
+    <row r="233" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E233" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="233" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E233" s="7"/>
-    </row>
     <row r="234" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E234" t="s">
+      <c r="E234" s="7"/>
+    </row>
+    <row r="235" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E235" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="235" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E235" s="6"/>
-    </row>
     <row r="236" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E236" t="s">
+      <c r="E236" s="6"/>
+    </row>
+    <row r="237" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E237" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="237" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E237" s="7"/>
-    </row>
     <row r="238" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E238" t="s">
+      <c r="E238" s="7"/>
+    </row>
+    <row r="239" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E239" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="239" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E239" s="6"/>
-    </row>
     <row r="240" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E240" t="s">
+      <c r="E240" s="6"/>
+    </row>
+    <row r="241" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E241" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E241" s="7"/>
-    </row>
     <row r="242" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E242" t="s">
+      <c r="E242" s="7"/>
+    </row>
+    <row r="243" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E243" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E243" s="6"/>
-    </row>
     <row r="244" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E244" t="s">
+      <c r="E244" s="6"/>
+    </row>
+    <row r="245" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E245" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E245" s="7"/>
-    </row>
     <row r="246" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E246" t="s">
+      <c r="E246" s="7"/>
+    </row>
+    <row r="247" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E247" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E247" s="6"/>
-    </row>
     <row r="248" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E248" t="s">
+      <c r="E248" s="6"/>
+    </row>
+    <row r="249" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E249" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E249" s="7"/>
-    </row>
     <row r="250" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E250" t="s">
+      <c r="E250" s="7"/>
+    </row>
+    <row r="251" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E251" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E251" s="7"/>
-    </row>
     <row r="252" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E252" t="s">
+      <c r="E252" s="7"/>
+    </row>
+    <row r="253" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E253" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E253" s="7"/>
-    </row>
     <row r="254" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E254" t="s">
+      <c r="E254" s="7"/>
+    </row>
+    <row r="255" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E255" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E255" s="6"/>
-    </row>
     <row r="256" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E256" t="s">
+      <c r="E256" s="6"/>
+    </row>
+    <row r="257" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E257" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="257" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E257" s="7"/>
-    </row>
     <row r="258" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E258" t="s">
+      <c r="E258" s="7"/>
+    </row>
+    <row r="259" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E259" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="259" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E259" s="7"/>
-    </row>
-    <row r="261" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B261" s="1" t="s">
+    <row r="260" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E260" s="7"/>
+    </row>
+    <row r="262" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B262" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C261" s="1"/>
-      <c r="D261" s="1"/>
-      <c r="E261" s="1"/>
-      <c r="F261" s="1"/>
-      <c r="G261" s="1"/>
-    </row>
-    <row r="262" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B262" s="9"/>
-      <c r="C262" s="9"/>
-      <c r="D262" s="9"/>
-      <c r="E262" s="9"/>
-      <c r="F262" s="9"/>
-      <c r="G262" s="9"/>
-    </row>
-    <row r="263" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C263" s="2" t="s">
+      <c r="C262" s="1"/>
+      <c r="D262" s="1"/>
+      <c r="E262" s="1"/>
+      <c r="F262" s="1"/>
+      <c r="G262" s="1"/>
+    </row>
+    <row r="263" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B263" s="9"/>
+      <c r="C263" s="9"/>
+      <c r="D263" s="9"/>
+      <c r="E263" s="9"/>
+      <c r="F263" s="9"/>
+      <c r="G263" s="9"/>
+    </row>
+    <row r="264" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C264" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D263" s="2"/>
-      <c r="E263" s="2"/>
-      <c r="F263" s="2"/>
-      <c r="G263" s="2"/>
-    </row>
-    <row r="264" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="265" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D265" s="3" t="s">
+      <c r="D264" s="2"/>
+      <c r="E264" s="2"/>
+      <c r="F264" s="2"/>
+      <c r="G264" s="2"/>
+    </row>
+    <row r="265" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="266" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D266" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E265" s="3"/>
-      <c r="F265" s="3"/>
-      <c r="G265" s="3"/>
-    </row>
-    <row r="266" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D266" s="10"/>
-      <c r="E266" t="s">
+      <c r="E266" s="3"/>
+      <c r="F266" s="3"/>
+      <c r="G266" s="3"/>
+    </row>
+    <row r="267" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D267" s="10"/>
+      <c r="E267" t="s">
         <v>214</v>
       </c>
-      <c r="F266" s="10"/>
-      <c r="G266" s="10"/>
-    </row>
-    <row r="267" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E267" s="7"/>
+      <c r="F267" s="10"/>
+      <c r="G267" s="10"/>
     </row>
     <row r="268" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E268" t="s">
-        <v>8</v>
-      </c>
-      <c r="F268" t="s">
-        <v>215</v>
-      </c>
+      <c r="E268" s="7"/>
     </row>
     <row r="269" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E269" t="s">
-        <v>128</v>
-      </c>
-      <c r="F269" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F269" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="270" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E270" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F270" s="7"/>
     </row>
     <row r="271" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E271" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F271" s="7"/>
     </row>
     <row r="272" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E272" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F272" s="7"/>
     </row>
     <row r="273" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E273" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F273" s="7"/>
     </row>
     <row r="274" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E274" t="s">
+        <v>132</v>
+      </c>
+      <c r="F274" s="7"/>
+    </row>
+    <row r="275" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E275" t="s">
         <v>133</v>
       </c>
-      <c r="F274" s="7"/>
-    </row>
-    <row r="277" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D277" s="3" t="s">
+      <c r="F275" s="7"/>
+    </row>
+    <row r="278" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D278" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E277" s="3"/>
-      <c r="F277" s="3"/>
-      <c r="G277" s="3"/>
-    </row>
-    <row r="278" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E278" t="s">
+      <c r="E278" s="3"/>
+      <c r="F278" s="3"/>
+      <c r="G278" s="3"/>
+    </row>
+    <row r="279" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E279" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="279" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E279" s="7"/>
-    </row>
     <row r="280" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E280" t="s">
+      <c r="E280" s="7"/>
+    </row>
+    <row r="281" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E281" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="281" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E281" s="6"/>
-    </row>
     <row r="282" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E282" t="s">
+      <c r="E282" s="6"/>
+    </row>
+    <row r="283" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E283" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="284" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E284" t="s">
-        <v>134</v>
-      </c>
-      <c r="F284" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="285" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E285" t="s">
-        <v>135</v>
-      </c>
-      <c r="F285" s="7"/>
+        <v>134</v>
+      </c>
+      <c r="F285" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="286" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E286" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F286" s="7"/>
     </row>
     <row r="287" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E287" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F287" s="7"/>
     </row>
     <row r="288" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E288" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F288" s="7"/>
     </row>
     <row r="289" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E289" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F289" s="7"/>
     </row>
     <row r="290" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E290" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F290" s="7"/>
     </row>
     <row r="291" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E291" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F291" s="7"/>
     </row>
     <row r="292" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E292" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F292" s="7"/>
     </row>
     <row r="293" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E293" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F293" s="7"/>
     </row>
     <row r="294" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E294" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F294" s="7"/>
     </row>
     <row r="295" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E295" t="s">
+        <v>144</v>
+      </c>
+      <c r="F295" s="7"/>
+    </row>
+    <row r="296" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E296" t="s">
         <v>145</v>
       </c>
-      <c r="F295" s="7"/>
-    </row>
-    <row r="298" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C298" s="2" t="s">
+      <c r="F296" s="7"/>
+    </row>
+    <row r="299" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C299" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D298" s="2"/>
-      <c r="E298" s="2"/>
-      <c r="F298" s="2"/>
-      <c r="G298" s="2"/>
-    </row>
-    <row r="299" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="300" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D300" s="3" t="s">
+      <c r="D299" s="2"/>
+      <c r="E299" s="2"/>
+      <c r="F299" s="2"/>
+      <c r="G299" s="2"/>
+    </row>
+    <row r="300" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="301" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D301" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E300" s="3"/>
-      <c r="F300" s="3"/>
-      <c r="G300" s="3"/>
-    </row>
-    <row r="301" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E301" t="s">
+      <c r="E301" s="3"/>
+      <c r="F301" s="3"/>
+      <c r="G301" s="3"/>
+    </row>
+    <row r="302" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E302" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="302" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E302" s="7"/>
-    </row>
     <row r="303" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E303" t="s">
+      <c r="E303" s="7"/>
+    </row>
+    <row r="304" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E304" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="304" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E304" s="7"/>
-    </row>
     <row r="305" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E305" t="s">
+      <c r="E305" s="7"/>
+    </row>
+    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E306" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="306" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E306" s="7"/>
-    </row>
-    <row r="308" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D308" s="3" t="s">
+    <row r="307" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E307" s="7"/>
+    </row>
+    <row r="309" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D309" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E308" s="3"/>
-      <c r="F308" s="3"/>
-      <c r="G308" s="3"/>
-    </row>
-    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E309" t="s">
+      <c r="E309" s="3"/>
+      <c r="F309" s="3"/>
+      <c r="G309" s="3"/>
+    </row>
+    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E310" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E310" s="7"/>
-    </row>
     <row r="311" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E311" t="s">
+      <c r="E311" s="7"/>
+    </row>
+    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E312" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E312" s="7"/>
-    </row>
     <row r="313" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E313" t="s">
+      <c r="E313" s="7"/>
+    </row>
+    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E314" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E314" s="7"/>
-    </row>
     <row r="315" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E315" t="s">
+      <c r="E315" s="7"/>
+    </row>
+    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E316" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E316" s="7"/>
-    </row>
-    <row r="318" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C318" s="2" t="s">
+    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E317" s="7"/>
+    </row>
+    <row r="319" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C319" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D318" s="2"/>
-      <c r="E318" s="2"/>
-      <c r="F318" s="2"/>
-      <c r="G318" s="2"/>
-    </row>
-    <row r="319" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="320" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D320" s="3" t="s">
+      <c r="D319" s="2"/>
+      <c r="E319" s="2"/>
+      <c r="F319" s="2"/>
+      <c r="G319" s="2"/>
+    </row>
+    <row r="320" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="321" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D321" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E320" s="3"/>
-      <c r="F320" s="3"/>
-      <c r="G320" s="3"/>
-    </row>
-    <row r="321" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E321" t="s">
+      <c r="E321" s="3"/>
+      <c r="F321" s="3"/>
+      <c r="G321" s="3"/>
+    </row>
+    <row r="322" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E322" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="322" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E322" s="7"/>
-    </row>
-    <row r="323" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E323" t="s">
+    <row r="323" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E323" s="7"/>
+    </row>
+    <row r="324" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E324" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="324" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E324" s="7"/>
-    </row>
-    <row r="325" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E325" t="s">
+    <row r="325" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E325" s="7"/>
+    </row>
+    <row r="326" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E326" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="326" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E326" s="7"/>
-    </row>
-    <row r="327" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E327" t="s">
+    <row r="327" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E327" s="7"/>
+    </row>
+    <row r="328" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E328" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="328" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E328" s="7"/>
-    </row>
-    <row r="329" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E329" t="s">
+    <row r="329" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E329" s="7"/>
+    </row>
+    <row r="330" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E330" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="330" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E330" s="7"/>
-    </row>
-    <row r="331" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E331" t="s">
+    <row r="331" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E331" s="7"/>
+    </row>
+    <row r="332" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E332" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="332" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E332" s="7"/>
-    </row>
-    <row r="333" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E333" t="s">
+    <row r="333" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E333" s="7"/>
+    </row>
+    <row r="334" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E334" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="334" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E334" s="7"/>
-    </row>
-    <row r="335" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E335" t="s">
+    <row r="335" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E335" s="7"/>
+    </row>
+    <row r="336" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E336" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="336" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E336" s="7"/>
-    </row>
-    <row r="337" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E337" t="s">
+    <row r="337" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E337" s="7"/>
+    </row>
+    <row r="338" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E338" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="338" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E338" s="7"/>
-    </row>
-    <row r="339" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E339" t="s">
+    <row r="339" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E339" s="7"/>
+    </row>
+    <row r="340" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E340" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="340" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E340" s="7"/>
-    </row>
-    <row r="341" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E341" t="s">
+    <row r="341" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E341" s="7"/>
+    </row>
+    <row r="342" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E342" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="342" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E342" s="7"/>
-    </row>
-    <row r="343" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E343" t="s">
+    <row r="343" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E343" s="7"/>
+    </row>
+    <row r="344" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E344" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="344" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E344" s="7"/>
-    </row>
-    <row r="346" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D346" s="3" t="s">
+    <row r="345" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E345" s="7"/>
+    </row>
+    <row r="347" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D347" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E346" s="3"/>
-      <c r="F346" s="3"/>
-      <c r="G346" s="3"/>
-    </row>
-    <row r="348" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E348" t="s">
+      <c r="E347" s="3"/>
+      <c r="F347" s="3"/>
+      <c r="G347" s="3"/>
+    </row>
+    <row r="349" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E349" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="349" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E349" s="7"/>
-    </row>
-    <row r="350" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E350" t="s">
+    <row r="350" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E350" s="7"/>
+    </row>
+    <row r="351" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E351" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="351" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E351" s="7"/>
-    </row>
-    <row r="352" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B352" s="1" t="s">
+    <row r="352" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E352" s="7"/>
+    </row>
+    <row r="353" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B353" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C352" s="1"/>
-      <c r="D352" s="1"/>
-      <c r="E352" s="1"/>
-      <c r="F352" s="1"/>
-      <c r="G352" s="1"/>
-    </row>
-    <row r="353" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B353" s="9"/>
-      <c r="C353" s="9"/>
-      <c r="D353" s="9"/>
-      <c r="E353" s="9"/>
-      <c r="F353" s="9"/>
-      <c r="G353" s="9"/>
-    </row>
-    <row r="354" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C354" s="2" t="s">
+      <c r="C353" s="1"/>
+      <c r="D353" s="1"/>
+      <c r="E353" s="1"/>
+      <c r="F353" s="1"/>
+      <c r="G353" s="1"/>
+    </row>
+    <row r="354" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B354" s="9"/>
+      <c r="C354" s="9"/>
+      <c r="D354" s="9"/>
+      <c r="E354" s="9"/>
+      <c r="F354" s="9"/>
+      <c r="G354" s="9"/>
+    </row>
+    <row r="355" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C355" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D354" s="2"/>
-      <c r="E354" s="2"/>
-      <c r="F354" s="2"/>
-      <c r="G354" s="2"/>
-    </row>
-    <row r="355" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="356" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D356" s="3" t="s">
+      <c r="D355" s="2"/>
+      <c r="E355" s="2"/>
+      <c r="F355" s="2"/>
+      <c r="G355" s="2"/>
+    </row>
+    <row r="356" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="357" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D357" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E356" s="3"/>
-      <c r="F356" s="3"/>
-      <c r="G356" s="3"/>
-    </row>
-    <row r="357" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E357" t="s">
-        <v>28</v>
-      </c>
+      <c r="E357" s="3"/>
+      <c r="F357" s="3"/>
+      <c r="G357" s="3"/>
     </row>
     <row r="358" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E358" t="s">
-        <v>8</v>
-      </c>
-      <c r="F358" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="359" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E359" t="s">
-        <v>147</v>
-      </c>
-      <c r="F359" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F359" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="360" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E360" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F360" s="7"/>
     </row>
     <row r="361" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E361" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F361" s="7"/>
     </row>
     <row r="362" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E362" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F362" s="7"/>
     </row>
     <row r="363" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E363" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F363" s="7"/>
     </row>
     <row r="364" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E364" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F364" s="7"/>
     </row>
     <row r="365" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E365" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F365" s="7"/>
     </row>
     <row r="366" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E366" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F366" s="7"/>
     </row>
     <row r="367" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E367" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F367" s="7"/>
     </row>
     <row r="368" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E368" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F368" s="7"/>
     </row>
     <row r="369" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E369" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F369" s="7"/>
     </row>
     <row r="370" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E370" t="s">
+        <v>157</v>
+      </c>
+      <c r="F370" s="7"/>
+    </row>
+    <row r="371" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E371" t="s">
         <v>158</v>
       </c>
-      <c r="F370" s="7"/>
-    </row>
-    <row r="372" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B372" t="s">
+      <c r="F371" s="7"/>
+    </row>
+    <row r="373" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B373" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="373" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D373" s="3" t="s">
+    <row r="374" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D374" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E373" s="3"/>
-      <c r="F373" s="3"/>
-      <c r="G373" s="3"/>
-    </row>
-    <row r="374" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E374" t="s">
-        <v>192</v>
-      </c>
+      <c r="E374" s="3"/>
+      <c r="F374" s="3"/>
+      <c r="G374" s="3"/>
     </row>
     <row r="375" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E375" t="s">
-        <v>100</v>
-      </c>
-      <c r="F375" t="s">
-        <v>9</v>
+        <v>192</v>
       </c>
     </row>
     <row r="376" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E376" t="s">
-        <v>160</v>
-      </c>
-      <c r="F376" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="F376" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="377" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E377" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F377" s="7"/>
     </row>
     <row r="378" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E378" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F378" s="7"/>
     </row>
     <row r="379" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E379" t="s">
+        <v>162</v>
+      </c>
+      <c r="F379" s="7"/>
+    </row>
+    <row r="380" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E380" t="s">
         <v>163</v>
       </c>
-      <c r="F379" s="7"/>
-    </row>
-    <row r="382" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C382" s="2" t="s">
+      <c r="F380" s="7"/>
+    </row>
+    <row r="383" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C383" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D382" s="2"/>
-      <c r="E382" s="2"/>
-      <c r="F382" s="2"/>
-      <c r="G382" s="2"/>
-    </row>
-    <row r="383" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="384" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D384" s="3" t="s">
+      <c r="D383" s="2"/>
+      <c r="E383" s="2"/>
+      <c r="F383" s="2"/>
+      <c r="G383" s="2"/>
+    </row>
+    <row r="384" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="385" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D385" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E384" s="3"/>
-      <c r="F384" s="3"/>
-      <c r="G384" s="3"/>
-    </row>
-    <row r="385" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E385" t="s">
+      <c r="E385" s="3"/>
+      <c r="F385" s="3"/>
+      <c r="G385" s="3"/>
+    </row>
+    <row r="386" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E386" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="386" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E386" t="s">
+    <row r="387" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E387" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="387" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E387" s="8" t="s">
+    <row r="388" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E388" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F387" s="7"/>
-    </row>
-    <row r="388" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E388" s="8" t="s">
+      <c r="F388" s="7"/>
+    </row>
+    <row r="389" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E389" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F388" s="7"/>
-    </row>
-    <row r="389" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E389" t="s">
+      <c r="F389" s="7"/>
+    </row>
+    <row r="390" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E390" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="390" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E390" s="8" t="s">
+    <row r="391" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E391" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F390" s="7"/>
-    </row>
-    <row r="391" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E391" s="8" t="s">
+      <c r="F391" s="7"/>
+    </row>
+    <row r="392" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E392" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="F391" s="7"/>
-    </row>
-    <row r="392" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E392" s="8" t="s">
+      <c r="F392" s="7"/>
+    </row>
+    <row r="393" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E393" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="F392" s="7"/>
-    </row>
-    <row r="393" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E393" s="8" t="s">
+      <c r="F393" s="7"/>
+    </row>
+    <row r="394" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E394" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="F393" s="7"/>
-    </row>
-    <row r="395" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E395" t="s">
+      <c r="F394" s="7"/>
+    </row>
+    <row r="396" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E396" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="396" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E396" s="7"/>
-    </row>
-    <row r="397" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E397" t="s">
+    <row r="397" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E397" s="7"/>
+    </row>
+    <row r="398" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E398" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="398" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E398" s="7"/>
-    </row>
-    <row r="399" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E399" t="s">
+    <row r="399" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E399" s="7"/>
+    </row>
+    <row r="400" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E400" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="400" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E400" s="7"/>
+    <row r="401" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E401" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23 E65 E57" xr:uid="{3C594C12-590A-7343-A03C-F6F925CF2C6D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23 E66 E58" xr:uid="{3C594C12-590A-7343-A03C-F6F925CF2C6D}">
       <formula1>YesNoPartial</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39 E84 E86 E107 E109 E111 E113 E117 E119 E125 E127 E135 E137:E138 E141 E143 E145 E147 E151 E153 E159 E161 E163 E165 E171 E177 E181 E187 E189 F194:F199 E205 E207 E209 E211 E215 E217 E225 E227 E251 E249 E257 E259 E253 E245 E241 E237 E233 E267 E279 E302 E304 E306 E310 E312 E314 E316 E322 E324 E328 E330 E332 E336 E340 E344 E349 F376:F379 F387:F388 F390:F393 E396 E398 E400 E45 E48" xr:uid="{4BED4D73-49DB-8D4A-8D1E-63B573D30EBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39 E85 E87 E108 E110 E112 E114 E118 E120 E126 E128 E136 E138:E139 E142 E144 E146 E148 E152 E154 E160 E162 E164 E166 E172 E178 E182 E188 E190 F195:F200 E206 E208 E210 E212 E216 E218 E226 E228 E252 E250 E258 E260 E254 E246 E242 E238 E234 E268 E280 E303 E305 E307 E311 E313 E315 E317 E323 E325 E329 E331 E333 E337 E341 E345 E350 F377:F380 F388:F389 F391:F394 E397 E399 E401 E45 E48" xr:uid="{4BED4D73-49DB-8D4A-8D1E-63B573D30EBF}">
       <formula1>YesNo</formula1>
     </dataValidation>
   </dataValidations>
@@ -5621,10 +5643,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:F54"/>
+  <dimension ref="B2:F81"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5632,7 +5654,7 @@
     <col min="1" max="1" width="7.1640625" customWidth="1"/>
     <col min="2" max="4" width="4.83203125" customWidth="1"/>
     <col min="5" max="5" width="61.1640625" customWidth="1"/>
-    <col min="6" max="6" width="41" customWidth="1"/>
+    <col min="6" max="6" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -5647,7 +5669,7 @@
     <row r="3" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="21" t="s">
-        <v>391</v>
+        <v>427</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
@@ -5682,7 +5704,7 @@
     <row r="10" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -5699,19 +5721,19 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E15" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.2">
@@ -5721,12 +5743,12 @@
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E21" s="23" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.2">
@@ -5736,12 +5758,12 @@
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E25" s="23" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.2">
@@ -5751,12 +5773,12 @@
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E29" s="23" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.2">
@@ -5764,83 +5786,150 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E33" s="23" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E35" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E36" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E37" s="23" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E39" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E40" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E41" s="23" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E43" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E44" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E45" s="23" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E50" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E51" s="23" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E54" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="23" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E58" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E59" s="23" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E62" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E63" s="23" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="4:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="3" t="s">
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="3:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
         <v>407</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E52" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E54" s="23" t="s">
-        <v>399</v>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E81" s="23" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -5848,7 +5937,7 @@
     <mergeCell ref="C4:F7"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14 E20 E24 E28 E32 E36 E40 E44 E53" xr:uid="{B2F94D8F-9865-1B44-97D4-DFF708939FA2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14 E20 E24 E28 E32 E36 E40 E44 E80 E50 E54 E58 E62" xr:uid="{B2F94D8F-9865-1B44-97D4-DFF708939FA2}">
       <formula1>YesNo</formula1>
     </dataValidation>
   </dataValidations>
@@ -5914,22 +6003,22 @@
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added Windows Hello check
</commit_message>
<xml_diff>
--- a/assets/AzureADAssessment-Interview.xlsx
+++ b/assets/AzureADAssessment-Interview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Documents/GitHub/AzureADAssessment/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C905AED3-369A-F24D-9CBB-2C4620D66500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D94496D-3BD9-364E-967E-3B895893F885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Guided Walkthrough" sheetId="3" r:id="rId1"/>
@@ -31,59 +31,59 @@
     <definedName name="AADC_Is_the_Azure_AD_Connect_version_more_than_6_months_behind_the_latest_release">'Post-Interview Assessment'!$E$28</definedName>
     <definedName name="AADC_Is_there_a_consistent_volume_trend_of_add_deletes_over_1__and_or_updates_is_over_10">'Post-Interview Assessment'!$E$62</definedName>
     <definedName name="AADC_Is_there_a_mismatch_between_the_production_and_staging_configuration">'Post-Interview Assessment'!$E$24</definedName>
-    <definedName name="AccMgmt_Are_all_your_office_clients_in_versions_that_support_modern_authentication">'Interview Questions'!$E$192</definedName>
+    <definedName name="AccMgmt_Are_all_your_office_clients_in_versions_that_support_modern_authentication">'Interview Questions'!$E$190</definedName>
     <definedName name="AccMgmt_Are_strong_credentials_used_for_SSPR">'Interview Questions'!#REF!</definedName>
     <definedName name="AccMgmt_Are_strong_credentials_used_in_conditional_access_policies">'Interview Questions'!$E$108</definedName>
-    <definedName name="AccMgmt_Are_there_applications_that_can_be_candidates_to_use_attribute_based_access_control">'Interview Questions'!$E$168</definedName>
+    <definedName name="AccMgmt_Are_there_applications_that_can_be_candidates_to_use_attribute_based_access_control">'Interview Questions'!$E$166</definedName>
     <definedName name="AccMgmt_Are_there_many_apps_using_passwords_for_client_secrets">'Post-Interview Assessment'!$E$80</definedName>
-    <definedName name="AccMgmt_Are_you_Archiving_AD_FS_audits">'Interview Questions'!$E$236</definedName>
-    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_security_incident_response">'Interview Questions'!$E$244</definedName>
-    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_support_and_troubleshooting_access_issues">'Interview Questions'!$E$246</definedName>
+    <definedName name="AccMgmt_Are_you_Archiving_AD_FS_audits">'Interview Questions'!$E$234</definedName>
+    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_security_incident_response">'Interview Questions'!$E$242</definedName>
+    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_support_and_troubleshooting_access_issues">'Interview Questions'!$E$244</definedName>
     <definedName name="AccMgmt_Ban_Weak_Passwords">'Interview Questions'!$F$97</definedName>
     <definedName name="AccMgmt_Detection_of_Leaked_Passwords">'Interview Questions'!$F$99</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$228</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$232</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Sign_in_Activity_Logs">'Interview Questions'!$E$224</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Office_365_activity_logs">'Interview Questions'!$E$240</definedName>
-    <definedName name="AccMgmt_Do_you_enable_SSO_for_capable_apps_or_are_the_apps_that_use_local_accounts">'Interview Questions'!$E$150</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$226</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$230</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Sign_in_Activity_Logs">'Interview Questions'!$E$222</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Office_365_activity_logs">'Interview Questions'!$E$238</definedName>
+    <definedName name="AccMgmt_Do_you_enable_SSO_for_capable_apps_or_are_the_apps_that_use_local_accounts">'Interview Questions'!$E$148</definedName>
     <definedName name="AccMgmt_Do_you_have_a_self_service_password_reset_solution">'Interview Questions'!$E$85</definedName>
-    <definedName name="AccMgmt_Do_you_have_a_SIEM_system">'Interview Questions'!$E$220</definedName>
-    <definedName name="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today">'Interview Questions'!$E$164</definedName>
-    <definedName name="AccMgmt_Do_you_have_applications_that_support_SAML_OpenID_connect_or_OAuth">'Interview Questions'!$E$146</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_SIEM_system">'Interview Questions'!$E$218</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today">'Interview Questions'!$E$162</definedName>
+    <definedName name="AccMgmt_Do_you_have_applications_that_support_SAML_OpenID_connect_or_OAuth">'Interview Questions'!$E$144</definedName>
     <definedName name="AccMgmt_Do_you_have_desktop_management_policies">'Interview Questions'!$E$130</definedName>
-    <definedName name="AccMgmt_Do_you_have_initiative_to_migrate_SSO_configuration_from_AD_FS_to_Azure_AD">'Interview Questions'!$E$158</definedName>
-    <definedName name="AccMgmt_Do_you_have_Intune_Application_Management_MAM_policies_defined">'Interview Questions'!$E$174</definedName>
+    <definedName name="AccMgmt_Do_you_have_initiative_to_migrate_SSO_configuration_from_AD_FS_to_Azure_AD">'Interview Questions'!$E$156</definedName>
+    <definedName name="AccMgmt_Do_you_have_Intune_Application_Management_MAM_policies_defined">'Interview Questions'!$E$172</definedName>
     <definedName name="AccMgmt_Do_you_have_mobile_management_policies_defined">'Interview Questions'!$E$128</definedName>
     <definedName name="AccMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$66</definedName>
     <definedName name="AccMgmt_Do_you_have_scripts_that_run_on_a_regular_basis">'Interview Questions'!#REF!</definedName>
-    <definedName name="AccMgmt_Do_you_have_service_accounts_or_applications_that_rely_on_legacy_authentication">'Interview Questions'!$E$198</definedName>
+    <definedName name="AccMgmt_Do_you_have_service_accounts_or_applications_that_rely_on_legacy_authentication">'Interview Questions'!$E$196</definedName>
     <definedName name="AccMgmt_Do_you_provision_strong_credentials_alongside_identity_provisioning_or_device_provisioning">'Interview Questions'!$E$106</definedName>
     <definedName name="AccMgmt_Do_you_provision_strong_credentials_to_all_users_with_privileged_roles">'Interview Questions'!$E$104</definedName>
     <definedName name="AccMgmt_Do_you_use_device_compliance_as_a_control_in_Conditional_Access">'Interview Questions'!$E$134</definedName>
-    <definedName name="AccMgmt_Do_you_use_them_in_CA_policies">'Interview Questions'!$E$176</definedName>
+    <definedName name="AccMgmt_Do_you_use_them_in_CA_policies">'Interview Questions'!$E$174</definedName>
     <definedName name="AccMgmt_Do_your_users_use_Windows_Hello_in_their_Windows_10_Desktops">'Interview Questions'!$E$138</definedName>
     <definedName name="AccMgmt_Enable_ADFS_Smart_Soft_Lockout">'Interview Questions'!$F$100</definedName>
     <definedName name="AccMgmt_Enable_passwordless_methods">'Interview Questions'!$F$96</definedName>
     <definedName name="AccMgmt_Enforce_MFA_registration">'Interview Questions'!$F$98</definedName>
-    <definedName name="AccMgmt_Have_you_deployed_Azure_Log_Analytics">'Interview Questions'!$E$212</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Azure_Log_Analytics">'Interview Questions'!$E$210</definedName>
     <definedName name="AccMgmt_Have_you_deployed_Hybrid_Azure_AD_joined_in_your_environment">'Interview Questions'!$E$132</definedName>
-    <definedName name="AccMgmt_Have_you_deployed_Windows_Hello_as_an_enterprise_wide_policy">'Interview Questions'!$E$140</definedName>
-    <definedName name="AccMgmt_Have_you_enabled_All_Office_365_Auditing">'Interview Questions'!$E$238</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Windows_Hello_as_an_enterprise_wide_policy">'Interview Questions'!#REF!</definedName>
+    <definedName name="AccMgmt_Have_you_enabled_All_Office_365_Auditing">'Interview Questions'!$E$236</definedName>
     <definedName name="AccMgmt_Have_you_enabled_Password_Hash_Sync">'Interview Questions'!$E$112</definedName>
-    <definedName name="AccMgmt_Have_you_explicitly_identified_regions_where_authentication_should_NOT_be_coming_from">'Interview Questions'!$E$204</definedName>
-    <definedName name="AccMgmt_Have_you_identified_the_regions_of_the_world_where_authentication_traffic_should_be_coming_from">'Interview Questions'!$E$202</definedName>
-    <definedName name="AccMgmt_If_so_do_you_have_configured_the_applications_to_support_SSO_using_those_protocols">'Interview Questions'!$E$148</definedName>
-    <definedName name="AccMgmt_If_so_does_your_operations_team_use_it_regularly_to_understand_Azure_AD_usage">'Interview Questions'!$E$214</definedName>
+    <definedName name="AccMgmt_Have_you_explicitly_identified_regions_where_authentication_should_NOT_be_coming_from">'Interview Questions'!$E$202</definedName>
+    <definedName name="AccMgmt_Have_you_identified_the_regions_of_the_world_where_authentication_traffic_should_be_coming_from">'Interview Questions'!$E$200</definedName>
+    <definedName name="AccMgmt_If_so_do_you_have_configured_the_applications_to_support_SSO_using_those_protocols">'Interview Questions'!$E$146</definedName>
+    <definedName name="AccMgmt_If_so_does_your_operations_team_use_it_regularly_to_understand_Azure_AD_usage">'Interview Questions'!$E$212</definedName>
     <definedName name="AccMgmt_If_yes__is_this_using_Azure_AD_s_self_service_password_reset_solution">'Interview Questions'!$E$87</definedName>
     <definedName name="AccMgmt_If_you_are_using_passwords_how_do_you_manage_the_them">'Interview Questions'!$E$122</definedName>
     <definedName name="AccMgmt_If_you_use_federated_authentication_do_you_use_windows_integrated_authentication_WIA_when_inside_the_corporate_network">'Interview Questions'!#REF!</definedName>
-    <definedName name="AccMgmt_Is_legacy_authentication_blocked_by_conditional_access">'Interview Questions'!$E$196</definedName>
-    <definedName name="AccMgmt_Is_legacy_authentication_disabled_at_the_mailbox_level">'Interview Questions'!$E$194</definedName>
+    <definedName name="AccMgmt_Is_legacy_authentication_blocked_by_conditional_access">'Interview Questions'!$E$194</definedName>
+    <definedName name="AccMgmt_Is_legacy_authentication_disabled_at_the_mailbox_level">'Interview Questions'!$E$192</definedName>
     <definedName name="AccMgmt_Is_the_password_reset_part_of_the_operational_procedures_to_remediate_a_user_incident">'Interview Questions'!$E$89</definedName>
     <definedName name="AccMgmt_Is_the_procedure_to_switch_to_PHS_practiced_enabled_to_the_IAM_Ops_team">'Interview Questions'!$E$114</definedName>
     <definedName name="AccMgmt_Password_policy_uses_complexity_based_rules">'Interview Questions'!$F$95</definedName>
-    <definedName name="AccMgmt_What_platforms_do_you_use_to_provide_SSO_to_the_applications">'Interview Questions'!$E$152</definedName>
-    <definedName name="AccMgmt_What_process_do_you_have_to_discover_applications_that_are_not_configured_using_the_SSO_enterprise_solution">'Interview Questions'!$E$154</definedName>
+    <definedName name="AccMgmt_What_platforms_do_you_use_to_provide_SSO_to_the_applications">'Interview Questions'!$E$150</definedName>
+    <definedName name="AccMgmt_What_process_do_you_have_to_discover_applications_that_are_not_configured_using_the_SSO_enterprise_solution">'Interview Questions'!$E$152</definedName>
     <definedName name="AD_AssessmentDate">'Interview Questions'!$E$14</definedName>
     <definedName name="AD_AssessorName">'Interview Questions'!$E$11</definedName>
     <definedName name="AD_OrgName">'Interview Questions'!$E$5</definedName>
@@ -91,26 +91,26 @@
     <definedName name="Do_you_enforce_a_policy_that_requires_all_applications_to_use_a_certificate_credential">'Interview Questions'!$E$120</definedName>
     <definedName name="EntMgmt_Do_you_use_Azure_AD_Outbound_provisioning_for_applications_in_your_environment_that_supports_Azure_AD_provisioning">'Interview Questions'!$E$58</definedName>
     <definedName name="EntMgmt_What_is_the_approach_to_provision_to_applications_today">'Interview Questions'!$E$55</definedName>
-    <definedName name="Gov_Access_Review_Guest_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$303</definedName>
-    <definedName name="Gov_Access_Review_Guest_Is_it_automated">'Interview Questions'!$E$291</definedName>
-    <definedName name="Gov_AccessReview_Privileged_If_so_are_they_automated">'Interview Questions'!$E$319</definedName>
-    <definedName name="Gov_All_Users_Is_it_automated">'Interview Questions'!$E$301</definedName>
-    <definedName name="Gov_Are_there_system_accounts_that_are_also_privileged">'Interview Questions'!$E$323</definedName>
-    <definedName name="Gov_Do_administrators_have_dedicated_accounts_used_to_perform_privileged_operations">'Interview Questions'!$E$311</definedName>
-    <definedName name="Gov_Do_administrators_have_standing_access_to_privileges_in_your_environment">'Interview Questions'!$E$309</definedName>
-    <definedName name="Gov_Do_you_assign_users_to_the_All_Users_group">'Interview Questions'!$E$299</definedName>
-    <definedName name="Gov_Do_you_have_a_guest_access_review_strategy_in_place">'Interview Questions'!$E$297</definedName>
-    <definedName name="Gov_Do_you_have_a_privileged_role_strategy_for_Azure_Resources">'Interview Questions'!$E$331</definedName>
-    <definedName name="Gov_Do_you_have_a_process_to_identify_the_least_privileged_role_to_different_users_in_your_organization">'Interview Questions'!$E$315</definedName>
-    <definedName name="Gov_Do_you_have_a_test_environment">'Interview Questions'!$E$266</definedName>
-    <definedName name="Gov_Do_you_have_access_reviews_in_place_for_privileged_accounts">'Interview Questions'!$E$317</definedName>
-    <definedName name="Gov_Do_you_have_an_access_review_strategy_in_place">'Interview Questions'!$E$289</definedName>
-    <definedName name="Gov_Do_you_have_emergency_accounts_also_known_as_break_glass_provisioned_in_your_Azure_AD_tenant">'Interview Questions'!$E$336</definedName>
-    <definedName name="Gov_Do_you_have_owners_in_your_organization_for_all_the_tasks_listed_below">'Interview Questions'!$E$254</definedName>
-    <definedName name="Gov_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$293</definedName>
-    <definedName name="Gov_If_not_what_is_the_strategy_to_clean_up_remove_access">'Interview Questions'!$E$321</definedName>
-    <definedName name="Gov_If_so_how_do_establish_ownership_of_those_accounts">'Interview Questions'!$E$325</definedName>
-    <definedName name="Gov_Is_there_any_global_admin_outside_the_IAM_team">'Interview Questions'!$E$327</definedName>
+    <definedName name="Gov_Access_Review_Guest_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$301</definedName>
+    <definedName name="Gov_Access_Review_Guest_Is_it_automated">'Interview Questions'!$E$289</definedName>
+    <definedName name="Gov_AccessReview_Privileged_If_so_are_they_automated">'Interview Questions'!$E$317</definedName>
+    <definedName name="Gov_All_Users_Is_it_automated">'Interview Questions'!$E$299</definedName>
+    <definedName name="Gov_Are_there_system_accounts_that_are_also_privileged">'Interview Questions'!$E$321</definedName>
+    <definedName name="Gov_Do_administrators_have_dedicated_accounts_used_to_perform_privileged_operations">'Interview Questions'!$E$309</definedName>
+    <definedName name="Gov_Do_administrators_have_standing_access_to_privileges_in_your_environment">'Interview Questions'!$E$307</definedName>
+    <definedName name="Gov_Do_you_assign_users_to_the_All_Users_group">'Interview Questions'!$E$297</definedName>
+    <definedName name="Gov_Do_you_have_a_guest_access_review_strategy_in_place">'Interview Questions'!$E$295</definedName>
+    <definedName name="Gov_Do_you_have_a_privileged_role_strategy_for_Azure_Resources">'Interview Questions'!$E$329</definedName>
+    <definedName name="Gov_Do_you_have_a_process_to_identify_the_least_privileged_role_to_different_users_in_your_organization">'Interview Questions'!$E$313</definedName>
+    <definedName name="Gov_Do_you_have_a_test_environment">'Interview Questions'!$E$264</definedName>
+    <definedName name="Gov_Do_you_have_access_reviews_in_place_for_privileged_accounts">'Interview Questions'!$E$315</definedName>
+    <definedName name="Gov_Do_you_have_an_access_review_strategy_in_place">'Interview Questions'!$E$287</definedName>
+    <definedName name="Gov_Do_you_have_emergency_accounts_also_known_as_break_glass_provisioned_in_your_Azure_AD_tenant">'Interview Questions'!$E$334</definedName>
+    <definedName name="Gov_Do_you_have_owners_in_your_organization_for_all_the_tasks_listed_below">'Interview Questions'!$E$252</definedName>
+    <definedName name="Gov_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$291</definedName>
+    <definedName name="Gov_If_not_what_is_the_strategy_to_clean_up_remove_access">'Interview Questions'!$E$319</definedName>
+    <definedName name="Gov_If_so_how_do_establish_ownership_of_those_accounts">'Interview Questions'!$E$323</definedName>
+    <definedName name="Gov_Is_there_any_global_admin_outside_the_IAM_team">'Interview Questions'!$E$325</definedName>
     <definedName name="IdMgmt_Do_you_have_a_disaster_recovery_production_instance_of_AAD_Connect_deployed_in_Staging_Mode">'Interview Questions'!$E$45</definedName>
     <definedName name="IdMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$23</definedName>
     <definedName name="IdMgmt_Do_you_synchronize_the_same_forest_where_users_log_in_to_their_Windows_devices">'Interview Questions'!$E$39</definedName>
@@ -123,19 +123,19 @@
     <definedName name="Lic_If_GBL_is_not_used__how_would_you_rate_your_current_approach_to_licensing">'Guided Walkthrough'!$G$116</definedName>
     <definedName name="Lic_If_yes__is_GBL_deployed_against_on_premises_groups_that_lack_lifecycle_management">'Guided Walkthrough'!$G$113</definedName>
     <definedName name="LookupLicenceMaturity">Lookups!$B$14:$B$17</definedName>
-    <definedName name="Ops_Are_there_compensating_controls_for_cases_where_the_answer_above_is_No">'Interview Questions'!$E$387</definedName>
-    <definedName name="Ops_Azure_AD_App_Proxy_debug_connector_group_deployed">'Interview Questions'!$F$365</definedName>
-    <definedName name="Ops_Debugging_tools_deployed_in_debug_app_proxy_connector">'Interview Questions'!$F$366</definedName>
-    <definedName name="Ops_Is_any_of_the_servers_above_virtualized_If_so__is_there_proper_isolation_between_VM_Host_administrators_and_the_IAM_team">'Interview Questions'!$E$383</definedName>
-    <definedName name="Ops_Is_there_proper_isolation_between_SQL_Admins_and_the_IAM_team">'Interview Questions'!$E$385</definedName>
-    <definedName name="Ops_Multiple_Azure_AD_Application_Proxy_connectors_per_group_deployed">'Interview Questions'!$F$363</definedName>
-    <definedName name="Ops_Multiple_Azure_AD_Pass_through_authentication_agents_deployed">'Interview Questions'!$F$364</definedName>
-    <definedName name="Ops_Secured_Azure_AD_App_Proxy_Connector">'Interview Questions'!$F$378</definedName>
-    <definedName name="Ops_Secured_Azure_AD_Connect_Servers">'Interview Questions'!$F$374</definedName>
-    <definedName name="Ops_Secured_NPS_Extension">'Interview Questions'!$F$380</definedName>
-    <definedName name="Ops_Secured_Pass_through_Authentication_Agent">'Interview Questions'!$F$379</definedName>
-    <definedName name="Ops_Secured_SQL_Server_for_ADFS">'Interview Questions'!$F$377</definedName>
-    <definedName name="Ops_Secured_SQL_Server_for_Azure_AD_Connect">'Interview Questions'!$F$375</definedName>
+    <definedName name="Ops_Are_there_compensating_controls_for_cases_where_the_answer_above_is_No">'Interview Questions'!$E$385</definedName>
+    <definedName name="Ops_Azure_AD_App_Proxy_debug_connector_group_deployed">'Interview Questions'!$F$363</definedName>
+    <definedName name="Ops_Debugging_tools_deployed_in_debug_app_proxy_connector">'Interview Questions'!$F$364</definedName>
+    <definedName name="Ops_Is_any_of_the_servers_above_virtualized_If_so__is_there_proper_isolation_between_VM_Host_administrators_and_the_IAM_team">'Interview Questions'!$E$381</definedName>
+    <definedName name="Ops_Is_there_proper_isolation_between_SQL_Admins_and_the_IAM_team">'Interview Questions'!$E$383</definedName>
+    <definedName name="Ops_Multiple_Azure_AD_Application_Proxy_connectors_per_group_deployed">'Interview Questions'!$F$361</definedName>
+    <definedName name="Ops_Multiple_Azure_AD_Pass_through_authentication_agents_deployed">'Interview Questions'!$F$362</definedName>
+    <definedName name="Ops_Secured_Azure_AD_App_Proxy_Connector">'Interview Questions'!$F$376</definedName>
+    <definedName name="Ops_Secured_Azure_AD_Connect_Servers">'Interview Questions'!$F$372</definedName>
+    <definedName name="Ops_Secured_NPS_Extension">'Interview Questions'!$F$378</definedName>
+    <definedName name="Ops_Secured_Pass_through_Authentication_Agent">'Interview Questions'!$F$377</definedName>
+    <definedName name="Ops_Secured_SQL_Server_for_ADFS">'Interview Questions'!$F$375</definedName>
+    <definedName name="Ops_Secured_SQL_Server_for_Azure_AD_Connect">'Interview Questions'!$F$373</definedName>
     <definedName name="YesNo">Lookups!$B$9:$B$11</definedName>
     <definedName name="YesNoPartial">Lookups!$B$3:$B$6</definedName>
   </definedNames>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="421">
   <si>
     <t>Identity Management</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>Check: Windows Hello for Business</t>
-  </si>
-  <si>
-    <t>Do your users use Windows Hello in their Windows 10 Desktops?</t>
   </si>
   <si>
     <t xml:space="preserve">Application Authentication and Assignment </t>
@@ -1243,9 +1240,6 @@
       </rPr>
       <t xml:space="preserve"> tab to answer the remaining questions.</t>
     </r>
-  </si>
-  <si>
-    <t>Have you deployed Windows Hello as an enterprise-wide policy?</t>
   </si>
   <si>
     <t>Are there “system accounts” that are also privileged?</t>
@@ -1509,6 +1503,9 @@
   </si>
   <si>
     <t>Do you have mobile management conditional access policies defined?</t>
+  </si>
+  <si>
+    <t>Has Windows Hello been deployed enterprise wide to all users?</t>
   </si>
 </sst>
 </file>
@@ -1889,8 +1886,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}" name="Table4" displayName="Table4" ref="E180:F186" totalsRowShown="0">
-  <autoFilter ref="E180:F186" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}" name="Table4" displayName="Table4" ref="E178:F184" totalsRowShown="0">
+  <autoFilter ref="E178:F184" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2F02BBB5-1E25-204E-B1A1-4DC986B80F65}" name="Best Practice"/>
     <tableColumn id="2" xr3:uid="{3C3E276B-0F40-5E47-996E-D83E08871D21}" name="Implemented by customer?" dataCellStyle="20% - Accent6"/>
@@ -1900,8 +1897,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}" name="Table5" displayName="Table5" ref="E255:F261" totalsRowShown="0">
-  <autoFilter ref="E255:F261" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}" name="Table5" displayName="Table5" ref="E253:F259" totalsRowShown="0">
+  <autoFilter ref="E253:F259" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2457BC44-3D28-2542-B982-8033983B8754}" name="Task"/>
     <tableColumn id="2" xr3:uid="{CED65D15-1D68-B246-875D-F0A2C4A946D3}" name="Person or Team name" dataCellStyle="20% - Accent6"/>
@@ -1911,8 +1908,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}" name="Table6" displayName="Table6" ref="E271:F282" totalsRowShown="0">
-  <autoFilter ref="E271:F282" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}" name="Table6" displayName="Table6" ref="E269:F280" totalsRowShown="0">
+  <autoFilter ref="E269:F280" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A3FEF98E-FE28-B84C-8912-4098BA527E76}" name="Kind of Change"/>
     <tableColumn id="2" xr3:uid="{CC851B68-8394-934D-96E0-625A92D7812E}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1922,8 +1919,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}" name="Table7" displayName="Table7" ref="E345:F357" totalsRowShown="0">
-  <autoFilter ref="E345:F357" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}" name="Table7" displayName="Table7" ref="E343:F355" totalsRowShown="0">
+  <autoFilter ref="E343:F355" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E9AA62EB-CA64-A84A-90FE-4FB406CFBB9B}" name="Task"/>
     <tableColumn id="2" xr3:uid="{A95B16A3-9350-3B42-AEC0-844DDF1A8645}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1933,8 +1930,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}" name="Table8" displayName="Table8" ref="E362:F366" totalsRowShown="0">
-  <autoFilter ref="E362:F366" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}" name="Table8" displayName="Table8" ref="E360:F364" totalsRowShown="0">
+  <autoFilter ref="E360:F364" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8E26C403-A376-C242-AC8E-6B61F7C1302E}" name="Best Practice"/>
     <tableColumn id="2" xr3:uid="{020742E9-39A6-0A45-9032-2C3C5E3B59B3}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -2262,7 +2259,7 @@
   <sheetData>
     <row r="2" spans="2:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2280,7 +2277,7 @@
     <row r="3" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C4" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2324,7 +2321,7 @@
     </row>
     <row r="8" spans="2:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2341,7 +2338,7 @@
     <row r="9" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="2:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D10" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -2357,7 +2354,7 @@
     <row r="11" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E12" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -2371,12 +2368,12 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F13" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E15" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -2390,32 +2387,32 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F16" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F19" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F22" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.2">
@@ -2423,7 +2420,7 @@
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.2">
@@ -2431,17 +2428,17 @@
     </row>
     <row r="30" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F31" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E33" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -2455,52 +2452,52 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F34" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F38" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F41" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -2508,7 +2505,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -2516,7 +2513,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G51" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -2524,7 +2521,7 @@
     </row>
     <row r="54" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E54" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -2538,32 +2535,32 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E55" s="11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F59" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -2571,7 +2568,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -2579,7 +2576,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -2587,7 +2584,7 @@
     </row>
     <row r="70" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E70" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -2601,15 +2598,15 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E71" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -2623,87 +2620,87 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E74" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F76" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F77" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F78" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F79" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F80" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F81" s="11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="83" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F83" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F84" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="85" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F85" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F86" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F87" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="88" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F88" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F89" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="90" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F90" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="92" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E92" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -2717,17 +2714,17 @@
     </row>
     <row r="93" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E93" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="94" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E94" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E95" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -2741,20 +2738,20 @@
     </row>
     <row r="96" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F96" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="97" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E97" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F97" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="99" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G99" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="100" spans="5:7" x14ac:dyDescent="0.2">
@@ -2764,7 +2761,7 @@
     </row>
     <row r="101" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G101" s="13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="102" spans="5:7" x14ac:dyDescent="0.2">
@@ -2772,7 +2769,7 @@
     </row>
     <row r="103" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G103" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.2">
@@ -2785,7 +2782,7 @@
     </row>
     <row r="106" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G106" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="107" spans="5:7" x14ac:dyDescent="0.2">
@@ -2798,7 +2795,7 @@
     </row>
     <row r="109" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G109" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="110" spans="5:7" x14ac:dyDescent="0.2">
@@ -2811,7 +2808,7 @@
     </row>
     <row r="112" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G112" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="113" spans="5:14" x14ac:dyDescent="0.2">
@@ -2824,32 +2821,32 @@
     </row>
     <row r="115" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G115" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="116" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G116" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="117" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G117" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="118" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G118" s="13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="119" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G119" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="122" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E122" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
@@ -2863,17 +2860,17 @@
     </row>
     <row r="123" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E123" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="124" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E124" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E125" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -2887,17 +2884,17 @@
     </row>
     <row r="126" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E126" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E127" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E128" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
@@ -2911,77 +2908,77 @@
     </row>
     <row r="129" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E129" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="130" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="131" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F131" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="132" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F132" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="133" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F133" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="134" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F134" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="135" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F135" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="136" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F136" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="137" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F137" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="138" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F138" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="140" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F140" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="141" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F141" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="143" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F143" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="144" spans="5:6" x14ac:dyDescent="0.2">
       <c r="F144" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="147" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D147" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
@@ -2997,7 +2994,7 @@
     <row r="148" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="149" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E149" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F149" s="3"/>
       <c r="G149" s="3"/>
@@ -3011,28 +3008,28 @@
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E150" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G152" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G153" s="7"/>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G155" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="158" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E158" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
@@ -3046,17 +3043,17 @@
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E159" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E160" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="161" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G161" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="162" spans="5:14" x14ac:dyDescent="0.2">
@@ -3064,7 +3061,7 @@
     </row>
     <row r="164" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G164" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="165" spans="5:14" x14ac:dyDescent="0.2">
@@ -3072,7 +3069,7 @@
     </row>
     <row r="167" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E167" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F167" s="3"/>
       <c r="G167" s="3"/>
@@ -3086,102 +3083,102 @@
     </row>
     <row r="168" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E168" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="169" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E169" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="170" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F170" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="171" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F171" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="172" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F172" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="173" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F173" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="174" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F174" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="175" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G175" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="176" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G176" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="177" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F177" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="178" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F178" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="179" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F179" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="180" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F180" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="181" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F181" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="182" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F182" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="183" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F183" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="184" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F184" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="185" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F185" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="186" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E186" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="188" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E188" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
@@ -3195,17 +3192,17 @@
     </row>
     <row r="189" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E189" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="190" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E190" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="191" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E191" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F191" s="3"/>
       <c r="G191" s="3"/>
@@ -3219,12 +3216,12 @@
     </row>
     <row r="192" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E192" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="194" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G194" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="195" spans="5:14" x14ac:dyDescent="0.2">
@@ -3232,7 +3229,7 @@
     </row>
     <row r="197" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G197" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="198" spans="5:14" x14ac:dyDescent="0.2">
@@ -3240,7 +3237,7 @@
     </row>
     <row r="200" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G200" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="201" spans="5:14" x14ac:dyDescent="0.2">
@@ -3248,7 +3245,7 @@
     </row>
     <row r="203" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E203" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F203" s="3"/>
       <c r="G203" s="3"/>
@@ -3262,42 +3259,42 @@
     </row>
     <row r="204" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E204" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="206" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E206" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="207" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E207" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="208" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E208" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="209" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E209" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="210" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E210" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="211" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E211" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="212" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E212" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F212" s="3"/>
       <c r="G212" s="3"/>
@@ -3311,82 +3308,82 @@
     </row>
     <row r="213" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F213" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="214" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F214" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="216" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F216" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="217" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F217" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="218" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F218" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="219" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F219" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="220" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F220" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="222" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F222" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="223" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F223" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="225" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F225" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="226" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F226" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="227" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E227" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="228" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F228" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="229" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F229" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="230" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E230" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="231" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E231" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F231" s="3"/>
       <c r="G231" s="3"/>
@@ -3400,165 +3397,165 @@
     </row>
     <row r="232" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F232" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="233" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F233" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="234" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F234" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="235" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F235" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="236" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F236" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="237" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F237" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="238" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F238" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="239" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F239" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="240" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F240" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="241" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F241" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="242" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F242" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="243" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F243" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="244" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F244" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="245" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F245" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="246" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F246" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="247" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F247" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="248" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F248" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="249" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F249" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="250" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F250" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="251" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F251" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="252" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F252" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="253" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F253" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="254" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F254" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="255" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F255" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="257" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F257" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="258" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F258" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="260" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F260" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="261" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F261" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="263" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F263" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="264" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E264" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F264" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E266" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="267" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E267" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F267" s="3"/>
       <c r="G267" s="3"/>
@@ -3572,82 +3569,82 @@
     </row>
     <row r="269" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F269" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="270" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F270" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="271" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F271" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="272" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F272" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="273" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F273" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="274" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F274" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="275" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F275" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="276" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F276" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="277" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F277" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="278" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F278" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="279" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F279" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="280" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F280" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="281" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F281" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="282" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F282" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="283" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E283" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="284" spans="3:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C284" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D284" s="1"/>
       <c r="E284" s="1"/>
@@ -3664,7 +3661,7 @@
     <row r="285" spans="3:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="286" spans="3:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D286" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E286" s="2"/>
       <c r="F286" s="2"/>
@@ -3679,27 +3676,27 @@
     </row>
     <row r="287" spans="3:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="E287" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="288" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E288" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="289" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E289" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="291" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E291" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="292" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C292" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D292" s="1"/>
       <c r="E292" s="1"/>
@@ -3715,17 +3712,17 @@
     </row>
     <row r="293" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D293" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="295" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E295" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="299" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3816,10 +3813,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B2:G387"/>
+  <dimension ref="B2:G385"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A117" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3834,7 +3831,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3845,42 +3842,42 @@
     <row r="3" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E5" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E8" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E11" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E14" s="12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -3992,7 +3989,7 @@
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.2">
@@ -4010,7 +4007,7 @@
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E44" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.2">
@@ -4020,7 +4017,7 @@
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.2">
@@ -4097,7 +4094,7 @@
     </row>
     <row r="65" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E65" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="66" spans="5:6" x14ac:dyDescent="0.2">
@@ -4209,7 +4206,7 @@
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E86" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.2">
@@ -4249,7 +4246,7 @@
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E95" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F95" s="7" t="s">
         <v>5</v>
@@ -4257,7 +4254,7 @@
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E96" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F96" s="7" t="s">
         <v>5</v>
@@ -4265,7 +4262,7 @@
     </row>
     <row r="97" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E97" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>6</v>
@@ -4289,7 +4286,7 @@
     </row>
     <row r="100" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>6</v>
@@ -4315,7 +4312,7 @@
     </row>
     <row r="105" spans="4:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E105" s="24" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F105" s="24"/>
     </row>
@@ -4326,7 +4323,7 @@
     </row>
     <row r="107" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E107" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="108" spans="4:7" x14ac:dyDescent="0.2">
@@ -4376,7 +4373,7 @@
     </row>
     <row r="119" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E119" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="120" spans="3:7" x14ac:dyDescent="0.2">
@@ -4412,7 +4409,7 @@
     </row>
     <row r="127" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E127" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="128" spans="3:7" x14ac:dyDescent="0.2">
@@ -4440,7 +4437,7 @@
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E133" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="134" spans="3:7" x14ac:dyDescent="0.2">
@@ -4458,37 +4455,37 @@
     </row>
     <row r="137" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E137" t="s">
-        <v>62</v>
+        <v>420</v>
       </c>
     </row>
     <row r="138" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E139" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="140" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E140" s="7"/>
-    </row>
-    <row r="142" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C142" s="2" t="s">
+    <row r="140" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C140" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+    </row>
+    <row r="141" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="142" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D142" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2"/>
-      <c r="G142" s="2"/>
-    </row>
-    <row r="143" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="144" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D144" s="3" t="s">
+      <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3"/>
+    </row>
+    <row r="143" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E143" t="s">
         <v>64</v>
       </c>
-      <c r="E144" s="3"/>
-      <c r="F144" s="3"/>
-      <c r="G144" s="3"/>
+    </row>
+    <row r="144" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E144" s="7"/>
     </row>
     <row r="145" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E145" t="s">
@@ -4520,23 +4517,23 @@
       </c>
     </row>
     <row r="152" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E152" s="7"/>
-    </row>
-    <row r="153" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E153" t="s">
+      <c r="E152" s="6"/>
+    </row>
+    <row r="154" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D154" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="154" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E154" s="6"/>
-    </row>
-    <row r="156" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D156" s="3" t="s">
+      <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3"/>
+    </row>
+    <row r="155" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E155" t="s">
         <v>70</v>
       </c>
-      <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
-      <c r="G156" s="3"/>
+    </row>
+    <row r="156" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E156" s="7"/>
     </row>
     <row r="157" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E157" t="s">
@@ -4544,23 +4541,23 @@
       </c>
     </row>
     <row r="158" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E158" s="7"/>
-    </row>
-    <row r="159" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E159" t="s">
+      <c r="E158" s="6"/>
+    </row>
+    <row r="160" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D160" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="160" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E160" s="6"/>
-    </row>
-    <row r="162" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D162" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
-      <c r="G162" s="3"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
+    </row>
+    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E161" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="162" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E162" s="7"/>
     </row>
     <row r="163" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E163" t="s">
@@ -4568,41 +4565,41 @@
       </c>
     </row>
     <row r="164" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E164" s="7"/>
+      <c r="E164" s="6"/>
     </row>
     <row r="165" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E165" t="s">
-        <v>186</v>
+        <v>73</v>
       </c>
     </row>
     <row r="166" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E166" s="6"/>
-    </row>
-    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E167" t="s">
+      <c r="E166" s="7"/>
+    </row>
+    <row r="168" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C168" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="168" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E168" s="7"/>
-    </row>
-    <row r="170" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C170" s="2" t="s">
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
+      <c r="G168" s="2"/>
+    </row>
+    <row r="169" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="170" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D170" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D170" s="2"/>
-      <c r="E170" s="2"/>
-      <c r="F170" s="2"/>
-      <c r="G170" s="2"/>
-    </row>
-    <row r="171" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="172" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D172" s="3" t="s">
+      <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3"/>
+    </row>
+    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E171" t="s">
         <v>76</v>
       </c>
-      <c r="E172" s="3"/>
-      <c r="F172" s="3"/>
-      <c r="G172" s="3"/>
+    </row>
+    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E172" s="7"/>
     </row>
     <row r="173" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E173" t="s">
@@ -4612,83 +4609,83 @@
     <row r="174" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E174" s="7"/>
     </row>
-    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E175" t="s">
+    <row r="176" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D176" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="176" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E176" s="7"/>
-    </row>
-    <row r="178" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D178" s="3" t="s">
+      <c r="E176" s="3"/>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3"/>
+    </row>
+    <row r="178" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E178" t="s">
         <v>79</v>
       </c>
-      <c r="E178" s="3"/>
-      <c r="F178" s="3"/>
-      <c r="G178" s="3"/>
+      <c r="F178" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="179" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E179" t="s">
+        <v>81</v>
+      </c>
+      <c r="F179" s="7"/>
     </row>
     <row r="180" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E180" t="s">
-        <v>80</v>
-      </c>
-      <c r="F180" t="s">
-        <v>81</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F180" s="7"/>
     </row>
     <row r="181" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E181" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F181" s="7"/>
     </row>
     <row r="182" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E182" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F182" s="7"/>
     </row>
     <row r="183" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E183" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F183" s="7"/>
     </row>
     <row r="184" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E184" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E185" t="s">
-        <v>86</v>
-      </c>
-      <c r="F185" s="7"/>
-    </row>
-    <row r="186" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E186" t="s">
+    <row r="186" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C186" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F186" s="7"/>
-    </row>
-    <row r="188" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C188" s="2" t="s">
+      <c r="D186" s="2"/>
+      <c r="E186" s="2"/>
+      <c r="F186" s="2"/>
+      <c r="G186" s="2"/>
+    </row>
+    <row r="187" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="188" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D188" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D188" s="2"/>
-      <c r="E188" s="2"/>
-      <c r="F188" s="2"/>
-      <c r="G188" s="2"/>
-    </row>
-    <row r="189" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="190" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D190" s="3" t="s">
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+    </row>
+    <row r="189" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E189" t="s">
         <v>89</v>
       </c>
-      <c r="E190" s="3"/>
-      <c r="F190" s="3"/>
-      <c r="G190" s="3"/>
+    </row>
+    <row r="190" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E190" s="7"/>
     </row>
     <row r="191" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E191" t="s">
@@ -4714,21 +4711,21 @@
     <row r="196" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E196" s="7"/>
     </row>
-    <row r="197" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E197" t="s">
+    <row r="198" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D198" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="198" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E198" s="7"/>
-    </row>
-    <row r="200" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D200" s="3" t="s">
+      <c r="E198" s="3"/>
+      <c r="F198" s="3"/>
+      <c r="G198" s="3"/>
+    </row>
+    <row r="199" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E199" t="s">
         <v>94</v>
       </c>
-      <c r="E200" s="3"/>
-      <c r="F200" s="3"/>
-      <c r="G200" s="3"/>
+    </row>
+    <row r="200" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E200" s="7"/>
     </row>
     <row r="201" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E201" t="s">
@@ -4744,33 +4741,33 @@
       </c>
     </row>
     <row r="204" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E204" s="7"/>
-    </row>
-    <row r="205" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E205" t="s">
+      <c r="E204" s="6"/>
+    </row>
+    <row r="206" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C206" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="206" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E206" s="6"/>
-    </row>
-    <row r="208" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C208" s="2" t="s">
+      <c r="D206" s="2"/>
+      <c r="E206" s="2"/>
+      <c r="F206" s="2"/>
+      <c r="G206" s="2"/>
+    </row>
+    <row r="207" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="208" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D208" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D208" s="2"/>
-      <c r="E208" s="2"/>
-      <c r="F208" s="2"/>
-      <c r="G208" s="2"/>
-    </row>
-    <row r="209" spans="4:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="210" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D210" s="3" t="s">
+      <c r="E208" s="3"/>
+      <c r="F208" s="3"/>
+      <c r="G208" s="3"/>
+    </row>
+    <row r="209" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E209" t="s">
         <v>99</v>
       </c>
-      <c r="E210" s="3"/>
-      <c r="F210" s="3"/>
-      <c r="G210" s="3"/>
+    </row>
+    <row r="210" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E210" s="7"/>
     </row>
     <row r="211" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E211" t="s">
@@ -4786,23 +4783,23 @@
       </c>
     </row>
     <row r="214" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E214" s="7"/>
-    </row>
-    <row r="215" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E215" t="s">
+      <c r="E214" s="6"/>
+    </row>
+    <row r="216" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D216" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="216" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E216" s="6"/>
-    </row>
-    <row r="218" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D218" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E218" s="3"/>
-      <c r="F218" s="3"/>
-      <c r="G218" s="3"/>
+      <c r="E216" s="3"/>
+      <c r="F216" s="3"/>
+      <c r="G216" s="3"/>
+    </row>
+    <row r="217" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E217" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="218" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E218" s="7"/>
     </row>
     <row r="219" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E219" t="s">
@@ -4810,7 +4807,7 @@
       </c>
     </row>
     <row r="220" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E220" s="7"/>
+      <c r="E220" s="6"/>
     </row>
     <row r="221" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E221" t="s">
@@ -4818,7 +4815,7 @@
       </c>
     </row>
     <row r="222" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E222" s="6"/>
+      <c r="E222" s="7"/>
     </row>
     <row r="223" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E223" t="s">
@@ -4826,7 +4823,7 @@
       </c>
     </row>
     <row r="224" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E224" s="7"/>
+      <c r="E224" s="6"/>
     </row>
     <row r="225" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E225" t="s">
@@ -4834,39 +4831,39 @@
       </c>
     </row>
     <row r="226" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E226" s="6"/>
+      <c r="E226" s="7"/>
     </row>
     <row r="227" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E227" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="228" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E228" s="7"/>
+      <c r="E228" s="6"/>
     </row>
     <row r="229" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E229" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="230" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E230" s="6"/>
+      <c r="E230" s="7"/>
     </row>
     <row r="231" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E231" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="232" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E232" s="7"/>
+      <c r="E232" s="6"/>
     </row>
     <row r="233" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E233" t="s">
-        <v>190</v>
+        <v>103</v>
       </c>
     </row>
     <row r="234" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E234" s="6"/>
+      <c r="E234" s="7"/>
     </row>
     <row r="235" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E235" t="s">
@@ -4878,7 +4875,7 @@
     </row>
     <row r="237" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E237" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
     </row>
     <row r="238" spans="5:5" x14ac:dyDescent="0.2">
@@ -4886,19 +4883,19 @@
     </row>
     <row r="239" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E239" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="240" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E240" s="7"/>
+      <c r="E240" s="6"/>
     </row>
     <row r="241" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E241" t="s">
-        <v>190</v>
+        <v>105</v>
       </c>
     </row>
     <row r="242" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E242" s="6"/>
+      <c r="E242" s="7"/>
     </row>
     <row r="243" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E243" t="s">
@@ -4908,112 +4905,112 @@
     <row r="244" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E244" s="7"/>
     </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E245" t="s">
+    <row r="246" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B246" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C246" s="1"/>
+      <c r="D246" s="1"/>
+      <c r="E246" s="1"/>
+      <c r="F246" s="1"/>
+      <c r="G246" s="1"/>
+    </row>
+    <row r="247" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B247" s="9"/>
+      <c r="C247" s="9"/>
+      <c r="D247" s="9"/>
+      <c r="E247" s="9"/>
+      <c r="F247" s="9"/>
+      <c r="G247" s="9"/>
+    </row>
+    <row r="248" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C248" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D248" s="2"/>
+      <c r="E248" s="2"/>
+      <c r="F248" s="2"/>
+      <c r="G248" s="2"/>
+    </row>
+    <row r="249" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="250" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D250" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E250" s="3"/>
+      <c r="F250" s="3"/>
+      <c r="G250" s="3"/>
+    </row>
+    <row r="251" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D251" s="10"/>
+      <c r="E251" t="s">
+        <v>193</v>
+      </c>
+      <c r="F251" s="10"/>
+      <c r="G251" s="10"/>
+    </row>
+    <row r="252" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E252" s="7"/>
+    </row>
+    <row r="253" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E253" t="s">
+        <v>8</v>
+      </c>
+      <c r="F253" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="254" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E254" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E246" s="7"/>
-    </row>
-    <row r="248" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B248" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C248" s="1"/>
-      <c r="D248" s="1"/>
-      <c r="E248" s="1"/>
-      <c r="F248" s="1"/>
-      <c r="G248" s="1"/>
-    </row>
-    <row r="249" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="9"/>
-      <c r="C249" s="9"/>
-      <c r="D249" s="9"/>
-      <c r="E249" s="9"/>
-      <c r="F249" s="9"/>
-      <c r="G249" s="9"/>
-    </row>
-    <row r="250" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C250" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D250" s="2"/>
-      <c r="E250" s="2"/>
-      <c r="F250" s="2"/>
-      <c r="G250" s="2"/>
-    </row>
-    <row r="251" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="252" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D252" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E252" s="3"/>
-      <c r="F252" s="3"/>
-      <c r="G252" s="3"/>
-    </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D253" s="10"/>
-      <c r="E253" t="s">
-        <v>194</v>
-      </c>
-      <c r="F253" s="10"/>
-      <c r="G253" s="10"/>
-    </row>
-    <row r="254" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E254" s="7"/>
+      <c r="F254" s="7"/>
     </row>
     <row r="255" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E255" t="s">
-        <v>8</v>
-      </c>
-      <c r="F255" t="s">
-        <v>195</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="F255" s="7"/>
     </row>
     <row r="256" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E256" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F256" s="7"/>
     </row>
     <row r="257" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E257" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F257" s="7"/>
     </row>
     <row r="258" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E258" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F258" s="7"/>
     </row>
     <row r="259" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E259" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F259" s="7"/>
     </row>
-    <row r="260" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E260" t="s">
-        <v>112</v>
-      </c>
-      <c r="F260" s="7"/>
-    </row>
-    <row r="261" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E261" t="s">
-        <v>113</v>
-      </c>
-      <c r="F261" s="7"/>
-    </row>
-    <row r="264" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D264" s="3" t="s">
+    <row r="262" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D262" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E262" s="3"/>
+      <c r="F262" s="3"/>
+      <c r="G262" s="3"/>
+    </row>
+    <row r="263" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E263" t="s">
         <v>147</v>
       </c>
-      <c r="E264" s="3"/>
-      <c r="F264" s="3"/>
-      <c r="G264" s="3"/>
+    </row>
+    <row r="264" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E264" s="7"/>
     </row>
     <row r="265" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E265" t="s">
@@ -5021,246 +5018,246 @@
       </c>
     </row>
     <row r="266" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E266" s="7"/>
+      <c r="E266" s="6"/>
     </row>
     <row r="267" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E267" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="268" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E268" s="6"/>
-    </row>
     <row r="269" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E269" t="s">
-        <v>150</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F269" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="270" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E270" t="s">
+        <v>114</v>
+      </c>
+      <c r="F270" s="7"/>
     </row>
     <row r="271" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E271" t="s">
-        <v>114</v>
-      </c>
-      <c r="F271" t="s">
-        <v>9</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="F271" s="7"/>
     </row>
     <row r="272" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E272" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F272" s="7"/>
     </row>
     <row r="273" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E273" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F273" s="7"/>
     </row>
     <row r="274" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E274" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F274" s="7"/>
     </row>
     <row r="275" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E275" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F275" s="7"/>
     </row>
     <row r="276" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E276" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F276" s="7"/>
     </row>
     <row r="277" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E277" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F277" s="7"/>
     </row>
     <row r="278" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E278" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F278" s="7"/>
     </row>
     <row r="279" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E279" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F279" s="7"/>
     </row>
     <row r="280" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E280" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F280" s="7"/>
     </row>
-    <row r="281" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E281" t="s">
-        <v>124</v>
-      </c>
-      <c r="F281" s="7"/>
-    </row>
-    <row r="282" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E282" t="s">
-        <v>125</v>
-      </c>
-      <c r="F282" s="7"/>
-    </row>
-    <row r="285" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C285" s="2" t="s">
+    <row r="283" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C283" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D283" s="2"/>
+      <c r="E283" s="2"/>
+      <c r="F283" s="2"/>
+      <c r="G283" s="2"/>
+    </row>
+    <row r="284" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="285" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D285" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D285" s="2"/>
-      <c r="E285" s="2"/>
-      <c r="F285" s="2"/>
-      <c r="G285" s="2"/>
-    </row>
-    <row r="286" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="287" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D287" s="3" t="s">
+      <c r="E285" s="3"/>
+      <c r="F285" s="3"/>
+      <c r="G285" s="3"/>
+    </row>
+    <row r="286" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E286" t="s">
         <v>152</v>
       </c>
-      <c r="E287" s="3"/>
-      <c r="F287" s="3"/>
-      <c r="G287" s="3"/>
+    </row>
+    <row r="287" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E287" s="7"/>
     </row>
     <row r="288" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E288" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="289" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E289" s="7"/>
     </row>
-    <row r="290" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E290" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="291" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E291" s="7"/>
     </row>
-    <row r="292" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E292" t="s">
+    <row r="293" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D293" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="293" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E293" s="7"/>
-    </row>
-    <row r="295" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D295" s="3" t="s">
+      <c r="E293" s="3"/>
+      <c r="F293" s="3"/>
+      <c r="G293" s="3"/>
+    </row>
+    <row r="294" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E294" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="295" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E295" s="7"/>
+    </row>
+    <row r="296" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E296" t="s">
         <v>156</v>
       </c>
-      <c r="E295" s="3"/>
-      <c r="F295" s="3"/>
-      <c r="G295" s="3"/>
-    </row>
-    <row r="296" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E296" t="s">
+    </row>
+    <row r="297" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E297" s="7"/>
+    </row>
+    <row r="298" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E298" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="297" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E297" s="7"/>
-    </row>
-    <row r="298" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E298" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="299" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="299" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E299" s="7"/>
     </row>
-    <row r="300" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="300" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E300" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="301" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="301" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E301" s="7"/>
     </row>
-    <row r="302" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E302" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="303" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E303" s="7"/>
-    </row>
-    <row r="305" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C305" s="2" t="s">
+    <row r="303" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C303" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D303" s="2"/>
+      <c r="E303" s="2"/>
+      <c r="F303" s="2"/>
+      <c r="G303" s="2"/>
+    </row>
+    <row r="304" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="305" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D305" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E305" s="3"/>
+      <c r="F305" s="3"/>
+      <c r="G305" s="3"/>
+    </row>
+    <row r="306" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E306" t="s">
         <v>158</v>
       </c>
-      <c r="D305" s="2"/>
-      <c r="E305" s="2"/>
-      <c r="F305" s="2"/>
-      <c r="G305" s="2"/>
-    </row>
-    <row r="306" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="307" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D307" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E307" s="3"/>
-      <c r="F307" s="3"/>
-      <c r="G307" s="3"/>
-    </row>
-    <row r="308" spans="3:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="307" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E307" s="7"/>
+    </row>
+    <row r="308" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E308" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="309" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E309" s="7"/>
     </row>
-    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="310" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E310" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="311" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E311" s="7"/>
     </row>
-    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="312" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E312" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="313" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="313" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E313" s="7"/>
     </row>
-    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="314" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E314" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="315" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E315" s="7"/>
     </row>
-    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="316" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E316" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="317" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E317" s="7"/>
     </row>
-    <row r="318" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="318" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E318" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="319" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E319" s="7"/>
     </row>
-    <row r="320" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="320" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E320" t="s">
-        <v>165</v>
+        <v>352</v>
       </c>
     </row>
     <row r="321" spans="4:7" x14ac:dyDescent="0.2">
@@ -5268,7 +5265,7 @@
     </row>
     <row r="322" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E322" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="323" spans="4:7" x14ac:dyDescent="0.2">
@@ -5284,7 +5281,7 @@
     </row>
     <row r="326" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E326" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="327" spans="4:7" x14ac:dyDescent="0.2">
@@ -5292,27 +5289,27 @@
     </row>
     <row r="328" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E328" t="s">
-        <v>356</v>
+        <v>165</v>
       </c>
     </row>
     <row r="329" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E329" s="7"/>
     </row>
-    <row r="330" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E330" t="s">
+    <row r="331" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D331" s="3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="331" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E331" s="7"/>
-    </row>
-    <row r="333" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D333" s="3" t="s">
+      <c r="E331" s="3"/>
+      <c r="F331" s="3"/>
+      <c r="G331" s="3"/>
+    </row>
+    <row r="333" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E333" t="s">
         <v>167</v>
       </c>
-      <c r="E333" s="3"/>
-      <c r="F333" s="3"/>
-      <c r="G333" s="3"/>
+    </row>
+    <row r="334" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E334" s="7"/>
     </row>
     <row r="335" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E335" t="s">
@@ -5322,277 +5319,269 @@
     <row r="336" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E336" s="7"/>
     </row>
-    <row r="337" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E337" t="s">
+    <row r="337" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B337" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="338" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E338" s="7"/>
-    </row>
-    <row r="339" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B339" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C339" s="1"/>
-      <c r="D339" s="1"/>
-      <c r="E339" s="1"/>
-      <c r="F339" s="1"/>
-      <c r="G339" s="1"/>
-    </row>
-    <row r="340" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B340" s="9"/>
-      <c r="C340" s="9"/>
-      <c r="D340" s="9"/>
-      <c r="E340" s="9"/>
-      <c r="F340" s="9"/>
-      <c r="G340" s="9"/>
-    </row>
-    <row r="341" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C341" s="2" t="s">
+      <c r="C337" s="1"/>
+      <c r="D337" s="1"/>
+      <c r="E337" s="1"/>
+      <c r="F337" s="1"/>
+      <c r="G337" s="1"/>
+    </row>
+    <row r="338" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B338" s="9"/>
+      <c r="C338" s="9"/>
+      <c r="D338" s="9"/>
+      <c r="E338" s="9"/>
+      <c r="F338" s="9"/>
+      <c r="G338" s="9"/>
+    </row>
+    <row r="339" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C339" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D341" s="2"/>
-      <c r="E341" s="2"/>
-      <c r="F341" s="2"/>
-      <c r="G341" s="2"/>
-    </row>
-    <row r="342" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="343" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D343" s="3" t="s">
+      <c r="D339" s="2"/>
+      <c r="E339" s="2"/>
+      <c r="F339" s="2"/>
+      <c r="G339" s="2"/>
+    </row>
+    <row r="340" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="341" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D341" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E343" s="3"/>
-      <c r="F343" s="3"/>
-      <c r="G343" s="3"/>
+      <c r="E341" s="3"/>
+      <c r="F341" s="3"/>
+      <c r="G341" s="3"/>
+    </row>
+    <row r="342" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E342" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="343" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E343" t="s">
+        <v>8</v>
+      </c>
+      <c r="F343" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="344" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E344" t="s">
-        <v>28</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="F344" s="7"/>
     </row>
     <row r="345" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E345" t="s">
-        <v>8</v>
-      </c>
-      <c r="F345" t="s">
-        <v>9</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="F345" s="7"/>
     </row>
     <row r="346" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E346" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F346" s="7"/>
     </row>
     <row r="347" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E347" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F347" s="7"/>
     </row>
     <row r="348" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E348" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F348" s="7"/>
     </row>
     <row r="349" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E349" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F349" s="7"/>
     </row>
     <row r="350" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E350" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F350" s="7"/>
     </row>
     <row r="351" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E351" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F351" s="7"/>
     </row>
     <row r="352" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E352" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F352" s="7"/>
     </row>
     <row r="353" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E353" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F353" s="7"/>
     </row>
     <row r="354" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E354" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F354" s="7"/>
     </row>
     <row r="355" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E355" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F355" s="7"/>
     </row>
-    <row r="356" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E356" t="s">
-        <v>137</v>
-      </c>
-      <c r="F356" s="7"/>
-    </row>
     <row r="357" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E357" t="s">
+      <c r="B357" t="s">
         <v>138</v>
       </c>
-      <c r="F357" s="7"/>
+    </row>
+    <row r="358" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D358" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E358" s="3"/>
+      <c r="F358" s="3"/>
+      <c r="G358" s="3"/>
     </row>
     <row r="359" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B359" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="360" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D360" s="3" t="s">
+      <c r="E359" t="s">
         <v>171</v>
       </c>
-      <c r="E360" s="3"/>
-      <c r="F360" s="3"/>
-      <c r="G360" s="3"/>
+    </row>
+    <row r="360" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E360" t="s">
+        <v>79</v>
+      </c>
+      <c r="F360" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="361" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E361" t="s">
-        <v>172</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="F361" s="7"/>
     </row>
     <row r="362" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E362" t="s">
-        <v>80</v>
-      </c>
-      <c r="F362" t="s">
-        <v>9</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F362" s="7"/>
     </row>
     <row r="363" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E363" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F363" s="7"/>
     </row>
     <row r="364" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E364" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F364" s="7"/>
     </row>
-    <row r="365" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E365" t="s">
-        <v>142</v>
-      </c>
-      <c r="F365" s="7"/>
-    </row>
-    <row r="366" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E366" t="s">
+    <row r="367" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C367" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D367" s="2"/>
+      <c r="E367" s="2"/>
+      <c r="F367" s="2"/>
+      <c r="G367" s="2"/>
+    </row>
+    <row r="368" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="369" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D369" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E369" s="3"/>
+      <c r="F369" s="3"/>
+      <c r="G369" s="3"/>
+    </row>
+    <row r="370" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E370" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="371" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E371" t="s">
         <v>143</v>
       </c>
-      <c r="F366" s="7"/>
-    </row>
-    <row r="369" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C369" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D369" s="2"/>
-      <c r="E369" s="2"/>
-      <c r="F369" s="2"/>
-      <c r="G369" s="2"/>
-    </row>
-    <row r="370" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="371" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D371" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E371" s="3"/>
-      <c r="F371" s="3"/>
-      <c r="G371" s="3"/>
-    </row>
-    <row r="372" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E372" t="s">
+    </row>
+    <row r="372" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E372" s="8" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="373" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E373" t="s">
+      <c r="F372" s="7"/>
+    </row>
+    <row r="373" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E373" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F373" s="7"/>
+    </row>
+    <row r="374" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E374" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="374" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E374" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F374" s="7"/>
-    </row>
-    <row r="375" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="375" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E375" s="8" t="s">
         <v>177</v>
       </c>
       <c r="F375" s="7"/>
     </row>
-    <row r="376" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E376" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="377" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="376" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E376" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F376" s="7"/>
+    </row>
+    <row r="377" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E377" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F377" s="7"/>
     </row>
-    <row r="378" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="378" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E378" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F378" s="7"/>
     </row>
-    <row r="379" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E379" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="F379" s="7"/>
-    </row>
-    <row r="380" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E380" s="8" t="s">
+    <row r="380" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E380" t="s">
         <v>181</v>
       </c>
-      <c r="F380" s="7"/>
-    </row>
-    <row r="382" spans="3:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="381" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E381" s="7"/>
+    </row>
+    <row r="382" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E382" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="383" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="383" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E383" s="7"/>
     </row>
-    <row r="384" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="384" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E384" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="385" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E385" s="7"/>
-    </row>
-    <row r="386" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E386" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="387" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E387" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5602,7 +5591,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23 E66 E58" xr:uid="{3C594C12-590A-7343-A03C-F6F925CF2C6D}">
       <formula1>YesNoPartial</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39 E48 E89 E104 E106 E108 E112 E114 E120 E128 E130 E132 E134 E138 E140 E146 E148 E150 E152 E158 E164 E168 E174 E176 F181:F186 E192 E194 E196 E198 E202 E204 E212 E214 E238 E236 E244 E246 E240 E232 E228 E224 E220 E254 E266 E289 E291 E293 E297 E299 E301 E303 E309 E311 E315 E317 E319 E323 E327 E331 E336 F363:F366 F374:F375 F377:F380 E383 E385 E387 E45 E85 E87 F95:F100 E125" xr:uid="{4BED4D73-49DB-8D4A-8D1E-63B573D30EBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39 E48 E89 E104 E106 E108 E112 E114 E120 E128 E130 E132 E134 E138 E144 E146 E148 E150 E156 E162 E166 E172 E174 F179:F184 E190 E192 E194 E196 E200 E202 E210 E212 E236 E234 E242 E244 E238 E230 E226 E222 E218 E252 E264 E287 E289 E291 E295 E297 E299 E301 E307 E309 E313 E315 E317 E321 E325 E329 E334 F361:F364 F372:F373 F375:F378 E381 E383 E385 E45 E85 E87 F95:F100 E125" xr:uid="{4BED4D73-49DB-8D4A-8D1E-63B573D30EBF}">
       <formula1>YesNo</formula1>
     </dataValidation>
   </dataValidations>
@@ -5642,7 +5631,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5652,7 +5641,7 @@
     <row r="3" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="23" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -5678,7 +5667,7 @@
     </row>
     <row r="9" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -5687,14 +5676,14 @@
     <row r="10" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
@@ -5704,19 +5693,19 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E15" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.2">
@@ -5726,12 +5715,12 @@
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E21" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.2">
@@ -5741,12 +5730,12 @@
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E25" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.2">
@@ -5756,12 +5745,12 @@
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E29" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.2">
@@ -5771,12 +5760,12 @@
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E33" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E35" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
@@ -5786,12 +5775,12 @@
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E37" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E39" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
@@ -5801,12 +5790,12 @@
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E41" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E43" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.2">
@@ -5816,19 +5805,19 @@
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E45" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="47" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D47" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E49" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="50" spans="5:5" x14ac:dyDescent="0.2">
@@ -5838,12 +5827,12 @@
     </row>
     <row r="51" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E51" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="53" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E53" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.2">
@@ -5853,12 +5842,12 @@
     </row>
     <row r="55" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E55" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="57" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E57" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="58" spans="5:5" x14ac:dyDescent="0.2">
@@ -5868,12 +5857,12 @@
     </row>
     <row r="59" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E59" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="61" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E61" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="62" spans="5:5" x14ac:dyDescent="0.2">
@@ -5883,7 +5872,7 @@
     </row>
     <row r="63" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E63" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="66" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -5897,14 +5886,14 @@
     <row r="67" spans="3:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="68" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D68" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E70" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.2">
@@ -5912,7 +5901,7 @@
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E72" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="75" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -5926,14 +5915,14 @@
     <row r="76" spans="3:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D77" s="3" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E79" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.2">
@@ -5941,7 +5930,7 @@
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E81" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -5990,7 +5979,7 @@
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
@@ -6010,32 +5999,32 @@
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed sort order for P0 and added type check to spreadsheet parsing
</commit_message>
<xml_diff>
--- a/assets/AzureADAssessment-Interview.xlsx
+++ b/assets/AzureADAssessment-Interview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Documents/GitHub/AzureADAssessment/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D94496D-3BD9-364E-967E-3B895893F885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A013EBA9-FC02-E547-8E12-E12B675E9FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="1" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Guided Walkthrough" sheetId="3" r:id="rId1"/>
@@ -31,91 +31,87 @@
     <definedName name="AADC_Is_the_Azure_AD_Connect_version_more_than_6_months_behind_the_latest_release">'Post-Interview Assessment'!$E$28</definedName>
     <definedName name="AADC_Is_there_a_consistent_volume_trend_of_add_deletes_over_1__and_or_updates_is_over_10">'Post-Interview Assessment'!$E$62</definedName>
     <definedName name="AADC_Is_there_a_mismatch_between_the_production_and_staging_configuration">'Post-Interview Assessment'!$E$24</definedName>
-    <definedName name="AccMgmt_Are_all_your_office_clients_in_versions_that_support_modern_authentication">'Interview Questions'!$E$190</definedName>
-    <definedName name="AccMgmt_Are_strong_credentials_used_for_SSPR">'Interview Questions'!#REF!</definedName>
-    <definedName name="AccMgmt_Are_strong_credentials_used_in_conditional_access_policies">'Interview Questions'!$E$108</definedName>
-    <definedName name="AccMgmt_Are_there_applications_that_can_be_candidates_to_use_attribute_based_access_control">'Interview Questions'!$E$166</definedName>
+    <definedName name="AccMgmt_Are_all_your_office_clients_in_versions_that_support_modern_authentication">'Interview Questions'!$E$193</definedName>
+    <definedName name="AccMgmt_Are_strong_credentials_used_in_conditional_access_policies">'Interview Questions'!$E$111</definedName>
+    <definedName name="AccMgmt_Are_there_applications_that_can_be_candidates_to_use_attribute_based_access_control">'Interview Questions'!$E$169</definedName>
     <definedName name="AccMgmt_Are_there_many_apps_using_passwords_for_client_secrets">'Post-Interview Assessment'!$E$80</definedName>
-    <definedName name="AccMgmt_Are_you_Archiving_AD_FS_audits">'Interview Questions'!$E$234</definedName>
-    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_security_incident_response">'Interview Questions'!$E$242</definedName>
-    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_support_and_troubleshooting_access_issues">'Interview Questions'!$E$244</definedName>
-    <definedName name="AccMgmt_Ban_Weak_Passwords">'Interview Questions'!$F$97</definedName>
-    <definedName name="AccMgmt_Detection_of_Leaked_Passwords">'Interview Questions'!$F$99</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$226</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$230</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Sign_in_Activity_Logs">'Interview Questions'!$E$222</definedName>
-    <definedName name="AccMgmt_Do_you_archive_Office_365_activity_logs">'Interview Questions'!$E$238</definedName>
-    <definedName name="AccMgmt_Do_you_enable_SSO_for_capable_apps_or_are_the_apps_that_use_local_accounts">'Interview Questions'!$E$148</definedName>
-    <definedName name="AccMgmt_Do_you_have_a_self_service_password_reset_solution">'Interview Questions'!$E$85</definedName>
-    <definedName name="AccMgmt_Do_you_have_a_SIEM_system">'Interview Questions'!$E$218</definedName>
-    <definedName name="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today">'Interview Questions'!$E$162</definedName>
-    <definedName name="AccMgmt_Do_you_have_applications_that_support_SAML_OpenID_connect_or_OAuth">'Interview Questions'!$E$144</definedName>
-    <definedName name="AccMgmt_Do_you_have_desktop_management_policies">'Interview Questions'!$E$130</definedName>
-    <definedName name="AccMgmt_Do_you_have_initiative_to_migrate_SSO_configuration_from_AD_FS_to_Azure_AD">'Interview Questions'!$E$156</definedName>
-    <definedName name="AccMgmt_Do_you_have_Intune_Application_Management_MAM_policies_defined">'Interview Questions'!$E$172</definedName>
-    <definedName name="AccMgmt_Do_you_have_mobile_management_policies_defined">'Interview Questions'!$E$128</definedName>
-    <definedName name="AccMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$66</definedName>
-    <definedName name="AccMgmt_Do_you_have_scripts_that_run_on_a_regular_basis">'Interview Questions'!#REF!</definedName>
-    <definedName name="AccMgmt_Do_you_have_service_accounts_or_applications_that_rely_on_legacy_authentication">'Interview Questions'!$E$196</definedName>
-    <definedName name="AccMgmt_Do_you_provision_strong_credentials_alongside_identity_provisioning_or_device_provisioning">'Interview Questions'!$E$106</definedName>
-    <definedName name="AccMgmt_Do_you_provision_strong_credentials_to_all_users_with_privileged_roles">'Interview Questions'!$E$104</definedName>
-    <definedName name="AccMgmt_Do_you_use_device_compliance_as_a_control_in_Conditional_Access">'Interview Questions'!$E$134</definedName>
-    <definedName name="AccMgmt_Do_you_use_them_in_CA_policies">'Interview Questions'!$E$174</definedName>
-    <definedName name="AccMgmt_Do_your_users_use_Windows_Hello_in_their_Windows_10_Desktops">'Interview Questions'!$E$138</definedName>
-    <definedName name="AccMgmt_Enable_ADFS_Smart_Soft_Lockout">'Interview Questions'!$F$100</definedName>
-    <definedName name="AccMgmt_Enable_passwordless_methods">'Interview Questions'!$F$96</definedName>
-    <definedName name="AccMgmt_Enforce_MFA_registration">'Interview Questions'!$F$98</definedName>
-    <definedName name="AccMgmt_Have_you_deployed_Azure_Log_Analytics">'Interview Questions'!$E$210</definedName>
-    <definedName name="AccMgmt_Have_you_deployed_Hybrid_Azure_AD_joined_in_your_environment">'Interview Questions'!$E$132</definedName>
-    <definedName name="AccMgmt_Have_you_deployed_Windows_Hello_as_an_enterprise_wide_policy">'Interview Questions'!#REF!</definedName>
-    <definedName name="AccMgmt_Have_you_enabled_All_Office_365_Auditing">'Interview Questions'!$E$236</definedName>
-    <definedName name="AccMgmt_Have_you_enabled_Password_Hash_Sync">'Interview Questions'!$E$112</definedName>
-    <definedName name="AccMgmt_Have_you_explicitly_identified_regions_where_authentication_should_NOT_be_coming_from">'Interview Questions'!$E$202</definedName>
-    <definedName name="AccMgmt_Have_you_identified_the_regions_of_the_world_where_authentication_traffic_should_be_coming_from">'Interview Questions'!$E$200</definedName>
-    <definedName name="AccMgmt_If_so_do_you_have_configured_the_applications_to_support_SSO_using_those_protocols">'Interview Questions'!$E$146</definedName>
-    <definedName name="AccMgmt_If_so_does_your_operations_team_use_it_regularly_to_understand_Azure_AD_usage">'Interview Questions'!$E$212</definedName>
-    <definedName name="AccMgmt_If_yes__is_this_using_Azure_AD_s_self_service_password_reset_solution">'Interview Questions'!$E$87</definedName>
-    <definedName name="AccMgmt_If_you_are_using_passwords_how_do_you_manage_the_them">'Interview Questions'!$E$122</definedName>
-    <definedName name="AccMgmt_If_you_use_federated_authentication_do_you_use_windows_integrated_authentication_WIA_when_inside_the_corporate_network">'Interview Questions'!#REF!</definedName>
-    <definedName name="AccMgmt_Is_legacy_authentication_blocked_by_conditional_access">'Interview Questions'!$E$194</definedName>
-    <definedName name="AccMgmt_Is_legacy_authentication_disabled_at_the_mailbox_level">'Interview Questions'!$E$192</definedName>
-    <definedName name="AccMgmt_Is_the_password_reset_part_of_the_operational_procedures_to_remediate_a_user_incident">'Interview Questions'!$E$89</definedName>
-    <definedName name="AccMgmt_Is_the_procedure_to_switch_to_PHS_practiced_enabled_to_the_IAM_Ops_team">'Interview Questions'!$E$114</definedName>
-    <definedName name="AccMgmt_Password_policy_uses_complexity_based_rules">'Interview Questions'!$F$95</definedName>
-    <definedName name="AccMgmt_What_platforms_do_you_use_to_provide_SSO_to_the_applications">'Interview Questions'!$E$150</definedName>
-    <definedName name="AccMgmt_What_process_do_you_have_to_discover_applications_that_are_not_configured_using_the_SSO_enterprise_solution">'Interview Questions'!$E$152</definedName>
-    <definedName name="AD_AssessmentDate">'Interview Questions'!$E$14</definedName>
-    <definedName name="AD_AssessorName">'Interview Questions'!$E$11</definedName>
+    <definedName name="AccMgmt_Are_you_Archiving_AD_FS_audits">'Interview Questions'!$E$237</definedName>
+    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_security_incident_response">'Interview Questions'!$E$245</definedName>
+    <definedName name="AccMgmt_Are_you_using_these_data_sources_for_support_and_troubleshooting_access_issues">'Interview Questions'!$E$247</definedName>
+    <definedName name="AccMgmt_Ban_Weak_Passwords">'Interview Questions'!$F$100</definedName>
+    <definedName name="AccMgmt_Detection_of_Leaked_Passwords">'Interview Questions'!$F$102</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$229</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$233</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Azure_AD_Sign_in_Activity_Logs">'Interview Questions'!$E$225</definedName>
+    <definedName name="AccMgmt_Do_you_archive_Office_365_activity_logs">'Interview Questions'!$E$241</definedName>
+    <definedName name="AccMgmt_Do_you_enable_SSO_for_capable_apps_or_are_the_apps_that_use_local_accounts">'Interview Questions'!$E$151</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_self_service_password_reset_solution">'Interview Questions'!$E$88</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_SIEM_system">'Interview Questions'!$E$221</definedName>
+    <definedName name="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today">'Interview Questions'!$E$165</definedName>
+    <definedName name="AccMgmt_Do_you_have_applications_that_support_SAML_OpenID_connect_or_OAuth">'Interview Questions'!$E$147</definedName>
+    <definedName name="AccMgmt_Do_you_have_desktop_management_policies">'Interview Questions'!$E$133</definedName>
+    <definedName name="AccMgmt_Do_you_have_initiative_to_migrate_SSO_configuration_from_AD_FS_to_Azure_AD">'Interview Questions'!$E$159</definedName>
+    <definedName name="AccMgmt_Do_you_have_Intune_Application_Management_MAM_policies_defined">'Interview Questions'!$E$175</definedName>
+    <definedName name="AccMgmt_Do_you_have_mobile_management_policies_defined">'Interview Questions'!$E$131</definedName>
+    <definedName name="AccMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$69</definedName>
+    <definedName name="AccMgmt_Do_you_have_service_accounts_or_applications_that_rely_on_legacy_authentication">'Interview Questions'!$E$199</definedName>
+    <definedName name="AccMgmt_Do_you_provision_strong_credentials_alongside_identity_provisioning_or_device_provisioning">'Interview Questions'!$E$109</definedName>
+    <definedName name="AccMgmt_Do_you_provision_strong_credentials_to_all_users_with_privileged_roles">'Interview Questions'!$E$107</definedName>
+    <definedName name="AccMgmt_Do_you_use_device_compliance_as_a_control_in_Conditional_Access">'Interview Questions'!$E$137</definedName>
+    <definedName name="AccMgmt_Do_you_use_them_in_CA_policies">'Interview Questions'!$E$177</definedName>
+    <definedName name="AccMgmt_Do_your_users_use_Windows_Hello_in_their_Windows_10_Desktops">'Interview Questions'!$E$141</definedName>
+    <definedName name="AccMgmt_Enable_ADFS_Smart_Soft_Lockout">'Interview Questions'!$F$103</definedName>
+    <definedName name="AccMgmt_Enable_passwordless_methods">'Interview Questions'!$F$99</definedName>
+    <definedName name="AccMgmt_Enforce_MFA_registration">'Interview Questions'!$F$101</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Azure_Log_Analytics">'Interview Questions'!$E$213</definedName>
+    <definedName name="AccMgmt_Have_you_deployed_Hybrid_Azure_AD_joined_in_your_environment">'Interview Questions'!$E$135</definedName>
+    <definedName name="AccMgmt_Have_you_enabled_All_Office_365_Auditing">'Interview Questions'!$E$239</definedName>
+    <definedName name="AccMgmt_Have_you_enabled_Password_Hash_Sync">'Interview Questions'!$E$115</definedName>
+    <definedName name="AccMgmt_Have_you_explicitly_identified_regions_where_authentication_should_NOT_be_coming_from">'Interview Questions'!$E$205</definedName>
+    <definedName name="AccMgmt_Have_you_identified_the_regions_of_the_world_where_authentication_traffic_should_be_coming_from">'Interview Questions'!$E$203</definedName>
+    <definedName name="AccMgmt_If_so_do_you_have_configured_the_applications_to_support_SSO_using_those_protocols">'Interview Questions'!$E$149</definedName>
+    <definedName name="AccMgmt_If_so_does_your_operations_team_use_it_regularly_to_understand_Azure_AD_usage">'Interview Questions'!$E$215</definedName>
+    <definedName name="AccMgmt_If_yes__is_this_using_Azure_AD_s_self_service_password_reset_solution">'Interview Questions'!$E$90</definedName>
+    <definedName name="AccMgmt_If_you_are_using_passwords_how_do_you_manage_the_them">'Interview Questions'!$E$125</definedName>
+    <definedName name="AccMgmt_Is_legacy_authentication_blocked_by_conditional_access">'Interview Questions'!$E$197</definedName>
+    <definedName name="AccMgmt_Is_legacy_authentication_disabled_at_the_mailbox_level">'Interview Questions'!$E$195</definedName>
+    <definedName name="AccMgmt_Is_the_password_reset_part_of_the_operational_procedures_to_remediate_a_user_incident">'Interview Questions'!$E$92</definedName>
+    <definedName name="AccMgmt_Is_the_procedure_to_switch_to_PHS_practiced_enabled_to_the_IAM_Ops_team">'Interview Questions'!$E$117</definedName>
+    <definedName name="AccMgmt_Password_policy_uses_complexity_based_rules">'Interview Questions'!$F$98</definedName>
+    <definedName name="AccMgmt_What_platforms_do_you_use_to_provide_SSO_to_the_applications">'Interview Questions'!$E$153</definedName>
+    <definedName name="AccMgmt_What_process_do_you_have_to_discover_applications_that_are_not_configured_using_the_SSO_enterprise_solution">'Interview Questions'!$E$155</definedName>
+    <definedName name="AD_AssessmentDate">'Interview Questions'!$E$17</definedName>
+    <definedName name="AD_AssessorName">'Interview Questions'!$E$14</definedName>
     <definedName name="AD_OrgName">'Interview Questions'!$E$5</definedName>
-    <definedName name="AD_OrgPrimaryContact">'Interview Questions'!$E$8</definedName>
-    <definedName name="Do_you_enforce_a_policy_that_requires_all_applications_to_use_a_certificate_credential">'Interview Questions'!$E$120</definedName>
-    <definedName name="EntMgmt_Do_you_use_Azure_AD_Outbound_provisioning_for_applications_in_your_environment_that_supports_Azure_AD_provisioning">'Interview Questions'!$E$58</definedName>
-    <definedName name="EntMgmt_What_is_the_approach_to_provision_to_applications_today">'Interview Questions'!$E$55</definedName>
-    <definedName name="Gov_Access_Review_Guest_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$301</definedName>
-    <definedName name="Gov_Access_Review_Guest_Is_it_automated">'Interview Questions'!$E$289</definedName>
-    <definedName name="Gov_AccessReview_Privileged_If_so_are_they_automated">'Interview Questions'!$E$317</definedName>
-    <definedName name="Gov_All_Users_Is_it_automated">'Interview Questions'!$E$299</definedName>
-    <definedName name="Gov_Are_there_system_accounts_that_are_also_privileged">'Interview Questions'!$E$321</definedName>
-    <definedName name="Gov_Do_administrators_have_dedicated_accounts_used_to_perform_privileged_operations">'Interview Questions'!$E$309</definedName>
-    <definedName name="Gov_Do_administrators_have_standing_access_to_privileges_in_your_environment">'Interview Questions'!$E$307</definedName>
-    <definedName name="Gov_Do_you_assign_users_to_the_All_Users_group">'Interview Questions'!$E$297</definedName>
-    <definedName name="Gov_Do_you_have_a_guest_access_review_strategy_in_place">'Interview Questions'!$E$295</definedName>
-    <definedName name="Gov_Do_you_have_a_privileged_role_strategy_for_Azure_Resources">'Interview Questions'!$E$329</definedName>
-    <definedName name="Gov_Do_you_have_a_process_to_identify_the_least_privileged_role_to_different_users_in_your_organization">'Interview Questions'!$E$313</definedName>
-    <definedName name="Gov_Do_you_have_a_test_environment">'Interview Questions'!$E$264</definedName>
-    <definedName name="Gov_Do_you_have_access_reviews_in_place_for_privileged_accounts">'Interview Questions'!$E$315</definedName>
-    <definedName name="Gov_Do_you_have_an_access_review_strategy_in_place">'Interview Questions'!$E$287</definedName>
-    <definedName name="Gov_Do_you_have_emergency_accounts_also_known_as_break_glass_provisioned_in_your_Azure_AD_tenant">'Interview Questions'!$E$334</definedName>
-    <definedName name="Gov_Do_you_have_owners_in_your_organization_for_all_the_tasks_listed_below">'Interview Questions'!$E$252</definedName>
-    <definedName name="Gov_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$291</definedName>
-    <definedName name="Gov_If_not_what_is_the_strategy_to_clean_up_remove_access">'Interview Questions'!$E$319</definedName>
-    <definedName name="Gov_If_so_how_do_establish_ownership_of_those_accounts">'Interview Questions'!$E$323</definedName>
-    <definedName name="Gov_Is_there_any_global_admin_outside_the_IAM_team">'Interview Questions'!$E$325</definedName>
-    <definedName name="IdMgmt_Do_you_have_a_disaster_recovery_production_instance_of_AAD_Connect_deployed_in_Staging_Mode">'Interview Questions'!$E$45</definedName>
-    <definedName name="IdMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$23</definedName>
-    <definedName name="IdMgmt_Do_you_synchronize_the_same_forest_where_users_log_in_to_their_Windows_devices">'Interview Questions'!$E$39</definedName>
-    <definedName name="IdMgmt_If_yes_do_you_have_a_process_in_place_to_ensure_the_configuration_of_the_instances_are_kept_in_sync">'Interview Questions'!$E$48</definedName>
-    <definedName name="If_you_use_cloud_authentication__PHS_or_PTA___are_users_prompted_to_type_in_the_password">'Interview Questions'!#REF!</definedName>
+    <definedName name="AD_OrgPrimaryContact">'Interview Questions'!$E$11</definedName>
+    <definedName name="AD_TenantId">'Interview Questions'!$E$8</definedName>
+    <definedName name="Do_you_enforce_a_policy_that_requires_all_applications_to_use_a_certificate_credential">'Interview Questions'!$E$123</definedName>
+    <definedName name="EntMgmt_Do_you_use_Azure_AD_Outbound_provisioning_for_applications_in_your_environment_that_supports_Azure_AD_provisioning">'Interview Questions'!$E$61</definedName>
+    <definedName name="EntMgmt_What_is_the_approach_to_provision_to_applications_today">'Interview Questions'!$E$58</definedName>
+    <definedName name="Gov_Access_Review_Guest_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$304</definedName>
+    <definedName name="Gov_Access_Review_Guest_Is_it_automated">'Interview Questions'!$E$292</definedName>
+    <definedName name="Gov_AccessReview_Privileged_If_so_are_they_automated">'Interview Questions'!$E$320</definedName>
+    <definedName name="Gov_All_Users_Is_it_automated">'Interview Questions'!$E$302</definedName>
+    <definedName name="Gov_Are_there_system_accounts_that_are_also_privileged">'Interview Questions'!$E$324</definedName>
+    <definedName name="Gov_Do_administrators_have_dedicated_accounts_used_to_perform_privileged_operations">'Interview Questions'!$E$312</definedName>
+    <definedName name="Gov_Do_administrators_have_standing_access_to_privileges_in_your_environment">'Interview Questions'!$E$310</definedName>
+    <definedName name="Gov_Do_you_assign_users_to_the_All_Users_group">'Interview Questions'!$E$300</definedName>
+    <definedName name="Gov_Do_you_have_a_guest_access_review_strategy_in_place">'Interview Questions'!$E$298</definedName>
+    <definedName name="Gov_Do_you_have_a_privileged_role_strategy_for_Azure_Resources">'Interview Questions'!$E$332</definedName>
+    <definedName name="Gov_Do_you_have_a_process_to_identify_the_least_privileged_role_to_different_users_in_your_organization">'Interview Questions'!$E$316</definedName>
+    <definedName name="Gov_Do_you_have_a_test_environment">'Interview Questions'!$E$267</definedName>
+    <definedName name="Gov_Do_you_have_access_reviews_in_place_for_privileged_accounts">'Interview Questions'!$E$318</definedName>
+    <definedName name="Gov_Do_you_have_an_access_review_strategy_in_place">'Interview Questions'!$E$290</definedName>
+    <definedName name="Gov_Do_you_have_emergency_accounts_also_known_as_break_glass_provisioned_in_your_Azure_AD_tenant">'Interview Questions'!$E$337</definedName>
+    <definedName name="Gov_Do_you_have_owners_in_your_organization_for_all_the_tasks_listed_below">'Interview Questions'!$E$255</definedName>
+    <definedName name="Gov_Do_you_run_it_on_a_regular_basis">'Interview Questions'!$E$294</definedName>
+    <definedName name="Gov_If_not_what_is_the_strategy_to_clean_up_remove_access">'Interview Questions'!$E$322</definedName>
+    <definedName name="Gov_If_so_how_do_establish_ownership_of_those_accounts">'Interview Questions'!$E$326</definedName>
+    <definedName name="Gov_Is_there_any_global_admin_outside_the_IAM_team">'Interview Questions'!$E$328</definedName>
+    <definedName name="IdMgmt_Do_you_have_a_disaster_recovery_production_instance_of_AAD_Connect_deployed_in_Staging_Mode">'Interview Questions'!$E$48</definedName>
+    <definedName name="IdMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$26</definedName>
+    <definedName name="IdMgmt_Do_you_synchronize_the_same_forest_where_users_log_in_to_their_Windows_devices">'Interview Questions'!$E$42</definedName>
+    <definedName name="IdMgmt_If_yes_do_you_have_a_process_in_place_to_ensure_the_configuration_of_the_instances_are_kept_in_sync">'Interview Questions'!$E$51</definedName>
     <definedName name="Lic_Are_there_outstanding_licensing_errors_shown_in_the_portal">'Guided Walkthrough'!$G$100</definedName>
     <definedName name="Lic_Do_you_have_a_defined_process_automated_or_manual_to_monitor_and_resolve_licensing_errors">'Guided Walkthrough'!$G$104</definedName>
     <definedName name="Lic_Do_you_use_Group_Based_Licensing_to_assign_licenses">'Guided Walkthrough'!$G$110</definedName>
@@ -123,19 +119,19 @@
     <definedName name="Lic_If_GBL_is_not_used__how_would_you_rate_your_current_approach_to_licensing">'Guided Walkthrough'!$G$116</definedName>
     <definedName name="Lic_If_yes__is_GBL_deployed_against_on_premises_groups_that_lack_lifecycle_management">'Guided Walkthrough'!$G$113</definedName>
     <definedName name="LookupLicenceMaturity">Lookups!$B$14:$B$17</definedName>
-    <definedName name="Ops_Are_there_compensating_controls_for_cases_where_the_answer_above_is_No">'Interview Questions'!$E$385</definedName>
-    <definedName name="Ops_Azure_AD_App_Proxy_debug_connector_group_deployed">'Interview Questions'!$F$363</definedName>
-    <definedName name="Ops_Debugging_tools_deployed_in_debug_app_proxy_connector">'Interview Questions'!$F$364</definedName>
-    <definedName name="Ops_Is_any_of_the_servers_above_virtualized_If_so__is_there_proper_isolation_between_VM_Host_administrators_and_the_IAM_team">'Interview Questions'!$E$381</definedName>
-    <definedName name="Ops_Is_there_proper_isolation_between_SQL_Admins_and_the_IAM_team">'Interview Questions'!$E$383</definedName>
-    <definedName name="Ops_Multiple_Azure_AD_Application_Proxy_connectors_per_group_deployed">'Interview Questions'!$F$361</definedName>
-    <definedName name="Ops_Multiple_Azure_AD_Pass_through_authentication_agents_deployed">'Interview Questions'!$F$362</definedName>
-    <definedName name="Ops_Secured_Azure_AD_App_Proxy_Connector">'Interview Questions'!$F$376</definedName>
-    <definedName name="Ops_Secured_Azure_AD_Connect_Servers">'Interview Questions'!$F$372</definedName>
-    <definedName name="Ops_Secured_NPS_Extension">'Interview Questions'!$F$378</definedName>
-    <definedName name="Ops_Secured_Pass_through_Authentication_Agent">'Interview Questions'!$F$377</definedName>
-    <definedName name="Ops_Secured_SQL_Server_for_ADFS">'Interview Questions'!$F$375</definedName>
-    <definedName name="Ops_Secured_SQL_Server_for_Azure_AD_Connect">'Interview Questions'!$F$373</definedName>
+    <definedName name="Ops_Are_there_compensating_controls_for_cases_where_the_answer_above_is_No">'Interview Questions'!$E$388</definedName>
+    <definedName name="Ops_Azure_AD_App_Proxy_debug_connector_group_deployed">'Interview Questions'!$F$366</definedName>
+    <definedName name="Ops_Debugging_tools_deployed_in_debug_app_proxy_connector">'Interview Questions'!$F$367</definedName>
+    <definedName name="Ops_Is_any_of_the_servers_above_virtualized_If_so__is_there_proper_isolation_between_VM_Host_administrators_and_the_IAM_team">'Interview Questions'!$E$384</definedName>
+    <definedName name="Ops_Is_there_proper_isolation_between_SQL_Admins_and_the_IAM_team">'Interview Questions'!$E$386</definedName>
+    <definedName name="Ops_Multiple_Azure_AD_Application_Proxy_connectors_per_group_deployed">'Interview Questions'!$F$364</definedName>
+    <definedName name="Ops_Multiple_Azure_AD_Pass_through_authentication_agents_deployed">'Interview Questions'!$F$365</definedName>
+    <definedName name="Ops_Secured_Azure_AD_App_Proxy_Connector">'Interview Questions'!$F$379</definedName>
+    <definedName name="Ops_Secured_Azure_AD_Connect_Servers">'Interview Questions'!$F$375</definedName>
+    <definedName name="Ops_Secured_NPS_Extension">'Interview Questions'!$F$381</definedName>
+    <definedName name="Ops_Secured_Pass_through_Authentication_Agent">'Interview Questions'!$F$380</definedName>
+    <definedName name="Ops_Secured_SQL_Server_for_ADFS">'Interview Questions'!$F$378</definedName>
+    <definedName name="Ops_Secured_SQL_Server_for_Azure_AD_Connect">'Interview Questions'!$F$376</definedName>
     <definedName name="YesNo">Lookups!$B$9:$B$11</definedName>
     <definedName name="YesNoPartial">Lookups!$B$3:$B$6</definedName>
   </definedNames>
@@ -159,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="423">
   <si>
     <t>Identity Management</t>
   </si>
@@ -1288,9 +1284,6 @@
   </si>
   <si>
     <t>Merill Fernando</t>
-  </si>
-  <si>
-    <t>8 Jan 2020</t>
   </si>
   <si>
     <t>Sync Configuration</t>
@@ -1506,6 +1499,15 @@
   </si>
   <si>
     <t>Has Windows Hello been deployed enterprise wide to all users?</t>
+  </si>
+  <si>
+    <t>Tenant ID</t>
+  </si>
+  <si>
+    <t>22 Jan 2020</t>
+  </si>
+  <si>
+    <t>233-43434</t>
   </si>
 </sst>
 </file>
@@ -1811,6 +1813,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1822,13 +1825,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
@@ -1853,8 +1855,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B36D8961-BC83-5D43-B45B-1CFA5936C943}" name="Table1" displayName="Table1" ref="E25:F32" totalsRowShown="0">
-  <autoFilter ref="E25:F32" xr:uid="{B36D8961-BC83-5D43-B45B-1CFA5936C943}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B36D8961-BC83-5D43-B45B-1CFA5936C943}" name="Table1" displayName="Table1" ref="E28:F35" totalsRowShown="0">
+  <autoFilter ref="E28:F35" xr:uid="{B36D8961-BC83-5D43-B45B-1CFA5936C943}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4ED8CD0E-9332-654B-A2F0-5F3AB7F52CAA}" name="Task"/>
     <tableColumn id="2" xr3:uid="{967EBA5C-CDB3-F147-8472-01C37BF57B1D}" name="Name of Person/Team owning task" dataCellStyle="20% - Accent6"/>
@@ -1864,8 +1866,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1C4D0D2B-6272-644B-B58A-F2D915C5B531}" name="Table2" displayName="Table2" ref="E68:F79" totalsRowShown="0">
-  <autoFilter ref="E68:F79" xr:uid="{1C4D0D2B-6272-644B-B58A-F2D915C5B531}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1C4D0D2B-6272-644B-B58A-F2D915C5B531}" name="Table2" displayName="Table2" ref="E71:F82" totalsRowShown="0">
+  <autoFilter ref="E71:F82" xr:uid="{1C4D0D2B-6272-644B-B58A-F2D915C5B531}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C04652F9-C32E-3C48-8CFD-8D2D01D07ADB}" name="Task"/>
     <tableColumn id="2" xr3:uid="{24027322-E3B5-184F-9BAA-F77393BB4FF9}" name="Name of Person/Team owning task" dataCellStyle="20% - Accent6"/>
@@ -1875,8 +1877,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6048BA92-D829-6543-BE60-C242238787A6}" name="Table3" displayName="Table3" ref="E94:F100" totalsRowShown="0">
-  <autoFilter ref="E94:F100" xr:uid="{6048BA92-D829-6543-BE60-C242238787A6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6048BA92-D829-6543-BE60-C242238787A6}" name="Table3" displayName="Table3" ref="E97:F103" totalsRowShown="0">
+  <autoFilter ref="E97:F103" xr:uid="{6048BA92-D829-6543-BE60-C242238787A6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{65AE8C0B-4B46-A24D-86F8-26F3FA1BFA41}" name="Policy Setting"/>
     <tableColumn id="2" xr3:uid="{F0A657E9-871F-E942-AB05-DE5CB9B6CBF1}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1886,8 +1888,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}" name="Table4" displayName="Table4" ref="E178:F184" totalsRowShown="0">
-  <autoFilter ref="E178:F184" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}" name="Table4" displayName="Table4" ref="E181:F187" totalsRowShown="0">
+  <autoFilter ref="E181:F187" xr:uid="{CF375A00-F71F-4F45-A2BB-86A2EE2F423E}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2F02BBB5-1E25-204E-B1A1-4DC986B80F65}" name="Best Practice"/>
     <tableColumn id="2" xr3:uid="{3C3E276B-0F40-5E47-996E-D83E08871D21}" name="Implemented by customer?" dataCellStyle="20% - Accent6"/>
@@ -1897,8 +1899,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}" name="Table5" displayName="Table5" ref="E253:F259" totalsRowShown="0">
-  <autoFilter ref="E253:F259" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}" name="Table5" displayName="Table5" ref="E256:F262" totalsRowShown="0">
+  <autoFilter ref="E256:F262" xr:uid="{C38CFA0A-8AA7-4D4F-B3A9-68020E3A12BB}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2457BC44-3D28-2542-B982-8033983B8754}" name="Task"/>
     <tableColumn id="2" xr3:uid="{CED65D15-1D68-B246-875D-F0A2C4A946D3}" name="Person or Team name" dataCellStyle="20% - Accent6"/>
@@ -1908,8 +1910,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}" name="Table6" displayName="Table6" ref="E269:F280" totalsRowShown="0">
-  <autoFilter ref="E269:F280" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}" name="Table6" displayName="Table6" ref="E272:F283" totalsRowShown="0">
+  <autoFilter ref="E272:F283" xr:uid="{E594F828-D477-B945-8006-CCA22CA7B726}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A3FEF98E-FE28-B84C-8912-4098BA527E76}" name="Kind of Change"/>
     <tableColumn id="2" xr3:uid="{CC851B68-8394-934D-96E0-625A92D7812E}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1919,8 +1921,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}" name="Table7" displayName="Table7" ref="E343:F355" totalsRowShown="0">
-  <autoFilter ref="E343:F355" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}" name="Table7" displayName="Table7" ref="E346:F358" totalsRowShown="0">
+  <autoFilter ref="E346:F358" xr:uid="{2B226A2F-D20D-244C-A7E2-A31BEA253D96}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E9AA62EB-CA64-A84A-90FE-4FB406CFBB9B}" name="Task"/>
     <tableColumn id="2" xr3:uid="{A95B16A3-9350-3B42-AEC0-844DDF1A8645}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -1930,8 +1932,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}" name="Table8" displayName="Table8" ref="E360:F364" totalsRowShown="0">
-  <autoFilter ref="E360:F364" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}" name="Table8" displayName="Table8" ref="E363:F367" totalsRowShown="0">
+  <autoFilter ref="E363:F367" xr:uid="{DE0E52F7-D903-7E40-AD71-705086EC1DE5}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{8E26C403-A376-C242-AC8E-6B61F7C1302E}" name="Best Practice"/>
     <tableColumn id="2" xr3:uid="{020742E9-39A6-0A45-9032-2C3C5E3B59B3}" name="Customer Answer" dataCellStyle="20% - Accent6"/>
@@ -2276,48 +2278,48 @@
     </row>
     <row r="3" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="19"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="22"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="23"/>
     </row>
     <row r="8" spans="2:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
@@ -2751,7 +2753,7 @@
     </row>
     <row r="99" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G99" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="100" spans="5:7" x14ac:dyDescent="0.2">
@@ -2761,7 +2763,7 @@
     </row>
     <row r="101" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G101" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="102" spans="5:7" x14ac:dyDescent="0.2">
@@ -2769,7 +2771,7 @@
     </row>
     <row r="103" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G103" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.2">
@@ -2782,7 +2784,7 @@
     </row>
     <row r="106" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G106" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="107" spans="5:7" x14ac:dyDescent="0.2">
@@ -2795,7 +2797,7 @@
     </row>
     <row r="109" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G109" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110" spans="5:7" x14ac:dyDescent="0.2">
@@ -2808,7 +2810,7 @@
     </row>
     <row r="112" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G112" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="113" spans="5:14" x14ac:dyDescent="0.2">
@@ -2821,27 +2823,27 @@
     </row>
     <row r="115" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G115" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="116" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G116" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="117" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G117" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="118" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G118" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="119" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G119" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="122" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3813,10 +3815,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B2:G385"/>
+  <dimension ref="B2:G388"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A117" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3852,425 +3854,411 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>365</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="5" t="s">
-        <v>366</v>
+      <c r="E8" s="12" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E11" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="12" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E17" s="12" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E22" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E23" s="5" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E26" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E25" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
         <v>8</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E26" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E27" t="s">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E28" t="s">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E29" t="s">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E30" t="s">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E31" t="s">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E32" t="s">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="34" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="2" t="s">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="37" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E38" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E39" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E41" t="s">
-        <v>21</v>
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E42" s="7"/>
+      <c r="E42" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E44" t="s">
-        <v>373</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E45" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="E45" s="7"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E48" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E51" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="1" t="s">
+    <row r="54" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="E54" t="s">
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E55" s="7"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E57" t="s">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E58" s="7"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E58" s="7" t="s">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E61" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="1" t="s">
+    <row r="63" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C62" s="2" t="s">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D64" s="3" t="s">
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E65" t="s">
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E69" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>29</v>
+      </c>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>30</v>
+      </c>
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>31</v>
+      </c>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>33</v>
+      </c>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>34</v>
+      </c>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>36</v>
+      </c>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>37</v>
+      </c>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" s="7"/>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>39</v>
+      </c>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="84" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D86" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E88" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E89" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E66" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E68" t="s">
-        <v>8</v>
-      </c>
-      <c r="F68" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E69" t="s">
-        <v>29</v>
-      </c>
-      <c r="F69" s="7"/>
-    </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E70" t="s">
-        <v>30</v>
-      </c>
-      <c r="F70" s="7"/>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E71" t="s">
-        <v>31</v>
-      </c>
-      <c r="F71" s="7"/>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E72" t="s">
-        <v>32</v>
-      </c>
-      <c r="F72" s="7"/>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E73" t="s">
-        <v>33</v>
-      </c>
-      <c r="F73" s="7"/>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E74" t="s">
-        <v>34</v>
-      </c>
-      <c r="F74" s="7"/>
-    </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E75" t="s">
-        <v>35</v>
-      </c>
-      <c r="F75" s="7"/>
-    </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E76" t="s">
-        <v>36</v>
-      </c>
-      <c r="F76" s="7"/>
-    </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E77" t="s">
-        <v>37</v>
-      </c>
-      <c r="F77" s="7"/>
-    </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E78" t="s">
-        <v>38</v>
-      </c>
-      <c r="F78" s="7"/>
-    </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E79" t="s">
-        <v>39</v>
-      </c>
-      <c r="F79" s="7"/>
-    </row>
-    <row r="81" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C81" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="83" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D83" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E84" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E85" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E86" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E87" s="7"/>
-    </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E88" t="s">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E90" s="7"/>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E91" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E89" s="7"/>
-    </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E90" t="s">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E92" s="7"/>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E93" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E91" s="6"/>
-    </row>
-    <row r="92" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D92" s="3" t="s">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E94" s="6"/>
+    </row>
+    <row r="95" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D95" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-    </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E94" t="s">
-        <v>46</v>
-      </c>
-      <c r="F94" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E95" t="s">
-        <v>410</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E96" t="s">
-        <v>408</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
     </row>
     <row r="97" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E97" t="s">
-        <v>411</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>6</v>
+        <v>46</v>
+      </c>
+      <c r="F97" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E98" t="s">
-        <v>47</v>
+        <v>409</v>
       </c>
       <c r="F98" s="7" t="s">
         <v>5</v>
@@ -4278,1320 +4266,1344 @@
     </row>
     <row r="99" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E99" t="s">
-        <v>48</v>
+        <v>407</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D102" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
+    <row r="101" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E101" t="s">
+        <v>47</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E102" t="s">
+        <v>48</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="103" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E103" t="s">
+        <v>408</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D105" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+    </row>
+    <row r="106" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E106" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E104" s="7" t="s">
+    <row r="107" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E107" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="4:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E105" s="24" t="s">
+    <row r="108" spans="4:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E108" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="F108" s="24"/>
+    </row>
+    <row r="109" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E109" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E110" t="s">
         <v>412</v>
       </c>
-      <c r="F105" s="24"/>
-    </row>
-    <row r="106" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E106" s="7" t="s">
+    </row>
+    <row r="111" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E111" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E107" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="108" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E108" s="7" t="s">
+    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D113" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E114" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E115" s="7"/>
+    </row>
+    <row r="116" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E116" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="117" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E118" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="119" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E119" s="6"/>
+    </row>
+    <row r="121" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D121" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+    </row>
+    <row r="122" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E122" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="123" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E123" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E124" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="125" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E125" s="6"/>
+    </row>
+    <row r="127" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C127" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+    </row>
+    <row r="128" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="129" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D129" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+    </row>
+    <row r="130" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E130" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="131" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E131" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D110" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
-      <c r="G110" s="3"/>
-    </row>
-    <row r="111" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E111" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="112" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E112" s="7"/>
-    </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E113" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="114" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E114" s="7"/>
-    </row>
-    <row r="115" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E115" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="116" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E116" s="6"/>
-    </row>
-    <row r="118" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D118" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
-    </row>
-    <row r="119" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E119" t="s">
+    <row r="132" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E132" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="133" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E133" s="7"/>
+    </row>
+    <row r="134" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E134" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E135" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E136" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="120" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E120" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="121" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E121" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="122" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E122" s="6"/>
-    </row>
-    <row r="124" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C124" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
-    </row>
-    <row r="125" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="126" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D126" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
-      <c r="G126" s="3"/>
-    </row>
-    <row r="127" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E127" t="s">
+    <row r="137" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E137" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E139" s="3"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
+    </row>
+    <row r="140" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E140" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="128" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E128" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E129" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="130" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E130" s="7"/>
-    </row>
-    <row r="131" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E131" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="132" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E132" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="133" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E133" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="134" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E134" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="136" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D136" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E136" s="3"/>
-      <c r="F136" s="3"/>
-      <c r="G136" s="3"/>
-    </row>
-    <row r="137" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E137" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="138" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E138" s="7"/>
-    </row>
-    <row r="140" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C140" s="2" t="s">
+    <row r="141" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E141" s="7"/>
+    </row>
+    <row r="143" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C143" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
-    </row>
-    <row r="141" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="142" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D142" s="3" t="s">
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+    </row>
+    <row r="144" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="145" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D145" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E142" s="3"/>
-      <c r="F142" s="3"/>
-      <c r="G142" s="3"/>
-    </row>
-    <row r="143" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E143" t="s">
+      <c r="E145" s="3"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3"/>
+    </row>
+    <row r="146" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E146" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="144" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E144" s="7"/>
-    </row>
-    <row r="145" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E145" t="s">
+    <row r="147" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E147" s="7"/>
+    </row>
+    <row r="148" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E148" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="146" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E146" s="7"/>
-    </row>
-    <row r="147" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E147" t="s">
+    <row r="149" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E149" s="7"/>
+    </row>
+    <row r="150" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E150" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="148" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E148" s="7"/>
-    </row>
-    <row r="149" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E149" t="s">
+    <row r="151" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E151" s="7"/>
+    </row>
+    <row r="152" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E152" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="150" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E150" s="7"/>
-    </row>
-    <row r="151" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E151" t="s">
+    <row r="153" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E153" s="7"/>
+    </row>
+    <row r="154" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E154" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="152" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E152" s="6"/>
-    </row>
-    <row r="154" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D154" s="3" t="s">
+    <row r="155" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E155" s="6"/>
+    </row>
+    <row r="157" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D157" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E154" s="3"/>
-      <c r="F154" s="3"/>
-      <c r="G154" s="3"/>
-    </row>
-    <row r="155" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E155" t="s">
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3"/>
+    </row>
+    <row r="158" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E158" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="156" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E156" s="7"/>
-    </row>
-    <row r="157" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E157" t="s">
+    <row r="159" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E160" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="158" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E158" s="6"/>
-    </row>
-    <row r="160" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D160" s="3" t="s">
+    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E161" s="6"/>
+    </row>
+    <row r="163" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D163" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
-      <c r="G160" s="3"/>
-    </row>
-    <row r="161" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E161" t="s">
+      <c r="E163" s="3"/>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
+    </row>
+    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E164" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="162" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E162" s="7"/>
-    </row>
-    <row r="163" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E163" t="s">
+    <row r="165" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E165" s="7"/>
+    </row>
+    <row r="166" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E166" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="164" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E164" s="6"/>
-    </row>
-    <row r="165" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E165" t="s">
+    <row r="167" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E167" s="6"/>
+    </row>
+    <row r="168" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E168" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="166" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E166" s="7"/>
-    </row>
-    <row r="168" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C168" s="2" t="s">
+    <row r="169" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E169" s="7"/>
+    </row>
+    <row r="171" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C171" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D168" s="2"/>
-      <c r="E168" s="2"/>
-      <c r="F168" s="2"/>
-      <c r="G168" s="2"/>
-    </row>
-    <row r="169" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="170" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D170" s="3" t="s">
+      <c r="D171" s="2"/>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
+      <c r="G171" s="2"/>
+    </row>
+    <row r="172" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="173" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D173" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E170" s="3"/>
-      <c r="F170" s="3"/>
-      <c r="G170" s="3"/>
-    </row>
-    <row r="171" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E171" t="s">
+      <c r="E173" s="3"/>
+      <c r="F173" s="3"/>
+      <c r="G173" s="3"/>
+    </row>
+    <row r="174" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E174" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="172" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E172" s="7"/>
-    </row>
-    <row r="173" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E173" t="s">
+    <row r="175" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E175" s="7"/>
+    </row>
+    <row r="176" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E176" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E174" s="7"/>
-    </row>
-    <row r="176" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D176" s="3" t="s">
+    <row r="177" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E177" s="7"/>
+    </row>
+    <row r="179" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D179" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E176" s="3"/>
-      <c r="F176" s="3"/>
-      <c r="G176" s="3"/>
-    </row>
-    <row r="178" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E178" t="s">
-        <v>79</v>
-      </c>
-      <c r="F178" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="179" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E179" t="s">
-        <v>81</v>
-      </c>
-      <c r="F179" s="7"/>
-    </row>
-    <row r="180" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E180" t="s">
-        <v>82</v>
-      </c>
-      <c r="F180" s="7"/>
+      <c r="E179" s="3"/>
+      <c r="F179" s="3"/>
+      <c r="G179" s="3"/>
     </row>
     <row r="181" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E181" t="s">
-        <v>83</v>
-      </c>
-      <c r="F181" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="F181" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="182" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E182" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F182" s="7"/>
     </row>
     <row r="183" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E183" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F183" s="7"/>
     </row>
     <row r="184" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E184" t="s">
+        <v>83</v>
+      </c>
+      <c r="F184" s="7"/>
+    </row>
+    <row r="185" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E185" t="s">
+        <v>84</v>
+      </c>
+      <c r="F185" s="7"/>
+    </row>
+    <row r="186" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E186" t="s">
+        <v>85</v>
+      </c>
+      <c r="F186" s="7"/>
+    </row>
+    <row r="187" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E187" t="s">
         <v>86</v>
       </c>
-      <c r="F184" s="7"/>
-    </row>
-    <row r="186" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C186" s="2" t="s">
+      <c r="F187" s="7"/>
+    </row>
+    <row r="189" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C189" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D186" s="2"/>
-      <c r="E186" s="2"/>
-      <c r="F186" s="2"/>
-      <c r="G186" s="2"/>
-    </row>
-    <row r="187" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="188" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D188" s="3" t="s">
+      <c r="D189" s="2"/>
+      <c r="E189" s="2"/>
+      <c r="F189" s="2"/>
+      <c r="G189" s="2"/>
+    </row>
+    <row r="190" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="191" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D191" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E188" s="3"/>
-      <c r="F188" s="3"/>
-      <c r="G188" s="3"/>
-    </row>
-    <row r="189" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E189" t="s">
+      <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
+    </row>
+    <row r="192" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E192" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="190" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E190" s="7"/>
-    </row>
-    <row r="191" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E191" t="s">
+    <row r="193" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E193" s="7"/>
+    </row>
+    <row r="194" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E194" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="192" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E192" s="7"/>
-    </row>
-    <row r="193" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E193" t="s">
+    <row r="195" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E195" s="7"/>
+    </row>
+    <row r="196" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E196" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="194" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E194" s="7"/>
-    </row>
-    <row r="195" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E195" t="s">
+    <row r="197" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E197" s="7"/>
+    </row>
+    <row r="198" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E198" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="196" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E196" s="7"/>
-    </row>
-    <row r="198" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D198" s="3" t="s">
+    <row r="199" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E199" s="7"/>
+    </row>
+    <row r="201" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D201" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E198" s="3"/>
-      <c r="F198" s="3"/>
-      <c r="G198" s="3"/>
-    </row>
-    <row r="199" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E199" t="s">
+      <c r="E201" s="3"/>
+      <c r="F201" s="3"/>
+      <c r="G201" s="3"/>
+    </row>
+    <row r="202" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E202" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="200" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E200" s="7"/>
-    </row>
-    <row r="201" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E201" t="s">
+    <row r="203" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E203" s="7"/>
+    </row>
+    <row r="204" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E204" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="202" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E202" s="7"/>
-    </row>
-    <row r="203" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E203" t="s">
+    <row r="205" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E205" s="7"/>
+    </row>
+    <row r="206" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E206" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="204" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E204" s="6"/>
-    </row>
-    <row r="206" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C206" s="2" t="s">
+    <row r="207" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E207" s="6"/>
+    </row>
+    <row r="209" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C209" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D206" s="2"/>
-      <c r="E206" s="2"/>
-      <c r="F206" s="2"/>
-      <c r="G206" s="2"/>
-    </row>
-    <row r="207" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="208" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D208" s="3" t="s">
+      <c r="D209" s="2"/>
+      <c r="E209" s="2"/>
+      <c r="F209" s="2"/>
+      <c r="G209" s="2"/>
+    </row>
+    <row r="210" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="211" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D211" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E208" s="3"/>
-      <c r="F208" s="3"/>
-      <c r="G208" s="3"/>
-    </row>
-    <row r="209" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E209" t="s">
+      <c r="E211" s="3"/>
+      <c r="F211" s="3"/>
+      <c r="G211" s="3"/>
+    </row>
+    <row r="212" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E212" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="210" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E210" s="7"/>
-    </row>
-    <row r="211" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E211" t="s">
+    <row r="213" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E213" s="7"/>
+    </row>
+    <row r="214" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E214" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="212" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E212" s="7"/>
-    </row>
-    <row r="213" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E213" t="s">
+    <row r="215" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E215" s="7"/>
+    </row>
+    <row r="216" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E216" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="214" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E214" s="6"/>
-    </row>
-    <row r="216" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D216" s="3" t="s">
+    <row r="217" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E217" s="6"/>
+    </row>
+    <row r="219" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D219" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E216" s="3"/>
-      <c r="F216" s="3"/>
-      <c r="G216" s="3"/>
-    </row>
-    <row r="217" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E217" t="s">
+      <c r="E219" s="3"/>
+      <c r="F219" s="3"/>
+      <c r="G219" s="3"/>
+    </row>
+    <row r="220" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E220" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="218" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E218" s="7"/>
-    </row>
-    <row r="219" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E219" t="s">
+    <row r="221" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E221" s="7"/>
+    </row>
+    <row r="222" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E222" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="220" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E220" s="6"/>
-    </row>
-    <row r="221" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E221" t="s">
+    <row r="223" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E223" s="6"/>
+    </row>
+    <row r="224" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E224" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="222" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E222" s="7"/>
-    </row>
-    <row r="223" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E223" t="s">
+    <row r="225" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E225" s="7"/>
+    </row>
+    <row r="226" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E226" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="224" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E224" s="6"/>
-    </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E225" t="s">
+    <row r="227" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E227" s="6"/>
+    </row>
+    <row r="228" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E228" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E226" s="7"/>
-    </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E227" t="s">
+    <row r="229" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E229" s="7"/>
+    </row>
+    <row r="230" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E230" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E228" s="6"/>
-    </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E229" t="s">
+    <row r="231" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E231" s="6"/>
+    </row>
+    <row r="232" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E232" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E230" s="7"/>
-    </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E231" t="s">
+    <row r="233" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E233" s="7"/>
+    </row>
+    <row r="234" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E234" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E232" s="6"/>
-    </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E233" t="s">
+    <row r="235" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E235" s="6"/>
+    </row>
+    <row r="236" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E236" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E234" s="7"/>
-    </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E235" t="s">
+    <row r="237" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E237" s="7"/>
+    </row>
+    <row r="238" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E238" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E236" s="7"/>
-    </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E237" t="s">
+    <row r="239" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E239" s="7"/>
+    </row>
+    <row r="240" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E240" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E238" s="7"/>
-    </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E239" t="s">
+    <row r="241" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E241" s="7"/>
+    </row>
+    <row r="242" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E242" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E240" s="6"/>
-    </row>
-    <row r="241" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E241" t="s">
+    <row r="243" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E243" s="6"/>
+    </row>
+    <row r="244" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E244" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E242" s="7"/>
-    </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E243" t="s">
+    <row r="245" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E245" s="7"/>
+    </row>
+    <row r="246" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E246" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E244" s="7"/>
-    </row>
-    <row r="246" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B246" s="1" t="s">
+    <row r="247" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E247" s="7"/>
+    </row>
+    <row r="249" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B249" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C246" s="1"/>
-      <c r="D246" s="1"/>
-      <c r="E246" s="1"/>
-      <c r="F246" s="1"/>
-      <c r="G246" s="1"/>
-    </row>
-    <row r="247" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="9"/>
-      <c r="C247" s="9"/>
-      <c r="D247" s="9"/>
-      <c r="E247" s="9"/>
-      <c r="F247" s="9"/>
-      <c r="G247" s="9"/>
-    </row>
-    <row r="248" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C248" s="2" t="s">
+      <c r="C249" s="1"/>
+      <c r="D249" s="1"/>
+      <c r="E249" s="1"/>
+      <c r="F249" s="1"/>
+      <c r="G249" s="1"/>
+    </row>
+    <row r="250" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B250" s="9"/>
+      <c r="C250" s="9"/>
+      <c r="D250" s="9"/>
+      <c r="E250" s="9"/>
+      <c r="F250" s="9"/>
+      <c r="G250" s="9"/>
+    </row>
+    <row r="251" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C251" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D248" s="2"/>
-      <c r="E248" s="2"/>
-      <c r="F248" s="2"/>
-      <c r="G248" s="2"/>
-    </row>
-    <row r="249" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="250" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D250" s="3" t="s">
+      <c r="D251" s="2"/>
+      <c r="E251" s="2"/>
+      <c r="F251" s="2"/>
+      <c r="G251" s="2"/>
+    </row>
+    <row r="252" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="253" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D253" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E250" s="3"/>
-      <c r="F250" s="3"/>
-      <c r="G250" s="3"/>
-    </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D251" s="10"/>
-      <c r="E251" t="s">
+      <c r="E253" s="3"/>
+      <c r="F253" s="3"/>
+      <c r="G253" s="3"/>
+    </row>
+    <row r="254" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D254" s="10"/>
+      <c r="E254" t="s">
         <v>193</v>
       </c>
-      <c r="F251" s="10"/>
-      <c r="G251" s="10"/>
-    </row>
-    <row r="252" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E252" s="7"/>
-    </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E253" t="s">
-        <v>8</v>
-      </c>
-      <c r="F253" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="254" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E254" t="s">
-        <v>107</v>
-      </c>
-      <c r="F254" s="7"/>
+      <c r="F254" s="10"/>
+      <c r="G254" s="10"/>
     </row>
     <row r="255" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E255" t="s">
-        <v>108</v>
-      </c>
-      <c r="F255" s="7"/>
+      <c r="E255" s="7"/>
     </row>
     <row r="256" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E256" t="s">
-        <v>109</v>
-      </c>
-      <c r="F256" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F256" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="257" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E257" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F257" s="7"/>
     </row>
     <row r="258" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E258" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F258" s="7"/>
     </row>
     <row r="259" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E259" t="s">
+        <v>109</v>
+      </c>
+      <c r="F259" s="7"/>
+    </row>
+    <row r="260" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E260" t="s">
+        <v>110</v>
+      </c>
+      <c r="F260" s="7"/>
+    </row>
+    <row r="261" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E261" t="s">
+        <v>111</v>
+      </c>
+      <c r="F261" s="7"/>
+    </row>
+    <row r="262" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E262" t="s">
         <v>112</v>
       </c>
-      <c r="F259" s="7"/>
-    </row>
-    <row r="262" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D262" s="3" t="s">
+      <c r="F262" s="7"/>
+    </row>
+    <row r="265" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D265" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E262" s="3"/>
-      <c r="F262" s="3"/>
-      <c r="G262" s="3"/>
-    </row>
-    <row r="263" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E263" t="s">
+      <c r="E265" s="3"/>
+      <c r="F265" s="3"/>
+      <c r="G265" s="3"/>
+    </row>
+    <row r="266" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E266" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="264" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E264" s="7"/>
-    </row>
-    <row r="265" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E265" t="s">
+    <row r="267" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E267" s="7"/>
+    </row>
+    <row r="268" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E268" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="266" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E266" s="6"/>
-    </row>
-    <row r="267" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E267" t="s">
-        <v>149</v>
-      </c>
-    </row>
     <row r="269" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E269" t="s">
-        <v>113</v>
-      </c>
-      <c r="F269" t="s">
-        <v>9</v>
-      </c>
+      <c r="E269" s="6"/>
     </row>
     <row r="270" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E270" t="s">
-        <v>114</v>
-      </c>
-      <c r="F270" s="7"/>
-    </row>
-    <row r="271" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E271" t="s">
-        <v>115</v>
-      </c>
-      <c r="F271" s="7"/>
+        <v>149</v>
+      </c>
     </row>
     <row r="272" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E272" t="s">
-        <v>116</v>
-      </c>
-      <c r="F272" s="7"/>
+        <v>113</v>
+      </c>
+      <c r="F272" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="273" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E273" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F273" s="7"/>
     </row>
     <row r="274" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E274" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F274" s="7"/>
     </row>
     <row r="275" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E275" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F275" s="7"/>
     </row>
     <row r="276" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E276" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F276" s="7"/>
     </row>
     <row r="277" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E277" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F277" s="7"/>
     </row>
     <row r="278" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E278" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F278" s="7"/>
     </row>
     <row r="279" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E279" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F279" s="7"/>
     </row>
     <row r="280" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E280" t="s">
+        <v>121</v>
+      </c>
+      <c r="F280" s="7"/>
+    </row>
+    <row r="281" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E281" t="s">
+        <v>122</v>
+      </c>
+      <c r="F281" s="7"/>
+    </row>
+    <row r="282" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E282" t="s">
+        <v>123</v>
+      </c>
+      <c r="F282" s="7"/>
+    </row>
+    <row r="283" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E283" t="s">
         <v>124</v>
       </c>
-      <c r="F280" s="7"/>
-    </row>
-    <row r="283" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C283" s="2" t="s">
+      <c r="F283" s="7"/>
+    </row>
+    <row r="286" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C286" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D283" s="2"/>
-      <c r="E283" s="2"/>
-      <c r="F283" s="2"/>
-      <c r="G283" s="2"/>
-    </row>
-    <row r="284" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="285" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D285" s="3" t="s">
+      <c r="D286" s="2"/>
+      <c r="E286" s="2"/>
+      <c r="F286" s="2"/>
+      <c r="G286" s="2"/>
+    </row>
+    <row r="287" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="288" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D288" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E285" s="3"/>
-      <c r="F285" s="3"/>
-      <c r="G285" s="3"/>
-    </row>
-    <row r="286" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E286" t="s">
+      <c r="E288" s="3"/>
+      <c r="F288" s="3"/>
+      <c r="G288" s="3"/>
+    </row>
+    <row r="289" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E289" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="287" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E287" s="7"/>
-    </row>
-    <row r="288" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E288" t="s">
+    <row r="290" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E290" s="7"/>
+    </row>
+    <row r="291" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E291" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="289" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E289" s="7"/>
-    </row>
-    <row r="290" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E290" t="s">
+    <row r="292" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E292" s="7"/>
+    </row>
+    <row r="293" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E293" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="291" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E291" s="7"/>
-    </row>
-    <row r="293" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D293" s="3" t="s">
+    <row r="294" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E294" s="7"/>
+    </row>
+    <row r="296" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D296" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E293" s="3"/>
-      <c r="F293" s="3"/>
-      <c r="G293" s="3"/>
-    </row>
-    <row r="294" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E294" t="s">
+      <c r="E296" s="3"/>
+      <c r="F296" s="3"/>
+      <c r="G296" s="3"/>
+    </row>
+    <row r="297" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E297" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="295" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E295" s="7"/>
-    </row>
-    <row r="296" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E296" t="s">
+    <row r="298" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E298" s="7"/>
+    </row>
+    <row r="299" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E299" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="297" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E297" s="7"/>
-    </row>
-    <row r="298" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E298" t="s">
+    <row r="300" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E300" s="7"/>
+    </row>
+    <row r="301" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E301" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="299" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E299" s="7"/>
-    </row>
-    <row r="300" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E300" t="s">
+    <row r="302" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E302" s="7"/>
+    </row>
+    <row r="303" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E303" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="301" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E301" s="7"/>
-    </row>
-    <row r="303" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C303" s="2" t="s">
+    <row r="304" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E304" s="7"/>
+    </row>
+    <row r="306" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C306" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D303" s="2"/>
-      <c r="E303" s="2"/>
-      <c r="F303" s="2"/>
-      <c r="G303" s="2"/>
-    </row>
-    <row r="304" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="305" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D305" s="3" t="s">
+      <c r="D306" s="2"/>
+      <c r="E306" s="2"/>
+      <c r="F306" s="2"/>
+      <c r="G306" s="2"/>
+    </row>
+    <row r="307" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="308" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D308" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E305" s="3"/>
-      <c r="F305" s="3"/>
-      <c r="G305" s="3"/>
-    </row>
-    <row r="306" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E306" t="s">
+      <c r="E308" s="3"/>
+      <c r="F308" s="3"/>
+      <c r="G308" s="3"/>
+    </row>
+    <row r="309" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E309" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="307" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E307" s="7"/>
-    </row>
-    <row r="308" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E308" t="s">
+    <row r="310" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E310" s="7"/>
+    </row>
+    <row r="311" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E311" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="309" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E309" s="7"/>
-    </row>
-    <row r="310" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E310" t="s">
+    <row r="312" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E312" s="7"/>
+    </row>
+    <row r="313" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E313" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="311" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E311" s="7"/>
-    </row>
-    <row r="312" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E312" t="s">
+    <row r="314" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E314" s="7"/>
+    </row>
+    <row r="315" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E315" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="313" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E313" s="7"/>
-    </row>
-    <row r="314" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E314" t="s">
+    <row r="316" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E316" s="7"/>
+    </row>
+    <row r="317" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E317" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="315" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E315" s="7"/>
-    </row>
-    <row r="316" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E316" t="s">
+    <row r="318" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E318" s="7"/>
+    </row>
+    <row r="319" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E319" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="317" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E317" s="7"/>
-    </row>
-    <row r="318" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E318" t="s">
+    <row r="320" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E320" s="7"/>
+    </row>
+    <row r="321" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E321" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="319" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E319" s="7"/>
-    </row>
-    <row r="320" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E320" t="s">
+    <row r="322" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E322" s="7"/>
+    </row>
+    <row r="323" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E323" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="321" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E321" s="7"/>
-    </row>
-    <row r="322" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E322" t="s">
+    <row r="324" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E324" s="7"/>
+    </row>
+    <row r="325" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E325" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="323" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E323" s="7"/>
-    </row>
-    <row r="324" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E324" t="s">
+    <row r="326" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E326" s="7"/>
+    </row>
+    <row r="327" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E327" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="325" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E325" s="7"/>
-    </row>
-    <row r="326" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E326" t="s">
+    <row r="328" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E328" s="7"/>
+    </row>
+    <row r="329" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E329" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="327" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E327" s="7"/>
-    </row>
-    <row r="328" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E328" t="s">
+    <row r="330" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E330" s="7"/>
+    </row>
+    <row r="331" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E331" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="329" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E329" s="7"/>
-    </row>
-    <row r="331" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D331" s="3" t="s">
+    <row r="332" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E332" s="7"/>
+    </row>
+    <row r="334" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D334" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E331" s="3"/>
-      <c r="F331" s="3"/>
-      <c r="G331" s="3"/>
-    </row>
-    <row r="333" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E333" t="s">
+      <c r="E334" s="3"/>
+      <c r="F334" s="3"/>
+      <c r="G334" s="3"/>
+    </row>
+    <row r="336" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E336" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="334" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E334" s="7"/>
-    </row>
-    <row r="335" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E335" t="s">
+    <row r="337" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E337" s="7"/>
+    </row>
+    <row r="338" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E338" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="336" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E336" s="7"/>
-    </row>
-    <row r="337" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B337" s="1" t="s">
+    <row r="339" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E339" s="7"/>
+    </row>
+    <row r="340" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B340" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C337" s="1"/>
-      <c r="D337" s="1"/>
-      <c r="E337" s="1"/>
-      <c r="F337" s="1"/>
-      <c r="G337" s="1"/>
-    </row>
-    <row r="338" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B338" s="9"/>
-      <c r="C338" s="9"/>
-      <c r="D338" s="9"/>
-      <c r="E338" s="9"/>
-      <c r="F338" s="9"/>
-      <c r="G338" s="9"/>
-    </row>
-    <row r="339" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C339" s="2" t="s">
+      <c r="C340" s="1"/>
+      <c r="D340" s="1"/>
+      <c r="E340" s="1"/>
+      <c r="F340" s="1"/>
+      <c r="G340" s="1"/>
+    </row>
+    <row r="341" spans="2:7" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B341" s="9"/>
+      <c r="C341" s="9"/>
+      <c r="D341" s="9"/>
+      <c r="E341" s="9"/>
+      <c r="F341" s="9"/>
+      <c r="G341" s="9"/>
+    </row>
+    <row r="342" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C342" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D339" s="2"/>
-      <c r="E339" s="2"/>
-      <c r="F339" s="2"/>
-      <c r="G339" s="2"/>
-    </row>
-    <row r="340" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="341" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D341" s="3" t="s">
+      <c r="D342" s="2"/>
+      <c r="E342" s="2"/>
+      <c r="F342" s="2"/>
+      <c r="G342" s="2"/>
+    </row>
+    <row r="343" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="344" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D344" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E341" s="3"/>
-      <c r="F341" s="3"/>
-      <c r="G341" s="3"/>
-    </row>
-    <row r="342" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E342" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="343" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E343" t="s">
-        <v>8</v>
-      </c>
-      <c r="F343" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="344" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E344" t="s">
-        <v>126</v>
-      </c>
-      <c r="F344" s="7"/>
+      <c r="E344" s="3"/>
+      <c r="F344" s="3"/>
+      <c r="G344" s="3"/>
     </row>
     <row r="345" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E345" t="s">
-        <v>127</v>
-      </c>
-      <c r="F345" s="7"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="346" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E346" t="s">
-        <v>128</v>
-      </c>
-      <c r="F346" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F346" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="347" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E347" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F347" s="7"/>
     </row>
     <row r="348" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E348" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F348" s="7"/>
     </row>
     <row r="349" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E349" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F349" s="7"/>
     </row>
     <row r="350" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E350" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F350" s="7"/>
     </row>
     <row r="351" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E351" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F351" s="7"/>
     </row>
     <row r="352" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E352" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F352" s="7"/>
     </row>
     <row r="353" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E353" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F353" s="7"/>
     </row>
     <row r="354" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E354" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F354" s="7"/>
     </row>
     <row r="355" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E355" t="s">
+        <v>134</v>
+      </c>
+      <c r="F355" s="7"/>
+    </row>
+    <row r="356" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E356" t="s">
+        <v>135</v>
+      </c>
+      <c r="F356" s="7"/>
+    </row>
+    <row r="357" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E357" t="s">
+        <v>136</v>
+      </c>
+      <c r="F357" s="7"/>
+    </row>
+    <row r="358" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E358" t="s">
         <v>137</v>
       </c>
-      <c r="F355" s="7"/>
-    </row>
-    <row r="357" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B357" t="s">
+      <c r="F358" s="7"/>
+    </row>
+    <row r="360" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B360" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="358" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D358" s="3" t="s">
+    <row r="361" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D361" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E358" s="3"/>
-      <c r="F358" s="3"/>
-      <c r="G358" s="3"/>
-    </row>
-    <row r="359" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E359" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="360" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E360" t="s">
-        <v>79</v>
-      </c>
-      <c r="F360" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="361" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E361" t="s">
-        <v>139</v>
-      </c>
-      <c r="F361" s="7"/>
+      <c r="E361" s="3"/>
+      <c r="F361" s="3"/>
+      <c r="G361" s="3"/>
     </row>
     <row r="362" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E362" t="s">
-        <v>140</v>
-      </c>
-      <c r="F362" s="7"/>
+        <v>171</v>
+      </c>
     </row>
     <row r="363" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E363" t="s">
-        <v>141</v>
-      </c>
-      <c r="F363" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="F363" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="364" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E364" t="s">
+        <v>139</v>
+      </c>
+      <c r="F364" s="7"/>
+    </row>
+    <row r="365" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E365" t="s">
+        <v>140</v>
+      </c>
+      <c r="F365" s="7"/>
+    </row>
+    <row r="366" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E366" t="s">
+        <v>141</v>
+      </c>
+      <c r="F366" s="7"/>
+    </row>
+    <row r="367" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E367" t="s">
         <v>142</v>
       </c>
-      <c r="F364" s="7"/>
-    </row>
-    <row r="367" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C367" s="2" t="s">
+      <c r="F367" s="7"/>
+    </row>
+    <row r="370" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C370" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D367" s="2"/>
-      <c r="E367" s="2"/>
-      <c r="F367" s="2"/>
-      <c r="G367" s="2"/>
-    </row>
-    <row r="368" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="369" spans="4:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D369" s="3" t="s">
+      <c r="D370" s="2"/>
+      <c r="E370" s="2"/>
+      <c r="F370" s="2"/>
+      <c r="G370" s="2"/>
+    </row>
+    <row r="371" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="372" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D372" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E369" s="3"/>
-      <c r="F369" s="3"/>
-      <c r="G369" s="3"/>
-    </row>
-    <row r="370" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E370" t="s">
+      <c r="E372" s="3"/>
+      <c r="F372" s="3"/>
+      <c r="G372" s="3"/>
+    </row>
+    <row r="373" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E373" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="371" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E371" t="s">
+    <row r="374" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E374" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="372" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E372" s="8" t="s">
+    <row r="375" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E375" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="F372" s="7"/>
-    </row>
-    <row r="373" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E373" s="8" t="s">
+      <c r="F375" s="7"/>
+    </row>
+    <row r="376" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E376" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F373" s="7"/>
-    </row>
-    <row r="374" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E374" t="s">
+      <c r="F376" s="7"/>
+    </row>
+    <row r="377" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E377" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="375" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E375" s="8" t="s">
+    <row r="378" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E378" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="F375" s="7"/>
-    </row>
-    <row r="376" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E376" s="8" t="s">
+      <c r="F378" s="7"/>
+    </row>
+    <row r="379" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E379" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="F376" s="7"/>
-    </row>
-    <row r="377" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E377" s="8" t="s">
+      <c r="F379" s="7"/>
+    </row>
+    <row r="380" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E380" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="F377" s="7"/>
-    </row>
-    <row r="378" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E378" s="8" t="s">
+      <c r="F380" s="7"/>
+    </row>
+    <row r="381" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E381" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="F378" s="7"/>
-    </row>
-    <row r="380" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E380" t="s">
+      <c r="F381" s="7"/>
+    </row>
+    <row r="383" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E383" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="381" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E381" s="7"/>
-    </row>
-    <row r="382" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E382" t="s">
+    <row r="384" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E384" s="7"/>
+    </row>
+    <row r="385" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E385" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="383" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E383" s="7"/>
-    </row>
-    <row r="384" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="E384" t="s">
+    <row r="386" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E386" s="7"/>
+    </row>
+    <row r="387" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E387" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="385" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E385" s="7"/>
+    <row r="388" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E388" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="E108:F108"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23 E66 E58" xr:uid="{3C594C12-590A-7343-A03C-F6F925CF2C6D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26 E69 E61" xr:uid="{3C594C12-590A-7343-A03C-F6F925CF2C6D}">
       <formula1>YesNoPartial</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E39 E48 E89 E104 E106 E108 E112 E114 E120 E128 E130 E132 E134 E138 E144 E146 E148 E150 E156 E162 E166 E172 E174 F179:F184 E190 E192 E194 E196 E200 E202 E210 E212 E236 E234 E242 E244 E238 E230 E226 E222 E218 E252 E264 E287 E289 E291 E295 E297 E299 E301 E307 E309 E313 E315 E317 E321 E325 E329 E334 F361:F364 F372:F373 F375:F378 E381 E383 E385 E45 E85 E87 F95:F100 E125" xr:uid="{4BED4D73-49DB-8D4A-8D1E-63B573D30EBF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E42 E51 E92 E107 E109 E111 E115 E117 E123 E131 E133 E135 E137 E141 E147 E149 E151 E153 E159 E165 E169 E175 E177 F182:F187 E193 E195 E197 E199 E203 E205 E213 E215 E239 E237 E245 E247 E241 E233 E229 E225 E221 E255 E267 E290 E292 E294 E298 E300 E302 E304 E310 E312 E316 E318 E320 E324 E328 E332 E337 F364:F367 F375:F376 F378:F381 E384 E386 E388 E48 E88 E90 F98:F103 E128" xr:uid="{4BED4D73-49DB-8D4A-8D1E-63B573D30EBF}">
       <formula1>YesNo</formula1>
     </dataValidation>
   </dataValidations>
@@ -5640,30 +5652,30 @@
     </row>
     <row r="3" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="23" t="s">
-        <v>405</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="C4" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
     </row>
     <row r="9" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
@@ -5676,7 +5688,7 @@
     <row r="10" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -5693,19 +5705,19 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E15" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.2">
@@ -5715,12 +5727,12 @@
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E21" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.2">
@@ -5730,12 +5742,12 @@
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E25" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.2">
@@ -5745,12 +5757,12 @@
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E29" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.2">
@@ -5760,12 +5772,12 @@
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E33" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
@@ -5775,12 +5787,12 @@
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E37" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E39" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
@@ -5790,12 +5802,12 @@
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E41" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E43" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.2">
@@ -5805,19 +5817,19 @@
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E45" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D47" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E49" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="50" spans="5:5" x14ac:dyDescent="0.2">
@@ -5827,12 +5839,12 @@
     </row>
     <row r="51" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E51" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E53" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.2">
@@ -5842,12 +5854,12 @@
     </row>
     <row r="55" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E55" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="57" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E57" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="58" spans="5:5" x14ac:dyDescent="0.2">
@@ -5857,12 +5869,12 @@
     </row>
     <row r="59" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E59" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="61" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E61" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="62" spans="5:5" x14ac:dyDescent="0.2">
@@ -5872,7 +5884,7 @@
     </row>
     <row r="63" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E63" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="66" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -5886,14 +5898,14 @@
     <row r="67" spans="3:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="68" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D68" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E70" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.2">
@@ -5901,7 +5913,7 @@
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E72" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="75" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -5915,22 +5927,22 @@
     <row r="76" spans="3:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D77" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E79" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E80" s="25"/>
+      <c r="E80" s="14"/>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E81" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -6004,22 +6016,22 @@
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added duplicate ID check
</commit_message>
<xml_diff>
--- a/assets/AzureADAssessment-Interview.xlsx
+++ b/assets/AzureADAssessment-Interview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Documents/GitHub/AzureADAssessment/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A013EBA9-FC02-E547-8E12-E12B675E9FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86BC7AE-0A5A-D94C-919D-3043CE25A817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="1" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
   </bookViews>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="423">
   <si>
     <t>Identity Management</t>
   </si>
@@ -3817,8 +3817,8 @@
   </sheetPr>
   <dimension ref="B2:G388"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A123" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4471,7 +4471,9 @@
       </c>
     </row>
     <row r="141" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E141" s="7"/>
+      <c r="E141" s="7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="143" spans="3:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C143" s="2" t="s">

</xml_diff>

<commit_message>
Added app assignment checks
</commit_message>
<xml_diff>
--- a/assets/AzureADAssessment-Interview.xlsx
+++ b/assets/AzureADAssessment-Interview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Documents/GitHub/AzureADAssessment/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2101B15D-5CCE-2348-98D2-18A9BDFE1AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7500A3A-1C2B-9346-833C-15AB09D6D302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
   </bookViews>
@@ -43,6 +43,7 @@
     <definedName name="AccMgmt_Are_you_using_these_data_sources_for_support_and_troubleshooting_access_issues">'Interview Questions'!$E$247</definedName>
     <definedName name="AccMgmt_Ban_Weak_Passwords">'Interview Questions'!$F$100</definedName>
     <definedName name="AccMgmt_Detection_of_Leaked_Passwords">'Interview Questions'!$F$102</definedName>
+    <definedName name="AccMgmt_Did_you_find_applications_that_have_assignment_to_individual_groups">'Post-Interview Assessment'!$E$105</definedName>
     <definedName name="AccMgmt_Did_you_find_applications_that_have_assignment_to_individual_users">'Post-Interview Assessment'!$E$100</definedName>
     <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$229</definedName>
     <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$233</definedName>
@@ -160,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="436">
   <si>
     <t>Identity Management</t>
   </si>
@@ -1572,8 +1573,11 @@
     </r>
   </si>
   <si>
+    <t>Did you find that applications have assignment to groups and groups are managed by IT (as opposed to an access governance solution)?</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Did you find applications that have assignment to individual </t>
+      <t xml:space="preserve">Did you find applications that have assignment to </t>
     </r>
     <r>
       <rPr>
@@ -1597,9 +1601,6 @@
       </rPr>
       <t>, and there is no attestation / governance in place?</t>
     </r>
-  </si>
-  <si>
-    <t>Did you find that applications have assignment to groups and groups are managed by IT (as opposed to an access governance solution)?</t>
   </si>
 </sst>
 </file>
@@ -5763,8 +5764,8 @@
   </sheetPr>
   <dimension ref="B2:F112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A94" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6130,7 +6131,9 @@
       </c>
     </row>
     <row r="100" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E100" s="14"/>
+      <c r="E100" s="14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="101" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E101" s="13" t="s">
@@ -6144,11 +6147,13 @@
     </row>
     <row r="104" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E104" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="105" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E105" s="14"/>
+      <c r="E105" s="14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="106" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E106" s="13" t="s">
@@ -6162,11 +6167,13 @@
     </row>
     <row r="109" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E109" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="110" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E110" s="14"/>
+      <c r="E110" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="111" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E111" s="13" t="s">

</xml_diff>

<commit_message>
Added Trusted Networks checks
</commit_message>
<xml_diff>
--- a/assets/AzureADAssessment-Interview.xlsx
+++ b/assets/AzureADAssessment-Interview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Documents/GitHub/AzureADAssessment/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19739925-1603-B94B-9DB6-42AA403454B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1886BAE3-0C0C-0844-9B7A-1B6DDC46D6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{E37EFEB7-9F3A-5940-A041-8C77818D1C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Guided Walkthrough" sheetId="3" r:id="rId1"/>
@@ -45,6 +45,8 @@
     <definedName name="AccMgmt_Detection_of_Leaked_Passwords">'Interview Questions'!$F$102</definedName>
     <definedName name="AccMgmt_Did_you_find_applications_that_have_assignment_to_individual_groups">'Post-Interview Assessment'!$E$105</definedName>
     <definedName name="AccMgmt_Did_you_find_applications_that_have_assignment_to_individual_users">'Post-Interview Assessment'!$E$100</definedName>
+    <definedName name="AccMgmt_Did_you_find_customer_is_federated_does_not_use_insideCorporateNetwork_claim_but_there_are_no_trusted_networks_defined">'Post-Interview Assessment'!$E$118</definedName>
+    <definedName name="AccMgmt_Did_you_find_customer_is_federated_uses_insideCorporateNetwork_claim_there_are_no_trusted_networks_defined">'Post-Interview Assessment'!$E$121</definedName>
     <definedName name="AccMgmt_Do_you_archive_Azure_AD_Audits">'Interview Questions'!$E$235</definedName>
     <definedName name="AccMgmt_Do_you_archive_Azure_AD_Risk_Events">'Interview Questions'!$E$239</definedName>
     <definedName name="AccMgmt_Do_you_archive_Azure_AD_Sign_in_Activity_Logs">'Interview Questions'!$E$231</definedName>
@@ -76,6 +78,7 @@
     <definedName name="AccMgmt_Have_you_enabled_Password_Hash_Sync">'Interview Questions'!$E$115</definedName>
     <definedName name="AccMgmt_Have_you_explicitly_identified_regions_where_authentication_should_NOT_be_coming_from">'Interview Questions'!$E$211</definedName>
     <definedName name="AccMgmt_Have_you_identified_the_regions_of_the_world_where_authentication_traffic_should_be_coming_from">'Interview Questions'!$E$209</definedName>
+    <definedName name="AccMgmt_If_customer_is_federated_is_the_insideCorporateNetwork_claim_included_by_the_federated_identity_provider">'Interview Questions'!$E$175</definedName>
     <definedName name="AccMgmt_If_so__do_you_use_password_vaulting_with_these_apps">'Interview Questions'!$E$153</definedName>
     <definedName name="AccMgmt_If_so_does_your_operations_team_use_it_regularly_to_understand_Azure_AD_usage">'Interview Questions'!$E$221</definedName>
     <definedName name="AccMgmt_If_yes__is_this_using_Azure_AD_s_self_service_password_reset_solution">'Interview Questions'!$E$90</definedName>
@@ -113,7 +116,8 @@
     <definedName name="Gov_If_not_what_is_the_strategy_to_clean_up_remove_access">'Interview Questions'!$E$328</definedName>
     <definedName name="Gov_If_so_how_do_establish_ownership_of_those_accounts">'Interview Questions'!$E$332</definedName>
     <definedName name="Gov_Is_there_any_global_admin_outside_the_IAM_team">'Interview Questions'!$E$334</definedName>
-    <definedName name="GW_AADConnectHealth">'Guided Walkthrough'!$E$268</definedName>
+    <definedName name="GW_AADConnectHealth">'Guided Walkthrough'!$E$271</definedName>
+    <definedName name="GW_AADConnectSettings">'Guided Walkthrough'!$E$124</definedName>
     <definedName name="IdMgmt_Do_you_have_a_disaster_recovery_production_instance_of_AAD_Connect_deployed_in_Staging_Mode">'Interview Questions'!$E$48</definedName>
     <definedName name="IdMgmt_Do_you_have_owners_defined_for_the_following_tasks_in_your_organization">'Interview Questions'!$E$26</definedName>
     <definedName name="IdMgmt_Do_you_synchronize_the_same_forest_where_users_log_in_to_their_Windows_devices">'Interview Questions'!$E$42</definedName>
@@ -138,6 +142,8 @@
     <definedName name="Ops_Secured_Pass_through_Authentication_Agent">'Interview Questions'!$F$386</definedName>
     <definedName name="Ops_Secured_SQL_Server_for_ADFS">'Interview Questions'!$F$384</definedName>
     <definedName name="Ops_Secured_SQL_Server_for_Azure_AD_Connect">'Interview Questions'!$F$382</definedName>
+    <definedName name="Sec_Do_you_still_have_trusted_IPs_within_MFA_old_config">'Guided Walkthrough'!$G$166</definedName>
+    <definedName name="Sec_Is_Allow_users_to_remember_multi_factor_authentication_on_devices_they_trust_enabled">'Guided Walkthrough'!$G$169</definedName>
     <definedName name="YesNo">Lookups!$B$9:$B$11</definedName>
     <definedName name="YesNoPartial">Lookups!$B$3:$B$6</definedName>
   </definedNames>
@@ -161,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="446">
   <si>
     <t>Identity Management</t>
   </si>
@@ -908,9 +914,6 @@
   </si>
   <si>
     <t>How did you determine the IP Address ranges on name locations?</t>
-  </si>
-  <si>
-    <t>Do you still have trusted IPs within MFA old config experience? If so, why?</t>
   </si>
   <si>
     <t xml:space="preserve">Authentication methods - Policies </t>
@@ -1594,12 +1597,54 @@
 Note: If a question does not apply to the customer's environment or their scenario, answer them as 'Not Applicable' to exclude the check.</t>
     </r>
   </si>
+  <si>
+    <t>Contoso</t>
+  </si>
+  <si>
+    <t>00000-00000-00000-000</t>
+  </si>
+  <si>
+    <t>Contoso Admin</t>
+  </si>
+  <si>
+    <t>GTP Assessor</t>
+  </si>
+  <si>
+    <t>23 Nov 2021</t>
+  </si>
+  <si>
+    <t>Guided Walkthrough - AAD Connect Settings</t>
+  </si>
+  <si>
+    <t>Did you find customer is federated &amp; does not use "insideCorporateNetwork" claim &amp; there are no trusted networks defined?</t>
+  </si>
+  <si>
+    <t>Q. insideCorporateNetwork claim</t>
+  </si>
+  <si>
+    <t>AR0002 - Trusted Networks not defined (Generate report to see result)</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>Do you still have trusted IPs within MFA old config experience? (AAD Portal &gt; Users &gt; Per-user MFA &gt; Service Settings)</t>
+  </si>
+  <si>
+    <t>Is 'Allow users to remember multi-factor authentication on devices they trust' enabled? (AAD Portal &gt; Users &gt; Per-user MFA &gt; Service Settings)</t>
+  </si>
+  <si>
+    <t>Did you find customer is federated &amp; uses "insideCorporateNetwork" claim &amp; there are no trusted networks defined?</t>
+  </si>
+  <si>
+    <t>Answer as 'Not Applicable' if not federated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1688,6 +1733,27 @@
       <b/>
       <i/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1818,7 +1884,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
@@ -1837,6 +1903,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1852,6 +1919,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
@@ -2263,10 +2332,10 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A2:N300"/>
+  <dimension ref="A2:N303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:N7"/>
+    <sheetView showGridLines="0" topLeftCell="A144" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G166" sqref="G166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2299,62 +2368,62 @@
     </row>
     <row r="3" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="16" t="s">
-        <v>432</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>431</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
     </row>
     <row r="9" spans="2:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
@@ -2572,7 +2641,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E56" s="11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -2587,7 +2656,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F60" s="11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
@@ -2657,7 +2726,7 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E75" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -2672,7 +2741,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F78" s="11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -2692,7 +2761,7 @@
     </row>
     <row r="82" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F82" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="84" spans="5:14" x14ac:dyDescent="0.2">
@@ -2702,7 +2771,7 @@
     </row>
     <row r="85" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F85" s="11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="86" spans="5:14" x14ac:dyDescent="0.2">
@@ -2717,7 +2786,7 @@
     </row>
     <row r="88" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F88" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="89" spans="5:14" x14ac:dyDescent="0.2">
@@ -2732,7 +2801,7 @@
     </row>
     <row r="91" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F91" s="11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="93" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2751,7 +2820,7 @@
     </row>
     <row r="94" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E94" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="95" spans="5:14" x14ac:dyDescent="0.2">
@@ -2775,7 +2844,7 @@
     </row>
     <row r="97" spans="5:7" x14ac:dyDescent="0.2">
       <c r="F97" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="98" spans="5:7" x14ac:dyDescent="0.2">
@@ -2783,12 +2852,12 @@
         <v>131</v>
       </c>
       <c r="F98" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="100" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G100" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="101" spans="5:7" x14ac:dyDescent="0.2">
@@ -2796,7 +2865,7 @@
     </row>
     <row r="102" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G102" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="103" spans="5:7" x14ac:dyDescent="0.2">
@@ -2804,7 +2873,7 @@
     </row>
     <row r="104" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G104" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="105" spans="5:7" x14ac:dyDescent="0.2">
@@ -2815,7 +2884,7 @@
     </row>
     <row r="107" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G107" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="108" spans="5:7" x14ac:dyDescent="0.2">
@@ -2826,7 +2895,7 @@
     </row>
     <row r="110" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G110" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="111" spans="5:7" x14ac:dyDescent="0.2">
@@ -2837,7 +2906,7 @@
     </row>
     <row r="113" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G113" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="114" spans="5:14" x14ac:dyDescent="0.2">
@@ -2848,7 +2917,7 @@
     </row>
     <row r="116" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G116" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="117" spans="5:14" x14ac:dyDescent="0.2">
@@ -2856,17 +2925,17 @@
     </row>
     <row r="118" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G118" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="119" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G119" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="120" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G120" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="123" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3033,7 +3102,7 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E151" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
@@ -3045,12 +3114,15 @@
       <c r="A154" t="s">
         <v>131</v>
       </c>
-      <c r="G154" s="7"/>
+      <c r="G154" s="5"/>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G156" t="s">
         <v>246</v>
       </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G157" s="7"/>
     </row>
     <row r="159" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E159" s="3" t="s">
@@ -3068,7 +3140,7 @@
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E160" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="161" spans="5:14" x14ac:dyDescent="0.2">
@@ -3086,54 +3158,51 @@
     </row>
     <row r="165" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G165" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="166" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="G166" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="G168" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="169" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="G169" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E171" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="166" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="G166" s="7"/>
-    </row>
-    <row r="168" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E168" s="3" t="s">
+      <c r="F171" s="3"/>
+      <c r="G171" s="3"/>
+      <c r="H171" s="3"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="3"/>
+      <c r="K171" s="3"/>
+      <c r="L171" s="3"/>
+      <c r="M171" s="3"/>
+      <c r="N171" s="3"/>
+    </row>
+    <row r="172" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E172" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="F168" s="3"/>
-      <c r="G168" s="3"/>
-      <c r="H168" s="3"/>
-      <c r="I168" s="3"/>
-      <c r="J168" s="3"/>
-      <c r="K168" s="3"/>
-      <c r="L168" s="3"/>
-      <c r="M168" s="3"/>
-      <c r="N168" s="3"/>
-    </row>
-    <row r="169" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E169" s="11" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="170" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E170" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="171" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F171" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="172" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F172" s="11" t="s">
-        <v>332</v>
-      </c>
     </row>
     <row r="173" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F173" t="s">
+      <c r="E173" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="174" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F174" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="175" spans="5:14" x14ac:dyDescent="0.2">
@@ -3142,28 +3211,28 @@
       </c>
     </row>
     <row r="176" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="G176" t="s">
+      <c r="F176" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="177" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F177" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="178" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F178" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="179" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="G179" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="180" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="G180" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="177" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="G177" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="178" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F178" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="179" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F179" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="180" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F180" s="11" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="181" spans="5:14" x14ac:dyDescent="0.2">
@@ -3173,7 +3242,7 @@
     </row>
     <row r="182" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F182" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="183" spans="5:14" x14ac:dyDescent="0.2">
@@ -3188,7 +3257,7 @@
     </row>
     <row r="185" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F185" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="186" spans="5:14" x14ac:dyDescent="0.2">
@@ -3197,37 +3266,28 @@
       </c>
     </row>
     <row r="187" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E187" t="s">
+      <c r="F187" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="189" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E189" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F189" s="3"/>
-      <c r="G189" s="3"/>
-      <c r="H189" s="3"/>
-      <c r="I189" s="3"/>
-      <c r="J189" s="3"/>
-      <c r="K189" s="3"/>
-      <c r="L189" s="3"/>
-      <c r="M189" s="3"/>
-      <c r="N189" s="3"/>
+    <row r="188" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F188" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="189" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F189" s="11" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="190" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E190" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="191" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E191" t="s">
+      <c r="E190" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="192" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E192" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F192" s="3"/>
       <c r="G192" s="3"/>
@@ -3241,20 +3301,36 @@
     </row>
     <row r="193" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E193" s="11" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="195" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="G195" t="s">
-        <v>262</v>
-      </c>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="194" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E194" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="195" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E195" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F195" s="3"/>
+      <c r="G195" s="3"/>
+      <c r="H195" s="3"/>
+      <c r="I195" s="3"/>
+      <c r="J195" s="3"/>
+      <c r="K195" s="3"/>
+      <c r="L195" s="3"/>
+      <c r="M195" s="3"/>
+      <c r="N195" s="3"/>
     </row>
     <row r="196" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="G196" s="7"/>
+      <c r="E196" s="11" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="198" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G198" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="199" spans="5:14" x14ac:dyDescent="0.2">
@@ -3262,54 +3338,47 @@
     </row>
     <row r="201" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G201" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="202" spans="5:14" x14ac:dyDescent="0.2">
       <c r="G202" s="7"/>
     </row>
-    <row r="204" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E204" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="F204" s="3"/>
-      <c r="G204" s="3"/>
-      <c r="H204" s="3"/>
-      <c r="I204" s="3"/>
-      <c r="J204" s="3"/>
-      <c r="K204" s="3"/>
-      <c r="L204" s="3"/>
-      <c r="M204" s="3"/>
-      <c r="N204" s="3"/>
+    <row r="204" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="G204" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="205" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E205" s="11" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="207" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E207" t="s">
-        <v>267</v>
-      </c>
+      <c r="G205" s="7"/>
+    </row>
+    <row r="207" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E207" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F207" s="3"/>
+      <c r="G207" s="3"/>
+      <c r="H207" s="3"/>
+      <c r="I207" s="3"/>
+      <c r="J207" s="3"/>
+      <c r="K207" s="3"/>
+      <c r="L207" s="3"/>
+      <c r="M207" s="3"/>
+      <c r="N207" s="3"/>
     </row>
     <row r="208" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E208" s="11" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="209" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E209" t="s">
-        <v>131</v>
+        <v>265</v>
       </c>
     </row>
     <row r="210" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E210" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="211" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E211" s="11" t="s">
-        <v>269</v>
+        <v>325</v>
       </c>
     </row>
     <row r="212" spans="5:14" x14ac:dyDescent="0.2">
@@ -3317,33 +3386,38 @@
         <v>131</v>
       </c>
     </row>
-    <row r="213" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E213" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="F213" s="3"/>
-      <c r="G213" s="3"/>
-      <c r="H213" s="3"/>
-      <c r="I213" s="3"/>
-      <c r="J213" s="3"/>
-      <c r="K213" s="3"/>
-      <c r="L213" s="3"/>
-      <c r="M213" s="3"/>
-      <c r="N213" s="3"/>
+    <row r="213" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E213" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="214" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F214" t="s">
-        <v>271</v>
+      <c r="E214" s="11" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="215" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F215" s="11" t="s">
-        <v>325</v>
-      </c>
+      <c r="E215" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="216" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E216" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="F216" s="3"/>
+      <c r="G216" s="3"/>
+      <c r="H216" s="3"/>
+      <c r="I216" s="3"/>
+      <c r="J216" s="3"/>
+      <c r="K216" s="3"/>
+      <c r="L216" s="3"/>
+      <c r="M216" s="3"/>
+      <c r="N216" s="3"/>
     </row>
     <row r="217" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F217" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="218" spans="5:14" x14ac:dyDescent="0.2">
@@ -3351,14 +3425,9 @@
         <v>324</v>
       </c>
     </row>
-    <row r="219" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F219" t="s">
-        <v>131</v>
-      </c>
-    </row>
     <row r="220" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F220" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="221" spans="5:14" x14ac:dyDescent="0.2">
@@ -3366,9 +3435,14 @@
         <v>323</v>
       </c>
     </row>
+    <row r="222" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F222" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="223" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F223" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="224" spans="5:14" x14ac:dyDescent="0.2">
@@ -3378,7 +3452,7 @@
     </row>
     <row r="226" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F226" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="227" spans="5:14" x14ac:dyDescent="0.2">
@@ -3386,14 +3460,9 @@
         <v>321</v>
       </c>
     </row>
-    <row r="228" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E228" t="s">
-        <v>131</v>
-      </c>
-    </row>
     <row r="229" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F229" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="230" spans="5:14" x14ac:dyDescent="0.2">
@@ -3406,38 +3475,38 @@
         <v>131</v>
       </c>
     </row>
-    <row r="232" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E232" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="F232" s="3"/>
-      <c r="G232" s="3"/>
-      <c r="H232" s="3"/>
-      <c r="I232" s="3"/>
-      <c r="J232" s="3"/>
-      <c r="K232" s="3"/>
-      <c r="L232" s="3"/>
-      <c r="M232" s="3"/>
-      <c r="N232" s="3"/>
+    <row r="232" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F232" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="233" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F233" t="s">
-        <v>278</v>
+      <c r="F233" s="11" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="234" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F234" s="11" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="235" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F235" t="s">
+      <c r="E234" t="s">
         <v>131</v>
       </c>
+    </row>
+    <row r="235" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E235" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F235" s="3"/>
+      <c r="G235" s="3"/>
+      <c r="H235" s="3"/>
+      <c r="I235" s="3"/>
+      <c r="J235" s="3"/>
+      <c r="K235" s="3"/>
+      <c r="L235" s="3"/>
+      <c r="M235" s="3"/>
+      <c r="N235" s="3"/>
     </row>
     <row r="236" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F236" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="237" spans="5:14" x14ac:dyDescent="0.2">
@@ -3452,7 +3521,7 @@
     </row>
     <row r="239" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F239" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="240" spans="5:14" x14ac:dyDescent="0.2">
@@ -3467,7 +3536,7 @@
     </row>
     <row r="242" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F242" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="243" spans="6:6" x14ac:dyDescent="0.2">
@@ -3482,7 +3551,7 @@
     </row>
     <row r="245" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F245" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="246" spans="6:6" x14ac:dyDescent="0.2">
@@ -3497,7 +3566,7 @@
     </row>
     <row r="248" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F248" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="249" spans="6:6" x14ac:dyDescent="0.2">
@@ -3512,7 +3581,7 @@
     </row>
     <row r="251" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F251" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="252" spans="6:6" x14ac:dyDescent="0.2">
@@ -3527,7 +3596,7 @@
     </row>
     <row r="254" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F254" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="255" spans="6:6" x14ac:dyDescent="0.2">
@@ -3540,19 +3609,24 @@
         <v>131</v>
       </c>
     </row>
+    <row r="257" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F257" t="s">
+        <v>284</v>
+      </c>
+    </row>
     <row r="258" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F258" t="s">
-        <v>299</v>
+      <c r="F258" s="11" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="259" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F259" s="11" t="s">
-        <v>302</v>
+      <c r="F259" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="261" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F261" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="262" spans="5:14" x14ac:dyDescent="0.2">
@@ -3562,59 +3636,54 @@
     </row>
     <row r="264" spans="5:14" x14ac:dyDescent="0.2">
       <c r="F264" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="265" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F265" s="11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="267" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="F267" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="268" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E268" t="s">
+        <v>131</v>
+      </c>
+      <c r="F268" s="11" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="265" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E265" t="s">
-        <v>131</v>
-      </c>
-      <c r="F265" s="11" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="267" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E267" t="s">
+    <row r="270" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E270" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="271" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E271" s="3" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="268" spans="5:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E268" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="F268" s="3"/>
-      <c r="G268" s="3"/>
-      <c r="H268" s="3"/>
-      <c r="I268" s="3"/>
-      <c r="J268" s="3"/>
-      <c r="K268" s="3"/>
-      <c r="L268" s="3"/>
-      <c r="M268" s="3"/>
-      <c r="N268" s="3"/>
-    </row>
-    <row r="270" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F270" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="271" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F271" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="272" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="F272" t="s">
-        <v>131</v>
-      </c>
+      <c r="F271" s="3"/>
+      <c r="G271" s="3"/>
+      <c r="H271" s="3"/>
+      <c r="I271" s="3"/>
+      <c r="J271" s="3"/>
+      <c r="K271" s="3"/>
+      <c r="L271" s="3"/>
+      <c r="M271" s="3"/>
+      <c r="N271" s="3"/>
     </row>
     <row r="273" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F273" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="274" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F274" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="275" spans="3:14" x14ac:dyDescent="0.2">
@@ -3624,12 +3693,12 @@
     </row>
     <row r="276" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F276" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="277" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F277" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="278" spans="3:14" x14ac:dyDescent="0.2">
@@ -3639,7 +3708,7 @@
     </row>
     <row r="279" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F279" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="280" spans="3:14" x14ac:dyDescent="0.2">
@@ -3654,7 +3723,7 @@
     </row>
     <row r="282" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F282" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="283" spans="3:14" x14ac:dyDescent="0.2">
@@ -3663,90 +3732,105 @@
       </c>
     </row>
     <row r="284" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="E284" t="s">
+      <c r="F284" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="285" spans="3:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C285" s="1" t="s">
+    <row r="285" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F285" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="286" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F286" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="287" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="E287" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="288" spans="3:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C288" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D288" s="1"/>
+      <c r="E288" s="1"/>
+      <c r="F288" s="1"/>
+      <c r="G288" s="1"/>
+      <c r="H288" s="1"/>
+      <c r="I288" s="1"/>
+      <c r="J288" s="1"/>
+      <c r="K288" s="1"/>
+      <c r="L288" s="1"/>
+      <c r="M288" s="1"/>
+      <c r="N288" s="1"/>
+    </row>
+    <row r="289" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="290" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D290" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D285" s="1"/>
-      <c r="E285" s="1"/>
-      <c r="F285" s="1"/>
-      <c r="G285" s="1"/>
-      <c r="H285" s="1"/>
-      <c r="I285" s="1"/>
-      <c r="J285" s="1"/>
-      <c r="K285" s="1"/>
-      <c r="L285" s="1"/>
-      <c r="M285" s="1"/>
-      <c r="N285" s="1"/>
-    </row>
-    <row r="286" spans="3:14" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="287" spans="3:14" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D287" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E287" s="2"/>
-      <c r="F287" s="2"/>
-      <c r="G287" s="2"/>
-      <c r="H287" s="2"/>
-      <c r="I287" s="2"/>
-      <c r="J287" s="2"/>
-      <c r="K287" s="2"/>
-      <c r="L287" s="2"/>
-      <c r="M287" s="2"/>
-      <c r="N287" s="2"/>
-    </row>
-    <row r="288" spans="3:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="E288" s="11" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E289" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E290" t="s">
-        <v>295</v>
+      <c r="E290" s="2"/>
+      <c r="F290" s="2"/>
+      <c r="G290" s="2"/>
+      <c r="H290" s="2"/>
+      <c r="I290" s="2"/>
+      <c r="J290" s="2"/>
+      <c r="K290" s="2"/>
+      <c r="L290" s="2"/>
+      <c r="M290" s="2"/>
+      <c r="N290" s="2"/>
+    </row>
+    <row r="291" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E291" s="11" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="292" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E292" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E293" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E295" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="293" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C293" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D293" s="1"/>
-      <c r="E293" s="1"/>
-      <c r="F293" s="1"/>
-      <c r="G293" s="1"/>
-      <c r="H293" s="1"/>
-      <c r="I293" s="1"/>
-      <c r="J293" s="1"/>
-      <c r="K293" s="1"/>
-      <c r="L293" s="1"/>
-      <c r="M293" s="1"/>
-      <c r="N293" s="1"/>
-    </row>
-    <row r="294" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="D294" s="11" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E296" t="s">
+    <row r="296" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C296" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D296" s="1"/>
+      <c r="E296" s="1"/>
+      <c r="F296" s="1"/>
+      <c r="G296" s="1"/>
+      <c r="H296" s="1"/>
+      <c r="I296" s="1"/>
+      <c r="J296" s="1"/>
+      <c r="K296" s="1"/>
+      <c r="L296" s="1"/>
+      <c r="M296" s="1"/>
+      <c r="N296" s="1"/>
+    </row>
+    <row r="297" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D297" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E299" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A300" t="s">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3755,7 +3839,7 @@
     <mergeCell ref="C4:N7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G101 G105 G108 G111 G114" xr:uid="{1357A57D-6496-CE42-A721-3AD1367F1890}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G101 G105 G108 G111 G114 G154 G166 G169" xr:uid="{1357A57D-6496-CE42-A721-3AD1367F1890}">
       <formula1>YesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G117" xr:uid="{0A5E8D50-E528-1F4C-B6E2-6D8BA756812E}">
@@ -3780,41 +3864,41 @@
     <hyperlink ref="F139" r:id="rId15" location="blade/Microsoft_AAD_IAM/PasswordResetMenuBlade/Notifications " xr:uid="{8FC84638-0F95-0E47-B0E4-93D45D5D5FE5}"/>
     <hyperlink ref="F142" r:id="rId16" location="blade/Microsoft_AAD_IAM/PasswordResetMenuBlade/Customization  " xr:uid="{187DCBC0-4EF3-F446-84E3-8756AFCC0E1E}"/>
     <hyperlink ref="F145" r:id="rId17" location="blade/Microsoft_AAD_IAM/PasswordResetMenuBlade/OnPremisesIntegration  " xr:uid="{5CA6319A-BEF2-8F4F-98D9-41662559338B}"/>
-    <hyperlink ref="F259" r:id="rId18" location="blade/Microsoft_Azure_PIMCommon/ResourceMenuBlade/RoleSettings/resourceId//resourceType/tenant/provider/aadroles" xr:uid="{2012D58F-22AD-AF46-9A4D-C285F9300E0E}"/>
-    <hyperlink ref="F262" r:id="rId19" location="blade/Microsoft_Azure_PIMCommon/CommonMenuBlade/aadgroup/defaultMenuId/quickStart" xr:uid="{13E00922-8D7B-AF40-99BD-0BD602571793}"/>
-    <hyperlink ref="F265" r:id="rId20" location="blade/Microsoft_Azure_PIMCommon/CommonMenuBlade/azurerbac/defaultMenuId/quickStart" xr:uid="{E9B56DE6-D6D3-7340-8122-26F3C3EF1F1D}"/>
-    <hyperlink ref="E288" r:id="rId21" location="/MessageCenter" xr:uid="{2055B6FE-FCDF-9145-8BDF-CF36F4B7BF27}"/>
-    <hyperlink ref="D294" r:id="rId22" xr:uid="{C68B5C4C-3245-A849-AD4F-EA6B887BD5B4}"/>
-    <hyperlink ref="F283" r:id="rId23" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/generalsettings" xr:uid="{59A00C21-BE37-034F-96CF-FC9EBAA579F9}"/>
-    <hyperlink ref="F280" r:id="rId24" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/AddsServicesList" xr:uid="{F216795B-BCD0-E047-A41A-7DB359FBAA69}"/>
-    <hyperlink ref="F277" r:id="rId25" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/AdfsServicesList" xr:uid="{1331F16E-95BC-2843-A25F-6793AC411F54}"/>
-    <hyperlink ref="F271" r:id="rId26" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/SyncErros" xr:uid="{0E751130-4C6F-0A47-AAAE-28DA8CAAA257}"/>
-    <hyperlink ref="F274" r:id="rId27" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/SyncServicesList" xr:uid="{9A5A8BFB-82B6-CA4B-A465-71B16CC89A80}"/>
-    <hyperlink ref="F255" r:id="rId28" location="blade/Microsoft_Azure_PIMCommon/ResourceMenuBlade/aaddiscovery/resourceId//resourceType/tenant/provider/aadroles" xr:uid="{81D328F7-1470-244C-A26F-9D767B205465}"/>
-    <hyperlink ref="F252" r:id="rId29" location="blade/Microsoft_Azure_PIMCommon/ResourceMenuBlade/Alerts/resourceId//resourceType/tenant/provider/aadroles" xr:uid="{FC1F49B5-6E6D-4243-BA34-6393ADFE9411}"/>
-    <hyperlink ref="F249" r:id="rId30" location="blade/Microsoft_Azure_PIMCommon/ResourceMenuBlade/aadoverview/resourceId//resourceType/tenant/provider/aadroles" xr:uid="{A3DB2DD6-BBEF-BA49-A6F7-A27B75FF34F3}"/>
-    <hyperlink ref="F246" r:id="rId31" location="blade/Microsoft_AAD_ERM/DashboardBlade/Settings" xr:uid="{9CF26E13-FD2B-394A-8692-FCF0ADA574CE}"/>
-    <hyperlink ref="F243" r:id="rId32" location="blade/Microsoft_AAD_ERM/DashboardBlade/Overview" xr:uid="{8B91AE52-6F81-3843-A662-F314438B00B8}"/>
-    <hyperlink ref="F240" r:id="rId33" location="blade/Microsoft_AAD_ERM/DashboardBlade/elmSetting" xr:uid="{AD44E3D2-0556-C447-9660-5D7B0EB44972}"/>
-    <hyperlink ref="F237" r:id="rId34" location="blade/Microsoft_AAD_ERM/DashboardBlade/elmOrganizations" xr:uid="{56E3AE82-BE4E-0645-99AF-129FDD1545C6}"/>
-    <hyperlink ref="F234" r:id="rId35" location="blade/Microsoft_AAD_ERM/DashboardBlade/elmEntitlement" xr:uid="{7A571AA8-DBD9-5742-B9C1-9FE58D94EE62}"/>
-    <hyperlink ref="F230" r:id="rId36" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/WeeklyDigest" xr:uid="{C3E16DE5-8101-3141-A021-4E4A9C522CE5}"/>
-    <hyperlink ref="F227" r:id="rId37" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/UsersAtRiskAlerts" xr:uid="{568017BE-0A8B-1B48-86A3-57AA1FD3F377}"/>
-    <hyperlink ref="F224" r:id="rId38" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/MfaPolicy" xr:uid="{6FD25154-499E-8543-BEA5-690A03FADF79}"/>
-    <hyperlink ref="F221" r:id="rId39" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/SignInPolicy" xr:uid="{8F094B94-F2CB-DB4A-9401-7FB09E3F2DEA}"/>
-    <hyperlink ref="F218" r:id="rId40" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/UserPolicy" xr:uid="{FFBB5492-CEF3-3D4D-B8A2-B28F5B7BBF70}"/>
-    <hyperlink ref="F215" r:id="rId41" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/Overview" xr:uid="{C569830E-B67D-E14E-91FD-A19A53953EAC}"/>
-    <hyperlink ref="E211" r:id="rId42" location="blade/Microsoft_AAD_IAM/SecurityMenuBlade/RiskDetections" xr:uid="{BA718EB3-873E-F343-9E2A-7A5FCB72815F}"/>
-    <hyperlink ref="E208" r:id="rId43" location="blade/Microsoft_AAD_IAM/SecurityMenuBlade/RiskySignIns" xr:uid="{14F22F39-144A-7646-A9DC-60FC7C4CBB0F}"/>
-    <hyperlink ref="E205" r:id="rId44" location="blade/Microsoft_AAD_IAM/SecurityMenuBlade/RiskyUsers" xr:uid="{6588066C-8F2F-2141-AF1D-024B8DE236D1}"/>
-    <hyperlink ref="E193" r:id="rId45" location="blade/Microsoft_AAD_IAM/SecurityMenuBlade/ContinuousAccessEvaluation" xr:uid="{3782CD31-C4AD-914B-9EDC-183D018DE53C}"/>
-    <hyperlink ref="E190" r:id="rId46" location="blade/Microsoft_AAD_IAM/ConditionalAccessBlade/ClassicPolicies" xr:uid="{94ABCA99-15B2-FC46-8A90-B5C0322F6EC8}"/>
-    <hyperlink ref="F186" r:id="rId47" location="blade/Microsoft_AAD_IAM/MultifactorAuthenticationMenuBlade/PhoneCallSettings/fromProviders/" xr:uid="{2C329035-9803-2E41-BDEC-F95F78CF0FF9}"/>
-    <hyperlink ref="F183" r:id="rId48" location="blade/Microsoft_AAD_IAM/MultifactorAuthenticationMenuBlade/FraudAlert/fromProviders/" xr:uid="{C27FD6EE-6C39-9F46-B08C-FAAE7918BEF9}"/>
-    <hyperlink ref="F180" r:id="rId49" location="blade/Microsoft_AAD_IAM/MultifactorAuthenticationMenuBlade/BlockedUsers/fromProviders/" xr:uid="{A90D1099-A558-1642-A1BB-8E1BFB561408}"/>
-    <hyperlink ref="F175" r:id="rId50" location="blade/Microsoft_AAD_IAM/AuthenticationMethodsMenuBlade/AuthMethodsActivity" xr:uid="{54B2C85A-2E55-B144-B2B1-9BF20974A183}"/>
-    <hyperlink ref="E169" r:id="rId51" location="blade/Microsoft_AAD_IAM/AuthenticationMethodsMenuBlade/AdminAuthMethods" xr:uid="{940FFEB1-FA03-5F4E-9118-65B4CE2A9D98}"/>
-    <hyperlink ref="F172" r:id="rId52" location="blade/Microsoft_AAD_IAM/AuthenticationMethodsMenuBlade/PasswordProtection" xr:uid="{FA0B10A3-ECF8-D340-999A-ED47C61BB080}"/>
+    <hyperlink ref="F262" r:id="rId18" location="blade/Microsoft_Azure_PIMCommon/ResourceMenuBlade/RoleSettings/resourceId//resourceType/tenant/provider/aadroles" xr:uid="{2012D58F-22AD-AF46-9A4D-C285F9300E0E}"/>
+    <hyperlink ref="F265" r:id="rId19" location="blade/Microsoft_Azure_PIMCommon/CommonMenuBlade/aadgroup/defaultMenuId/quickStart" xr:uid="{13E00922-8D7B-AF40-99BD-0BD602571793}"/>
+    <hyperlink ref="F268" r:id="rId20" location="blade/Microsoft_Azure_PIMCommon/CommonMenuBlade/azurerbac/defaultMenuId/quickStart" xr:uid="{E9B56DE6-D6D3-7340-8122-26F3C3EF1F1D}"/>
+    <hyperlink ref="E291" r:id="rId21" location="/MessageCenter" xr:uid="{2055B6FE-FCDF-9145-8BDF-CF36F4B7BF27}"/>
+    <hyperlink ref="D297" r:id="rId22" xr:uid="{C68B5C4C-3245-A849-AD4F-EA6B887BD5B4}"/>
+    <hyperlink ref="F286" r:id="rId23" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/generalsettings" xr:uid="{59A00C21-BE37-034F-96CF-FC9EBAA579F9}"/>
+    <hyperlink ref="F283" r:id="rId24" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/AddsServicesList" xr:uid="{F216795B-BCD0-E047-A41A-7DB359FBAA69}"/>
+    <hyperlink ref="F280" r:id="rId25" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/AdfsServicesList" xr:uid="{1331F16E-95BC-2843-A25F-6793AC411F54}"/>
+    <hyperlink ref="F274" r:id="rId26" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/SyncErros" xr:uid="{0E751130-4C6F-0A47-AAAE-28DA8CAAA257}"/>
+    <hyperlink ref="F277" r:id="rId27" location="blade/Microsoft_Azure_ADHybridHealth/AadHealthMenuBlade/SyncServicesList" xr:uid="{9A5A8BFB-82B6-CA4B-A465-71B16CC89A80}"/>
+    <hyperlink ref="F258" r:id="rId28" location="blade/Microsoft_Azure_PIMCommon/ResourceMenuBlade/aaddiscovery/resourceId//resourceType/tenant/provider/aadroles" xr:uid="{81D328F7-1470-244C-A26F-9D767B205465}"/>
+    <hyperlink ref="F255" r:id="rId29" location="blade/Microsoft_Azure_PIMCommon/ResourceMenuBlade/Alerts/resourceId//resourceType/tenant/provider/aadroles" xr:uid="{FC1F49B5-6E6D-4243-BA34-6393ADFE9411}"/>
+    <hyperlink ref="F252" r:id="rId30" location="blade/Microsoft_Azure_PIMCommon/ResourceMenuBlade/aadoverview/resourceId//resourceType/tenant/provider/aadroles" xr:uid="{A3DB2DD6-BBEF-BA49-A6F7-A27B75FF34F3}"/>
+    <hyperlink ref="F249" r:id="rId31" location="blade/Microsoft_AAD_ERM/DashboardBlade/Settings" xr:uid="{9CF26E13-FD2B-394A-8692-FCF0ADA574CE}"/>
+    <hyperlink ref="F246" r:id="rId32" location="blade/Microsoft_AAD_ERM/DashboardBlade/Overview" xr:uid="{8B91AE52-6F81-3843-A662-F314438B00B8}"/>
+    <hyperlink ref="F243" r:id="rId33" location="blade/Microsoft_AAD_ERM/DashboardBlade/elmSetting" xr:uid="{AD44E3D2-0556-C447-9660-5D7B0EB44972}"/>
+    <hyperlink ref="F240" r:id="rId34" location="blade/Microsoft_AAD_ERM/DashboardBlade/elmOrganizations" xr:uid="{56E3AE82-BE4E-0645-99AF-129FDD1545C6}"/>
+    <hyperlink ref="F237" r:id="rId35" location="blade/Microsoft_AAD_ERM/DashboardBlade/elmEntitlement" xr:uid="{7A571AA8-DBD9-5742-B9C1-9FE58D94EE62}"/>
+    <hyperlink ref="F233" r:id="rId36" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/WeeklyDigest" xr:uid="{C3E16DE5-8101-3141-A021-4E4A9C522CE5}"/>
+    <hyperlink ref="F230" r:id="rId37" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/UsersAtRiskAlerts" xr:uid="{568017BE-0A8B-1B48-86A3-57AA1FD3F377}"/>
+    <hyperlink ref="F227" r:id="rId38" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/MfaPolicy" xr:uid="{6FD25154-499E-8543-BEA5-690A03FADF79}"/>
+    <hyperlink ref="F224" r:id="rId39" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/SignInPolicy" xr:uid="{8F094B94-F2CB-DB4A-9401-7FB09E3F2DEA}"/>
+    <hyperlink ref="F221" r:id="rId40" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/UserPolicy" xr:uid="{FFBB5492-CEF3-3D4D-B8A2-B28F5B7BBF70}"/>
+    <hyperlink ref="F218" r:id="rId41" location="blade/Microsoft_AAD_IAM/IdentityProtectionMenuBlade/Overview" xr:uid="{C569830E-B67D-E14E-91FD-A19A53953EAC}"/>
+    <hyperlink ref="E214" r:id="rId42" location="blade/Microsoft_AAD_IAM/SecurityMenuBlade/RiskDetections" xr:uid="{BA718EB3-873E-F343-9E2A-7A5FCB72815F}"/>
+    <hyperlink ref="E211" r:id="rId43" location="blade/Microsoft_AAD_IAM/SecurityMenuBlade/RiskySignIns" xr:uid="{14F22F39-144A-7646-A9DC-60FC7C4CBB0F}"/>
+    <hyperlink ref="E208" r:id="rId44" location="blade/Microsoft_AAD_IAM/SecurityMenuBlade/RiskyUsers" xr:uid="{6588066C-8F2F-2141-AF1D-024B8DE236D1}"/>
+    <hyperlink ref="E196" r:id="rId45" location="blade/Microsoft_AAD_IAM/SecurityMenuBlade/ContinuousAccessEvaluation" xr:uid="{3782CD31-C4AD-914B-9EDC-183D018DE53C}"/>
+    <hyperlink ref="E193" r:id="rId46" location="blade/Microsoft_AAD_IAM/ConditionalAccessBlade/ClassicPolicies" xr:uid="{94ABCA99-15B2-FC46-8A90-B5C0322F6EC8}"/>
+    <hyperlink ref="F189" r:id="rId47" location="blade/Microsoft_AAD_IAM/MultifactorAuthenticationMenuBlade/PhoneCallSettings/fromProviders/" xr:uid="{2C329035-9803-2E41-BDEC-F95F78CF0FF9}"/>
+    <hyperlink ref="F186" r:id="rId48" location="blade/Microsoft_AAD_IAM/MultifactorAuthenticationMenuBlade/FraudAlert/fromProviders/" xr:uid="{C27FD6EE-6C39-9F46-B08C-FAAE7918BEF9}"/>
+    <hyperlink ref="F183" r:id="rId49" location="blade/Microsoft_AAD_IAM/MultifactorAuthenticationMenuBlade/BlockedUsers/fromProviders/" xr:uid="{A90D1099-A558-1642-A1BB-8E1BFB561408}"/>
+    <hyperlink ref="F178" r:id="rId50" location="blade/Microsoft_AAD_IAM/AuthenticationMethodsMenuBlade/AuthMethodsActivity" xr:uid="{54B2C85A-2E55-B144-B2B1-9BF20974A183}"/>
+    <hyperlink ref="E172" r:id="rId51" location="blade/Microsoft_AAD_IAM/AuthenticationMethodsMenuBlade/AdminAuthMethods" xr:uid="{940FFEB1-FA03-5F4E-9118-65B4CE2A9D98}"/>
+    <hyperlink ref="F175" r:id="rId52" location="blade/Microsoft_AAD_IAM/AuthenticationMethodsMenuBlade/PasswordProtection" xr:uid="{FA0B10A3-ECF8-D340-999A-ED47C61BB080}"/>
     <hyperlink ref="E151" r:id="rId53" location="blade/Microsoft_AAD_IAM/ActiveDirectoryMenuBlade/IdentitySecureScore" xr:uid="{91B17E65-603C-8744-A4FC-055D2804305C}"/>
     <hyperlink ref="E94" r:id="rId54" location="blade/Microsoft_AAD_Devices/DevicesMenuBlade/DeviceSettings/menuId/" xr:uid="{9B0A7324-B0F6-0347-8F53-BE36B0C1D1A1}"/>
     <hyperlink ref="F91" r:id="rId55" location="blade/Microsoft_AAD_IAM/EnterpriseApplicationsInsightsMenuBlade/AppMigration" xr:uid="{FCA52BAF-1F22-1144-96F4-0AAA8EEBAC1F}"/>
@@ -3840,8 +3924,8 @@
   </sheetPr>
   <dimension ref="B2:G394"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView showGridLines="0" topLeftCell="A165" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3856,7 +3940,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3867,43 +3951,53 @@
     <row r="3" spans="2:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E11" s="5"/>
+      <c r="E11" s="16" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="19" spans="2:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
@@ -4028,7 +4122,7 @@
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.2">
@@ -4036,7 +4130,7 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="E50" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
@@ -4109,7 +4203,7 @@
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E68" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.2">
@@ -4217,7 +4311,7 @@
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E89" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.2">
@@ -4257,19 +4351,19 @@
     </row>
     <row r="98" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E98" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F98" s="7"/>
     </row>
     <row r="99" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E99" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F99" s="7"/>
     </row>
     <row r="100" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F100" s="7"/>
     </row>
@@ -4287,7 +4381,7 @@
     </row>
     <row r="103" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E103" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F103" s="7"/>
     </row>
@@ -4308,17 +4402,17 @@
       <c r="E107" s="7"/>
     </row>
     <row r="108" spans="4:7" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E108" s="17" t="s">
-        <v>399</v>
-      </c>
-      <c r="F108" s="17"/>
+      <c r="E108" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="F108" s="18"/>
     </row>
     <row r="109" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E109" s="7"/>
     </row>
     <row r="110" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E110" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="111" spans="4:7" x14ac:dyDescent="0.2">
@@ -4366,7 +4460,7 @@
     </row>
     <row r="122" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E122" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="123" spans="3:7" x14ac:dyDescent="0.2">
@@ -4400,7 +4494,7 @@
     </row>
     <row r="130" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E130" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.2">
@@ -4424,7 +4518,7 @@
     </row>
     <row r="136" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E136" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="137" spans="3:7" x14ac:dyDescent="0.2">
@@ -4440,7 +4534,7 @@
     </row>
     <row r="140" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E140" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="141" spans="3:7" x14ac:dyDescent="0.2">
@@ -4465,28 +4559,28 @@
       <c r="G145" s="3"/>
     </row>
     <row r="146" spans="4:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E146" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="F146" s="19"/>
-      <c r="G146" s="19"/>
+      <c r="E146" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="F146" s="20"/>
+      <c r="G146" s="20"/>
     </row>
     <row r="147" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E147" s="7"/>
     </row>
     <row r="148" spans="4:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E148" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="F148" s="18"/>
-      <c r="G148" s="18"/>
+      <c r="E148" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="F148" s="19"/>
+      <c r="G148" s="19"/>
     </row>
     <row r="149" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E149" s="7"/>
     </row>
     <row r="150" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E150" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="151" spans="4:7" x14ac:dyDescent="0.2">
@@ -4494,7 +4588,7 @@
     </row>
     <row r="152" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E152" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="153" spans="4:7" x14ac:dyDescent="0.2">
@@ -4502,7 +4596,7 @@
     </row>
     <row r="154" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E154" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="155" spans="4:7" x14ac:dyDescent="0.2">
@@ -4518,7 +4612,7 @@
     </row>
     <row r="158" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E158" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="159" spans="4:7" x14ac:dyDescent="0.2">
@@ -4534,7 +4628,7 @@
     </row>
     <row r="163" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D163" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
@@ -4576,7 +4670,7 @@
     <row r="172" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="173" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D173" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E173" s="3"/>
       <c r="F173" s="3"/>
@@ -4584,7 +4678,7 @@
     </row>
     <row r="174" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E174" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="175" spans="3:7" x14ac:dyDescent="0.2">
@@ -5262,7 +5356,7 @@
     </row>
     <row r="329" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E329" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="330" spans="5:5" x14ac:dyDescent="0.2">
@@ -5270,7 +5364,7 @@
     </row>
     <row r="331" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E331" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="332" spans="5:5" x14ac:dyDescent="0.2">
@@ -5278,7 +5372,7 @@
     </row>
     <row r="333" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E333" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="334" spans="5:5" x14ac:dyDescent="0.2">
@@ -5286,7 +5380,7 @@
     </row>
     <row r="335" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E335" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="336" spans="5:5" x14ac:dyDescent="0.2">
@@ -5622,10 +5716,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B2:F112"/>
+  <dimension ref="B2:F125"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A111" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5638,7 +5732,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5647,34 +5741,34 @@
     </row>
     <row r="3" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="20" t="s">
-        <v>392</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="C4" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="9" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -5683,14 +5777,14 @@
     <row r="10" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D11" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
@@ -5698,24 +5792,24 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E15" s="13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E16" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.2">
@@ -5723,12 +5817,12 @@
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E22" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.2">
@@ -5736,12 +5830,12 @@
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E26" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.2">
@@ -5749,12 +5843,12 @@
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E30" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.2">
@@ -5762,12 +5856,12 @@
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E34" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E36" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
@@ -5775,12 +5869,12 @@
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E38" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E40" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
@@ -5788,12 +5882,12 @@
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E42" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E44" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.2">
@@ -5801,19 +5895,19 @@
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E46" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D48" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
     <row r="50" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E50" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="51" spans="5:5" x14ac:dyDescent="0.2">
@@ -5821,12 +5915,12 @@
     </row>
     <row r="52" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E52" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E54" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="55" spans="5:5" x14ac:dyDescent="0.2">
@@ -5834,12 +5928,12 @@
     </row>
     <row r="56" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E56" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="58" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E58" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="59" spans="5:5" x14ac:dyDescent="0.2">
@@ -5847,12 +5941,12 @@
     </row>
     <row r="60" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E60" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="62" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E62" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="63" spans="5:5" x14ac:dyDescent="0.2">
@@ -5860,7 +5954,7 @@
     </row>
     <row r="64" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E64" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="67" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -5874,14 +5968,14 @@
     <row r="68" spans="3:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="69" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D69" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E71" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.2">
@@ -5889,12 +5983,12 @@
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E73" s="13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E74" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="76" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -5908,14 +6002,14 @@
     <row r="77" spans="3:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="78" spans="3:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D78" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E80" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.2">
@@ -5923,19 +6017,19 @@
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E82" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="85" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D85" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
     </row>
     <row r="87" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E87" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="88" spans="4:6" x14ac:dyDescent="0.2">
@@ -5943,17 +6037,17 @@
     </row>
     <row r="89" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E89" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="90" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E90" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="92" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E92" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="93" spans="4:6" x14ac:dyDescent="0.2">
@@ -5961,19 +6055,19 @@
     </row>
     <row r="94" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E94" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="97" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D97" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
     </row>
     <row r="99" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E99" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="100" spans="4:6" x14ac:dyDescent="0.2">
@@ -5981,17 +6075,17 @@
     </row>
     <row r="101" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E101" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="102" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E102" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="104" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E104" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="105" spans="4:6" x14ac:dyDescent="0.2">
@@ -5999,17 +6093,17 @@
     </row>
     <row r="106" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E106" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="107" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E107" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="109" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E109" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="110" spans="4:6" x14ac:dyDescent="0.2">
@@ -6017,12 +6111,65 @@
     </row>
     <row r="111" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E111" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="112" spans="4:6" x14ac:dyDescent="0.2">
       <c r="E112" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="115" spans="4:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D115" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+    </row>
+    <row r="117" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E117" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="118" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E118" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F118" s="23" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="120" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E120" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="121" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E121" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F121" s="23" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="122" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E122" s="13" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="123" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E123" s="15" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="124" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E124" s="15" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="125" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E125" s="22" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -6030,7 +6177,7 @@
     <mergeCell ref="C4:F7"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14 E21 E25 E29 E33 E37 E41 E45 E72 E51 E55 E59 E63 E81 E88 E93 E100 E105 E110" xr:uid="{B2F94D8F-9865-1B44-97D4-DFF708939FA2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14 E21 E25 E29 E33 E37 E41 E45 E72 E51 E55 E59 E63 E81 E88 E93 E100 E105 E110 E118 E121" xr:uid="{B2F94D8F-9865-1B44-97D4-DFF708939FA2}">
       <formula1>YesNo</formula1>
     </dataValidation>
   </dataValidations>
@@ -6041,6 +6188,8 @@
     <hyperlink ref="E74" location="GW_AADConnectHealth" display="Guided Walkthrough: AAD Connect Health" xr:uid="{9C338C6D-F80B-A141-9907-3EE211654884}"/>
     <hyperlink ref="E107" location="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today" display="Q: App Assignment" xr:uid="{32662EAC-856D-7242-B40C-99E28266C8F5}"/>
     <hyperlink ref="E112" location="AccMgmt_Do_you_have_a_well_defined_approach_to_assign_access_to_applications_today" display="Q: App Assignment" xr:uid="{9023B8FB-991C-7641-B00B-5E7C2CC273DC}"/>
+    <hyperlink ref="E124" location="GW_AADConnectSettings" display="Guided Walkthrough - AAD Connect Settings" xr:uid="{2D2D86D9-D7D8-4642-94B7-616FC9A83395}"/>
+    <hyperlink ref="E123" location="AccMgmt_If_customer_is_federated_is_the_insideCorporateNetwork_claim_included_by_the_federated_identity_provider" display="Q. AAD Connect Settings" xr:uid="{5824A3D4-7703-3C40-AF03-F6BB45E410DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6079,7 +6228,7 @@
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
@@ -6099,32 +6248,32 @@
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>